<commit_message>
fixed capacity bug in wind-vs-pv data capacity restrictions are now set according to installed capacity, not any longer according to number of thermal generators
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\medea\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936BF649-5106-46E5-85B9-BEB59CA7BA0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEB151D-4CE6-470F-9A08-DCA02F5D4635}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="number_type_legend" sheetId="5" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <sheet name="cost_transport" sheetId="11" r:id="rId10"/>
     <sheet name="potentials" sheetId="12" r:id="rId11"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId12"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -673,58 +670,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Capacity"/>
-      <sheetName val="itm_installed"/>
-      <sheetName val="NTC"/>
-      <sheetName val="km"/>
-      <sheetName val="UpDownParms"/>
-      <sheetName val="StorageChars"/>
-      <sheetName val="Outputs"/>
-      <sheetName val="EffLoss"/>
-      <sheetName val="O&amp;M"/>
-      <sheetName val="kennlinien_logik"/>
-      <sheetName val="number_type_legend"/>
-      <sheetName val="gen_possibilities"/>
-      <sheetName val="WACC"/>
-      <sheetName val="itm_invest"/>
-      <sheetName val="itm_invest_bup"/>
-      <sheetName val="flex_params"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12">
-        <row r="2">
-          <cell r="B2">
-            <v>0.05</v>
-          </cell>
-          <cell r="C2">
-            <v>0.04</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,7 +973,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,7 +1711,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,7 +1748,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,7 +1910,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,11 +1966,11 @@
         <v>500000</v>
       </c>
       <c r="E3" s="1">
-        <f>C3*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$B3)/((1+[1]WACC!$B$2)^$B3-1)</f>
+        <f>C3*(WACC!$B$2*(1+WACC!$B$2)^$B3)/((1+WACC!$B$2)^$B3-1)</f>
         <v>43990.52352552236</v>
       </c>
       <c r="F3" s="1">
-        <f>D3*([1]WACC!$C$2*(1+[1]WACC!$C$2)^$B3)/((1+[1]WACC!$C$2)^$B3-1)</f>
+        <f>D3*(WACC!$C$2*(1+WACC!$C$2)^$B3)/((1+WACC!$C$2)^$B3-1)</f>
         <v>32005.981393227281</v>
       </c>
       <c r="K3" s="1"/>
@@ -2045,11 +1990,11 @@
         <v>3400000</v>
       </c>
       <c r="E4" s="1">
-        <f>C4*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$B4)/((1+[1]WACC!$B$2)^$B4-1)</f>
+        <f>C4*(WACC!$B$2*(1+WACC!$B$2)^$B4)/((1+WACC!$B$2)^$B4-1)</f>
         <v>174493.46896338798</v>
       </c>
       <c r="F4" s="1">
-        <f>D4*([1]WACC!$C$2*(1+[1]WACC!$C$2)^$B4)/((1+[1]WACC!$C$2)^$B4-1)</f>
+        <f>D4*(WACC!$C$2*(1+WACC!$C$2)^$B4)/((1+WACC!$C$2)^$B4-1)</f>
         <v>143578.60518393389</v>
       </c>
       <c r="K4" s="1"/>
@@ -2069,11 +2014,11 @@
         <v>1075000</v>
       </c>
       <c r="E5" s="1">
-        <f>C5*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$B5)/((1+[1]WACC!$B$2)^$B5-1)</f>
+        <f>C5*(WACC!$B$2*(1+WACC!$B$2)^$B5)/((1+WACC!$B$2)^$B5-1)</f>
         <v>76273.891596671834</v>
       </c>
       <c r="F5" s="1">
-        <f>D5*([1]WACC!$C$2*(1+[1]WACC!$C$2)^$B5)/((1+[1]WACC!$C$2)^$B5-1)</f>
+        <f>D5*(WACC!$C$2*(1+WACC!$C$2)^$B5)/((1+WACC!$C$2)^$B5-1)</f>
         <v>68812.859995438659</v>
       </c>
       <c r="K5" s="1"/>
@@ -2093,11 +2038,11 @@
         <v>2400000</v>
       </c>
       <c r="E6" s="1">
-        <f>C6*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$B6)/((1+[1]WACC!$B$2)^$B6-1)</f>
+        <f>C6*(WACC!$B$2*(1+WACC!$B$2)^$B6)/((1+WACC!$B$2)^$B6-1)</f>
         <v>170285.89751815109</v>
       </c>
       <c r="F6" s="1">
-        <f>D6*([1]WACC!$C$2*(1+[1]WACC!$C$2)^$B6)/((1+[1]WACC!$C$2)^$B6-1)</f>
+        <f>D6*(WACC!$C$2*(1+WACC!$C$2)^$B6)/((1+WACC!$C$2)^$B6-1)</f>
         <v>153628.71068749097</v>
       </c>
       <c r="K6" s="1"/>
@@ -2182,7 +2127,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2468,13 +2413,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262E26B0-C129-4904-8AA9-F9E48EA6FD9F}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2585,7 +2530,7 @@
         <v>6000000</v>
       </c>
       <c r="Q2" s="1">
-        <f>P2*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P2*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>349668.96699620999</v>
       </c>
     </row>
@@ -2639,7 +2584,7 @@
         <v>1500000</v>
       </c>
       <c r="Q3" s="1">
-        <f>P3*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P3*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>87417.241749052497</v>
       </c>
     </row>
@@ -2693,7 +2638,7 @@
         <v>1500000</v>
       </c>
       <c r="Q4" s="1">
-        <f>P4*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P4*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>87417.241749052497</v>
       </c>
     </row>
@@ -2747,7 +2692,7 @@
         <v>1750000</v>
       </c>
       <c r="Q5" s="1">
-        <f>P5*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P5*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>101986.78204056126</v>
       </c>
     </row>
@@ -2801,7 +2746,7 @@
         <v>1750000</v>
       </c>
       <c r="Q6" s="1">
-        <f>P6*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P6*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>101986.78204056126</v>
       </c>
     </row>
@@ -2855,7 +2800,7 @@
         <v>1500000</v>
       </c>
       <c r="Q7" s="1">
-        <f>P7*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P7*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>87417.241749052497</v>
       </c>
     </row>
@@ -2909,7 +2854,7 @@
         <v>1500000</v>
       </c>
       <c r="Q8" s="1">
-        <f>P8*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P8*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>87417.241749052497</v>
       </c>
     </row>
@@ -2963,7 +2908,7 @@
         <v>1600000</v>
       </c>
       <c r="Q9" s="1">
-        <f>P9*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P9*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>93245.05786565601</v>
       </c>
     </row>
@@ -3017,7 +2962,7 @@
         <v>1600000</v>
       </c>
       <c r="Q10" s="1">
-        <f>P10*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P10*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>93245.05786565601</v>
       </c>
     </row>
@@ -3071,7 +3016,7 @@
         <v>1750000</v>
       </c>
       <c r="Q11" s="1">
-        <f>P11*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P11*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>101986.78204056126</v>
       </c>
     </row>
@@ -3125,7 +3070,7 @@
         <v>1750000</v>
       </c>
       <c r="Q12" s="1">
-        <f>P12*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P12*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>101986.78204056126</v>
       </c>
     </row>
@@ -3179,7 +3124,7 @@
         <v>1800000</v>
       </c>
       <c r="Q13" s="1">
-        <f>P13*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P13*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>104900.69009886299</v>
       </c>
     </row>
@@ -3233,7 +3178,7 @@
         <v>525000</v>
       </c>
       <c r="Q14" s="1">
-        <f>P14*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P14*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>30596.034612168376</v>
       </c>
     </row>
@@ -3287,7 +3232,7 @@
         <v>525000</v>
       </c>
       <c r="Q15" s="1">
-        <f>P15*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P15*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>30596.034612168376</v>
       </c>
     </row>
@@ -3341,11 +3286,11 @@
         <v>550000</v>
       </c>
       <c r="Q16" s="1">
-        <f>P16*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P16*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>32052.988641319247</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>41.5</v>
       </c>
@@ -3395,11 +3340,11 @@
         <v>550000</v>
       </c>
       <c r="Q17" s="1">
-        <f>P17*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P17*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>32052.988641319247</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>42</v>
       </c>
@@ -3449,11 +3394,11 @@
         <v>575000</v>
       </c>
       <c r="Q18" s="1">
-        <f>P18*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P18*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>33509.942670470125</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>42.5</v>
       </c>
@@ -3503,11 +3448,11 @@
         <v>575000</v>
       </c>
       <c r="Q19" s="1">
-        <f>P19*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P19*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>33509.942670470125</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>43</v>
       </c>
@@ -3557,11 +3502,11 @@
         <v>700000</v>
       </c>
       <c r="Q20" s="1">
-        <f>P20*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P20*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>40794.712816224499</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>43.5</v>
       </c>
@@ -3611,11 +3556,11 @@
         <v>700000</v>
       </c>
       <c r="Q21" s="1">
-        <f>P21*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P21*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>40794.712816224499</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>44</v>
       </c>
@@ -3665,11 +3610,11 @@
         <v>800000</v>
       </c>
       <c r="Q22" s="1">
-        <f>P22*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P22*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>46622.528932828005</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>44.5</v>
       </c>
@@ -3719,11 +3664,11 @@
         <v>800000</v>
       </c>
       <c r="Q23" s="1">
-        <f>P23*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P23*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>46622.528932828005</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>45</v>
       </c>
@@ -3773,11 +3718,12 @@
         <v>800000</v>
       </c>
       <c r="Q24" s="1">
-        <f>P24*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P24*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>46622.528932828005</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T24" s="1"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>45.5</v>
       </c>
@@ -3827,11 +3773,11 @@
         <v>800000</v>
       </c>
       <c r="Q25" s="1">
-        <f>P25*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P25*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>46622.528932828005</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>49.5</v>
       </c>
@@ -3881,11 +3827,11 @@
         <v>200000</v>
       </c>
       <c r="Q26" s="1">
-        <f>P26*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P26*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>11655.632233207001</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>50</v>
       </c>
@@ -3935,11 +3881,11 @@
         <v>500000</v>
       </c>
       <c r="Q27" s="1">
-        <f>P27*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P27*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>29139.080583017501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>50.5</v>
       </c>
@@ -3989,11 +3935,11 @@
         <v>500000</v>
       </c>
       <c r="Q28" s="1">
-        <f>P28*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P28*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>29139.080583017501</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>51</v>
       </c>
@@ -4043,11 +3989,11 @@
         <v>500000</v>
       </c>
       <c r="Q29" s="1">
-        <f>P29*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P29*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>29139.080583017501</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>51.5</v>
       </c>
@@ -4097,11 +4043,11 @@
         <v>500000</v>
       </c>
       <c r="Q30" s="1">
-        <f>P30*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P30*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>29139.080583017501</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>52</v>
       </c>
@@ -4151,11 +4097,11 @@
         <v>500000</v>
       </c>
       <c r="Q31" s="1">
-        <f>P31*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P31*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>29139.080583017501</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>52.5</v>
       </c>
@@ -4205,7 +4151,7 @@
         <v>500000</v>
       </c>
       <c r="Q32" s="1">
-        <f>P32*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P32*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>29139.080583017501</v>
       </c>
     </row>
@@ -4259,7 +4205,7 @@
         <v>3000000</v>
       </c>
       <c r="Q33" s="1">
-        <f>P33*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P33*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>174834.48349810499</v>
       </c>
     </row>
@@ -4313,7 +4259,7 @@
         <v>2500000</v>
       </c>
       <c r="Q34" s="1">
-        <f>P34*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P34*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>145695.4029150875</v>
       </c>
     </row>
@@ -4367,7 +4313,7 @@
         <v>2500000</v>
       </c>
       <c r="Q35" s="1">
-        <f>P35*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P35*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>145695.4029150875</v>
       </c>
     </row>
@@ -4421,7 +4367,7 @@
         <v>2350000</v>
       </c>
       <c r="Q36" s="1">
-        <f>P36*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P36*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>136953.67874018225</v>
       </c>
     </row>
@@ -4475,7 +4421,7 @@
         <v>2350000</v>
       </c>
       <c r="Q37" s="1">
-        <f>P37*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P37*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>136953.67874018225</v>
       </c>
     </row>
@@ -4529,7 +4475,7 @@
         <v>550000</v>
       </c>
       <c r="Q38" s="1">
-        <f>P38*([1]WACC!$B$2*(1+[1]WACC!$B$2)^$O$2)/((1+[1]WACC!$B$2)^$O$2-1)</f>
+        <f>P38*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>32052.988641319247</v>
       </c>
     </row>
@@ -4547,7 +4493,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
reaorking data instantiation process
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEB151D-4CE6-470F-9A08-DCA02F5D4635}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C7C688-F9EA-48FA-9F3C-1C26CDBAE862}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="6" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="number_type_legend" sheetId="5" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="143">
   <si>
     <t>year</t>
   </si>
@@ -971,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC55109-0130-495D-B4C2-93D774DF9105}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
@@ -4487,13 +4487,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CDD314-E06C-4AC0-8DDE-77CC4444BECC}">
-  <dimension ref="A1:H191"/>
+  <dimension ref="A1:H171"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C144" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7160,75 +7160,75 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="5">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C157" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D157" s="6">
         <v>0</v>
       </c>
       <c r="E157" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C158" s="6">
-        <v>0</v>
+        <v>0.82</v>
       </c>
       <c r="D158" s="6">
         <v>0</v>
       </c>
       <c r="E158" s="6">
-        <v>0</v>
+        <v>0.85419999999999996</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="5">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C159" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D159" s="6">
         <v>0</v>
       </c>
       <c r="E159" s="6">
-        <v>0</v>
+        <v>0.54049999999999998</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="5">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C160" s="6">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D160" s="6">
         <v>0</v>
       </c>
       <c r="E160" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.65790000000000004</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="5">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B161" s="5" t="s">
         <v>63</v>
@@ -7243,77 +7243,77 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="5">
-        <v>61</v>
+        <v>70.5</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C162" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D162" s="6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E162" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="5">
-        <v>61</v>
+        <v>70.5</v>
       </c>
       <c r="B163" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C163" s="6">
-        <v>0</v>
+        <v>0.82</v>
       </c>
       <c r="D163" s="6">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="E163" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.85419999999999996</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="5">
-        <v>61</v>
+        <v>70.5</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C164" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D164" s="6">
-        <v>0</v>
+        <v>0.73750000000000004</v>
       </c>
       <c r="E164" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.54049999999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="5">
-        <v>61</v>
+        <v>70.5</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C165" s="6">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D165" s="6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E165" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.65790000000000004</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="5">
-        <v>61</v>
+        <v>70.5</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>63</v>
@@ -7328,9 +7328,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="5">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>59</v>
@@ -7339,15 +7339,15 @@
         <v>0</v>
       </c>
       <c r="D167" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E167" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>60</v>
@@ -7356,15 +7356,17 @@
         <v>0</v>
       </c>
       <c r="D168" s="6">
-        <v>0</v>
+        <f>$D$167*$E168+ROUND(LOG(E168)*0.25,3)</f>
+        <v>2.2189999999999999</v>
       </c>
       <c r="E168" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="F168" s="6"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="5">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="B169" s="5" t="s">
         <v>61</v>
@@ -7373,15 +7375,17 @@
         <v>0</v>
       </c>
       <c r="D169" s="6">
-        <v>0</v>
+        <f t="shared" ref="D169:D170" si="0">$D$167*$E169+ROUND(LOG(E169)*0.25,3)</f>
+        <v>0.59899999999999998</v>
       </c>
       <c r="E169" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="F169" s="6"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="5">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="B170" s="5" t="s">
         <v>62</v>
@@ -7390,15 +7394,17 @@
         <v>0</v>
       </c>
       <c r="D170" s="6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.425</v>
       </c>
       <c r="E170" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="F170" s="6"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="5">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="B171" s="5" t="s">
         <v>63</v>
@@ -7410,352 +7416,6 @@
         <v>0</v>
       </c>
       <c r="E171" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="5">
-        <v>63</v>
-      </c>
-      <c r="B172" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C172" s="6">
-        <v>1</v>
-      </c>
-      <c r="D172" s="6">
-        <v>0</v>
-      </c>
-      <c r="E172" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="5">
-        <v>63</v>
-      </c>
-      <c r="B173" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C173" s="6">
-        <v>0.66</v>
-      </c>
-      <c r="D173" s="6">
-        <v>0</v>
-      </c>
-      <c r="E173" s="6">
-        <v>0.6875</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="5">
-        <v>63</v>
-      </c>
-      <c r="B174" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C174" s="6">
-        <v>0.33</v>
-      </c>
-      <c r="D174" s="6">
-        <v>0</v>
-      </c>
-      <c r="E174" s="6">
-        <v>0.35680000000000001</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="5">
-        <v>63</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C175" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="D175" s="6">
-        <v>0</v>
-      </c>
-      <c r="E175" s="6">
-        <v>5.2600000000000001E-2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="5">
-        <v>63</v>
-      </c>
-      <c r="B176" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C176" s="6">
-        <v>0</v>
-      </c>
-      <c r="D176" s="6">
-        <v>0</v>
-      </c>
-      <c r="E176" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" s="5">
-        <v>70</v>
-      </c>
-      <c r="B177" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C177" s="6">
-        <v>1</v>
-      </c>
-      <c r="D177" s="6">
-        <v>0</v>
-      </c>
-      <c r="E177" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" s="5">
-        <v>70</v>
-      </c>
-      <c r="B178" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C178" s="6">
-        <v>0.82</v>
-      </c>
-      <c r="D178" s="6">
-        <v>0</v>
-      </c>
-      <c r="E178" s="6">
-        <v>0.85419999999999996</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A179" s="5">
-        <v>70</v>
-      </c>
-      <c r="B179" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C179" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D179" s="6">
-        <v>0</v>
-      </c>
-      <c r="E179" s="6">
-        <v>0.54049999999999998</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" s="5">
-        <v>70</v>
-      </c>
-      <c r="B180" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C180" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="D180" s="6">
-        <v>0</v>
-      </c>
-      <c r="E180" s="6">
-        <v>0.65790000000000004</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" s="5">
-        <v>70</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C181" s="6">
-        <v>0</v>
-      </c>
-      <c r="D181" s="6">
-        <v>0</v>
-      </c>
-      <c r="E181" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A182" s="5">
-        <v>70.5</v>
-      </c>
-      <c r="B182" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C182" s="6">
-        <v>1</v>
-      </c>
-      <c r="D182" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="E182" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A183" s="5">
-        <v>70.5</v>
-      </c>
-      <c r="B183" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C183" s="6">
-        <v>0.82</v>
-      </c>
-      <c r="D183" s="6">
-        <v>0.95</v>
-      </c>
-      <c r="E183" s="6">
-        <v>0.85419999999999996</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" s="5">
-        <v>70.5</v>
-      </c>
-      <c r="B184" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C184" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D184" s="6">
-        <v>0.73750000000000004</v>
-      </c>
-      <c r="E184" s="6">
-        <v>0.54049999999999998</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A185" s="5">
-        <v>70.5</v>
-      </c>
-      <c r="B185" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C185" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="D185" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="E185" s="6">
-        <v>0.65790000000000004</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" s="5">
-        <v>70.5</v>
-      </c>
-      <c r="B186" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C186" s="6">
-        <v>0</v>
-      </c>
-      <c r="D186" s="6">
-        <v>0</v>
-      </c>
-      <c r="E186" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A187" s="5">
-        <v>100</v>
-      </c>
-      <c r="B187" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C187" s="6">
-        <v>0</v>
-      </c>
-      <c r="D187" s="6">
-        <v>3</v>
-      </c>
-      <c r="E187" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A188" s="5">
-        <v>100</v>
-      </c>
-      <c r="B188" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C188" s="6">
-        <v>0</v>
-      </c>
-      <c r="D188" s="6">
-        <f>$D$187*$E188+ROUND(LOG(E188)*0.25,3)</f>
-        <v>2.2189999999999999</v>
-      </c>
-      <c r="E188" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="F188" s="6"/>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A189" s="5">
-        <v>100</v>
-      </c>
-      <c r="B189" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C189" s="6">
-        <v>0</v>
-      </c>
-      <c r="D189" s="6">
-        <f t="shared" ref="D189:D190" si="0">$D$187*$E189+ROUND(LOG(E189)*0.25,3)</f>
-        <v>0.59899999999999998</v>
-      </c>
-      <c r="E189" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="F189" s="6"/>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" s="5">
-        <v>100</v>
-      </c>
-      <c r="B190" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C190" s="6">
-        <v>0</v>
-      </c>
-      <c r="D190" s="6">
-        <f t="shared" si="0"/>
-        <v>1.425</v>
-      </c>
-      <c r="E190" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="F190" s="6"/>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="5">
-        <v>100</v>
-      </c>
-      <c r="B191" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C191" s="6">
-        <v>0</v>
-      </c>
-      <c r="D191" s="6">
-        <v>0</v>
-      </c>
-      <c r="E191" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished gdx instantiation rework, improved grid expansion cost assumptions
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\git_repos\medea\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB403F69-2DC5-48B7-A7F9-E0A11DB006A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121EB2A9-941B-4D94-A920-333F0A3671A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="16455" activeTab="6" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="number_type_legend" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="installed_itm" sheetId="2" r:id="rId5"/>
     <sheet name="param_thermal" sheetId="9" r:id="rId6"/>
     <sheet name="feasgen_thermal" sheetId="6" r:id="rId7"/>
-    <sheet name="NTC" sheetId="3" r:id="rId8"/>
+    <sheet name="ATC" sheetId="3" r:id="rId8"/>
     <sheet name="km" sheetId="4" r:id="rId9"/>
     <sheet name="cost_transport" sheetId="11" r:id="rId10"/>
     <sheet name="potentials" sheetId="12" r:id="rId11"/>
@@ -132,6 +132,328 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sebastian</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{15015C9C-05A8-4B29-91EB-A4856D055B06}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bad Aussee</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{4C6AD0E0-3CA8-4CDE-9A2F-32DDCE9D2F4A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Walhain</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{ED198303-CA4D-4147-8149-E80CBFD67BA3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sachseln</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{0E40F46B-1F2B-4677-B088-BBB8CB92A80E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Cihost</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{FE1470D8-4258-4C73-B850-3F5CAB8D515D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Niederdorla</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{CAEBE6AA-0246-460A-A5AF-F530BB899483}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Odder</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{B2F8B32B-E85F-4CB0-9532-2A68EB3BF92F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Vesdun</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9600A723-2A7D-40E9-A098-39CAF18E9C16}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Pusztavacs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{854C9F7C-4BBC-4F01-BEBB-D8F2A76B69D4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Narni</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{B57AFA70-8FB5-4640-8FBF-41028000B950}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lunteren</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{4B2277D0-F36D-4B71-82E2-FB393984B41D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Piatek</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{8236F644-4CB0-4EB6-A521-C9868338EBBB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Spodnja Slivnica</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{1EE3CBB4-7D74-4F98-9B0D-5DF673B85639}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Molca</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="145">
   <si>
@@ -578,9 +900,9 @@
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,13 +951,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -651,7 +992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -670,7 +1011,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -684,6 +1025,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -4709,7 +5051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CDD314-E06C-4AC0-8DDE-77CC4444BECC}">
   <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7075,11 +7417,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4160F9D6-85F4-409B-B165-F3480400FC38}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7129,6 +7471,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="20"/>
       <c r="D2">
         <v>1200</v>
       </c>
@@ -7138,12 +7484,16 @@
       <c r="F2">
         <v>4500</v>
       </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2">
         <v>300</v>
       </c>
       <c r="J2">
         <v>100</v>
       </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
       <c r="M2">
         <v>950</v>
       </c>
@@ -7152,12 +7502,24 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="20"/>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="G3" s="20"/>
       <c r="H3">
         <v>600</v>
       </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
       <c r="K3">
         <v>950</v>
       </c>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -7166,9 +7528,20 @@
       <c r="B4">
         <v>1200</v>
       </c>
+      <c r="C4" s="20"/>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="G4" s="20"/>
       <c r="H4">
         <v>1500</v>
       </c>
+      <c r="I4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -7177,12 +7550,23 @@
       <c r="B5">
         <v>700</v>
       </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <v>1750</v>
       </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
       <c r="L5">
         <v>600</v>
       </c>
+      <c r="M5" s="20"/>
       <c r="N5">
         <v>800</v>
       </c>
@@ -7197,40 +7581,72 @@
       <c r="E6">
         <v>1750</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
       <c r="G6">
         <v>800</v>
       </c>
       <c r="H6">
         <v>3200</v>
       </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
       <c r="L6">
         <v>150</v>
       </c>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7">
         <v>800</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
+      <c r="B8" s="20"/>
       <c r="C8">
         <v>600</v>
       </c>
       <c r="D8">
         <v>1500</v>
       </c>
+      <c r="E8" s="20"/>
       <c r="F8">
         <v>3200</v>
       </c>
+      <c r="G8" s="20"/>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="20"/>
       <c r="J8">
         <v>870</v>
       </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -7239,6 +7655,18 @@
       <c r="B9">
         <v>300</v>
       </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -7247,28 +7675,64 @@
       <c r="B10">
         <v>100</v>
       </c>
+      <c r="C10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
       <c r="H10">
         <v>870</v>
       </c>
+      <c r="I10" s="20"/>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="N10" s="20"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
+      <c r="B11" s="20"/>
       <c r="C11">
         <v>950</v>
       </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12">
         <v>600</v>
       </c>
       <c r="F12">
         <v>150</v>
       </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="20"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -7277,13 +7741,36 @@
       <c r="B13">
         <v>950</v>
       </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
       <c r="E14">
         <v>800</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7292,14 +7779,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A39B26-472C-4146-B74A-2E1C6D7D11B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A39B26-472C-4146-B74A-2E1C6D7D11B9}">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7349,98 +7836,364 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2">
+        <v>429</v>
+      </c>
+      <c r="E2">
+        <v>308</v>
+      </c>
       <c r="F2">
-        <v>230</v>
+        <v>464</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2">
+        <v>434</v>
+      </c>
+      <c r="J2">
+        <v>576</v>
+      </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2">
+        <v>198</v>
+      </c>
+      <c r="N2">
+        <v>422</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="20"/>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
       <c r="F3">
-        <v>437</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="G3" s="20"/>
       <c r="H3">
-        <v>342</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
       <c r="K3">
-        <v>163</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="B4">
+        <v>429</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4">
+        <v>512</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4">
+        <v>444</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4">
+        <v>591</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5">
+        <v>308</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>442</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5">
+        <v>389</v>
+      </c>
+      <c r="M5" s="20"/>
+      <c r="N5">
+        <v>305</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6">
-        <v>230</v>
+        <v>464</v>
       </c>
       <c r="C6">
-        <v>437</v>
+        <v>408</v>
+      </c>
+      <c r="D6">
+        <v>512</v>
+      </c>
+      <c r="E6">
+        <v>442</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>536</v>
       </c>
       <c r="H6">
-        <v>694</v>
-      </c>
+        <v>780</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6">
+        <v>349</v>
+      </c>
+      <c r="L6">
+        <v>633</v>
+      </c>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7">
+        <v>536</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
+      <c r="B8" s="20"/>
       <c r="C8">
-        <v>342</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="D8">
+        <v>444</v>
+      </c>
+      <c r="E8" s="20"/>
       <c r="F8">
-        <v>694</v>
-      </c>
+        <v>780</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="20"/>
+      <c r="J8">
+        <v>916</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
+      <c r="B9">
+        <v>434</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9">
+        <v>395</v>
+      </c>
+      <c r="N9">
+        <v>172</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
+      <c r="B10">
+        <v>576</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10">
+        <v>591</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10">
+        <v>916</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10">
+        <v>415</v>
+      </c>
+      <c r="N10" s="20"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
+      <c r="B11" s="20"/>
       <c r="C11">
-        <v>163</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11">
+        <v>349</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12">
+        <v>389</v>
+      </c>
+      <c r="F12">
+        <v>633</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="20"/>
+      <c r="N12">
+        <v>374</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
+      <c r="B13">
+        <v>198</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13">
+        <v>395</v>
+      </c>
+      <c r="J13">
+        <v>415</v>
+      </c>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="B14">
+        <v>422</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14">
+        <v>305</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14">
+        <v>172</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14">
+        <v>374</v>
+      </c>
+      <c r="M14" s="20"/>
+      <c r="N14">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed co-generation bug in main model; added biomass to wind_vs_pv analysis
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121EB2A9-941B-4D94-A920-333F0A3671A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C213970-648B-4E0B-9787-2E64148309F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="9" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="number_type_legend" sheetId="5" r:id="rId1"/>
@@ -146,7 +146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -155,7 +155,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Bad Aussee</t>
@@ -170,7 +170,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -179,7 +179,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Walhain</t>
@@ -194,7 +194,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -203,7 +203,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Sachseln</t>
@@ -218,7 +218,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -227,7 +227,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Cihost</t>
@@ -242,7 +242,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -251,7 +251,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Niederdorla</t>
@@ -266,7 +266,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -275,7 +275,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Odder</t>
@@ -290,7 +290,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -299,7 +299,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Vesdun</t>
@@ -314,7 +314,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -323,7 +323,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Pusztavacs</t>
@@ -338,7 +338,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -347,7 +347,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Narni</t>
@@ -362,7 +362,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -371,7 +371,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lunteren</t>
@@ -386,7 +386,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -395,7 +395,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Piatek</t>
@@ -410,7 +410,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -419,7 +419,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Spodnja Slivnica</t>
@@ -434,7 +434,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sebastian:</t>
         </r>
@@ -443,7 +443,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Molca</t>
@@ -902,7 +902,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -950,19 +950,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1042,6 +1029,1871 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT"/>
+              <a:t>biomass_chp</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>feasgen_thermal!$D$130:$D$133</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>feasgen_thermal!$C$130:$C$133</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0FCE-4C73-B01C-96116F10E6CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1097289392"/>
+        <c:axId val="1346366448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1097289392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1346366448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1346366448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1097289392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT"/>
+              <a:t>ng chp hi</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>feasgen_thermal!$D$86:$D$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.74999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>feasgen_thermal!$C$86:$C$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-85AB-4455-9A8C-A8FE319D5BA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1346179440"/>
+        <c:axId val="1346324432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1346179440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1346324432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1346324432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1346179440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C55AEDF4-7D55-405D-920C-732FA437DBBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15613A7B-BAB4-490D-941C-776C755C95BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1345,7 +3197,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,8 +3833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86480E31-139B-4EFE-B8CC-58C75AC65F1A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,7 +3863,7 @@
         <v>128</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -5052,10 +6904,10 @@
   <dimension ref="A1:E137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C104" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F136" sqref="F136"/>
+      <selection pane="bottomRight" activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7410,6 +9262,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7417,7 +9270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4160F9D6-85F4-409B-B165-F3480400FC38}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
increased model consistency, enabled disinvestment for intermittents
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C213970-648B-4E0B-9787-2E64148309F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EF3B6E-D06F-4AD7-9C55-F8AEC2BB6EF1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="9" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="number_type_legend" sheetId="5" r:id="rId1"/>
@@ -77,6 +77,40 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Sebastian</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{8E96404D-48E0-4D06-99A5-65DE40EA26E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assumed to be 2% of annual capital cost</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>Autor</author>
   </authors>
   <commentList>
@@ -132,7 +166,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sebastian</author>
@@ -455,7 +489,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="146">
   <si>
     <t>year</t>
   </si>
@@ -890,6 +924,9 @@
   </si>
   <si>
     <t>CHP coefficient</t>
+  </si>
+  <si>
+    <t>om_qfix</t>
   </si>
 </sst>
 </file>
@@ -902,7 +939,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -950,6 +987,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3195,7 +3245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC55109-0130-495D-B4C2-93D774DF9105}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C37" sqref="C37:C38"/>
     </sheetView>
@@ -3833,7 +3883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86480E31-139B-4EFE-B8CC-58C75AC65F1A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4317,14 +4367,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9B5A1D-EA9B-421F-AC28-39B233C76782}">
-  <dimension ref="A1:L38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9B5A1D-EA9B-421F-AC28-39B233C76782}">
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4332,7 +4382,7 @@
     <col min="3" max="4" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>64</v>
       </c>
@@ -4348,8 +4398,20 @@
       <c r="F1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -4365,8 +4427,20 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4387,10 +4461,26 @@
         <f>D3*(WACC!$C$2*(1+WACC!$C$2)^$B3)/((1+WACC!$C$2)^$B3-1)</f>
         <v>32005.981393227281</v>
       </c>
+      <c r="G3" s="1">
+        <f>0.02*C3</f>
+        <v>12400</v>
+      </c>
+      <c r="H3" s="1">
+        <f>0.02*D3</f>
+        <v>10000</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4411,10 +4501,25 @@
         <f>D4*(WACC!$C$2*(1+WACC!$C$2)^$B4)/((1+WACC!$C$2)^$B4-1)</f>
         <v>143578.60518393389</v>
       </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G6" si="0">0.02*C4</f>
+        <v>68000</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H6" si="1">0.02*D4</f>
+        <v>68000</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -4435,10 +4540,26 @@
         <f>D5*(WACC!$C$2*(1+WACC!$C$2)^$B5)/((1+WACC!$C$2)^$B5-1)</f>
         <v>68812.859995438659</v>
       </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>21500</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>21500</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -4459,44 +4580,59 @@
         <f>D6*(WACC!$C$2*(1+WACC!$C$2)^$B6)/((1+WACC!$C$2)^$B6-1)</f>
         <v>153628.71068749097</v>
       </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>48000</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>48000</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10" s="8"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" s="9"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C16" s="8"/>
       <c r="D16" s="1"/>
       <c r="E16" s="7"/>
@@ -4530,6 +4666,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4827,13 +4964,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262E26B0-C129-4904-8AA9-F9E48EA6FD9F}">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4932,10 +5069,10 @@
         <v>0.62</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="N2">
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="O2">
         <v>40</v>
@@ -4986,10 +5123,10 @@
         <v>0.65</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N3">
-        <v>60</v>
+        <v>750</v>
       </c>
       <c r="O3">
         <v>40</v>
@@ -5040,10 +5177,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N4">
-        <v>60</v>
+        <v>750</v>
       </c>
       <c r="O4">
         <v>40</v>
@@ -5094,10 +5231,10 @@
         <v>0.4</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N5">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="O5">
         <v>40</v>
@@ -5148,10 +5285,10 @@
         <v>0.35</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N6">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="O6">
         <v>40</v>
@@ -5202,10 +5339,10 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N7">
-        <v>50</v>
+        <v>750</v>
       </c>
       <c r="O7">
         <v>40</v>
@@ -5256,10 +5393,10 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N8">
-        <v>50</v>
+        <v>750</v>
       </c>
       <c r="O8">
         <v>40</v>
@@ -5310,10 +5447,10 @@
         <v>0.4</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N9">
-        <v>50</v>
+        <v>800</v>
       </c>
       <c r="O9">
         <v>40</v>
@@ -5364,10 +5501,10 @@
         <v>0.4</v>
       </c>
       <c r="M10">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N10">
-        <v>50</v>
+        <v>800</v>
       </c>
       <c r="O10">
         <v>40</v>
@@ -5418,10 +5555,10 @@
         <v>0.35699999999999998</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N11">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="O11">
         <v>40</v>
@@ -5472,10 +5609,10 @@
         <v>0.375</v>
       </c>
       <c r="M12">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N12">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="O12">
         <v>40</v>
@@ -5526,10 +5663,10 @@
         <v>0.2</v>
       </c>
       <c r="M13">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N13">
-        <v>50</v>
+        <v>1100</v>
       </c>
       <c r="O13">
         <v>40</v>
@@ -5580,10 +5717,10 @@
         <v>0.5</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N14">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="O14">
         <v>35</v>
@@ -5634,10 +5771,10 @@
         <v>0.5</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N15">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="O15">
         <v>35</v>
@@ -5688,10 +5825,10 @@
         <v>0.75</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N16">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="O16">
         <v>35</v>
@@ -5704,7 +5841,7 @@
         <v>32052.988641319247</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>41.5</v>
       </c>
@@ -5742,10 +5879,10 @@
         <v>0.7</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N17">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="O17">
         <v>35</v>
@@ -5758,7 +5895,7 @@
         <v>32052.988641319247</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>42</v>
       </c>
@@ -5796,10 +5933,10 @@
         <v>0.7</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N18">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="O18">
         <v>35</v>
@@ -5812,7 +5949,7 @@
         <v>33509.942670470125</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>42.5</v>
       </c>
@@ -5850,10 +5987,10 @@
         <v>0.65</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N19">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="O19">
         <v>35</v>
@@ -5866,7 +6003,7 @@
         <v>33509.942670470125</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>43</v>
       </c>
@@ -5904,10 +6041,10 @@
         <v>0.352112676056338</v>
       </c>
       <c r="M20">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N20">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="O20">
         <v>35</v>
@@ -5920,7 +6057,7 @@
         <v>40794.712816224499</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>43.5</v>
       </c>
@@ -5958,10 +6095,10 @@
         <v>0.375</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N21">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="O21">
         <v>35</v>
@@ -5974,7 +6111,7 @@
         <v>40794.712816224499</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>44</v>
       </c>
@@ -6012,10 +6149,10 @@
         <v>0.49872122762148335</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N22">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="O22">
         <v>35</v>
@@ -6028,7 +6165,7 @@
         <v>46622.528932828005</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>44.5</v>
       </c>
@@ -6066,10 +6203,10 @@
         <v>0.38</v>
       </c>
       <c r="M23">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N23">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="O23">
         <v>35</v>
@@ -6082,7 +6219,7 @@
         <v>46622.528932828005</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>45</v>
       </c>
@@ -6120,10 +6257,10 @@
         <v>0.25</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N24">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="O24">
         <v>35</v>
@@ -6135,9 +6272,8 @@
         <f>P24*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
         <v>46622.528932828005</v>
       </c>
-      <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>45.5</v>
       </c>
@@ -6175,10 +6311,10 @@
         <v>0.25</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N25">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="O25">
         <v>35</v>
@@ -6191,7 +6327,7 @@
         <v>46622.528932828005</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>49.5</v>
       </c>
@@ -6229,10 +6365,10 @@
         <v>0.99</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N26">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O26">
         <v>35</v>
@@ -6245,7 +6381,7 @@
         <v>11655.632233207001</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>50</v>
       </c>
@@ -6283,10 +6419,10 @@
         <v>0.5</v>
       </c>
       <c r="M27">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N27">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="O27">
         <v>35</v>
@@ -6299,7 +6435,7 @@
         <v>29139.080583017501</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>50.5</v>
       </c>
@@ -6337,10 +6473,10 @@
         <v>0.5</v>
       </c>
       <c r="M28">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N28">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="O28">
         <v>35</v>
@@ -6353,7 +6489,7 @@
         <v>29139.080583017501</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>51</v>
       </c>
@@ -6391,10 +6527,10 @@
         <v>0.77500000000000002</v>
       </c>
       <c r="M29">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N29">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="O29">
         <v>35</v>
@@ -6407,7 +6543,7 @@
         <v>29139.080583017501</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>51.5</v>
       </c>
@@ -6445,10 +6581,10 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="M30">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N30">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="O30">
         <v>35</v>
@@ -6461,7 +6597,7 @@
         <v>29139.080583017501</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>52</v>
       </c>
@@ -6499,23 +6635,23 @@
         <v>0.45454545454545453</v>
       </c>
       <c r="M31">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N31">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="O31">
         <v>35</v>
       </c>
       <c r="P31" s="1">
-        <v>500000</v>
+        <v>700000</v>
       </c>
       <c r="Q31" s="1">
         <f>P31*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
-        <v>29139.080583017501</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+        <v>40794.712816224499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>52.5</v>
       </c>
@@ -6553,20 +6689,20 @@
         <v>0.45454545454545453</v>
       </c>
       <c r="M32">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N32">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="O32">
         <v>35</v>
       </c>
       <c r="P32" s="1">
-        <v>500000</v>
+        <v>700000</v>
       </c>
       <c r="Q32" s="1">
         <f>P32*(WACC!$B$2*(1+WACC!$B$2)^$O$2)/((1+WACC!$B$2)^$O$2-1)</f>
-        <v>29139.080583017501</v>
+        <v>40794.712816224499</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -6607,10 +6743,10 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="N33">
-        <v>55</v>
+        <v>1500</v>
       </c>
       <c r="O33">
         <v>50</v>
@@ -6661,10 +6797,10 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="N34">
-        <v>55</v>
+        <v>1500</v>
       </c>
       <c r="O34">
         <v>50</v>
@@ -6715,10 +6851,10 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="N35">
-        <v>55</v>
+        <v>1500</v>
       </c>
       <c r="O35">
         <v>50</v>
@@ -6769,10 +6905,10 @@
         <v>0.5</v>
       </c>
       <c r="M36">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N36">
-        <v>100</v>
+        <v>1500</v>
       </c>
       <c r="O36">
         <v>35</v>
@@ -6823,10 +6959,10 @@
         <v>0.5</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="N37">
-        <v>100</v>
+        <v>1500</v>
       </c>
       <c r="O37">
         <v>35</v>
@@ -6877,10 +7013,10 @@
         <v>1</v>
       </c>
       <c r="M38">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="N38">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="O38">
         <v>25</v>
@@ -9639,7 +9775,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:N14"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
* new feature: external costs from air pollutants - re-write of thermal power plant data aggregation in prepare_data.py. now uses generic efficiencies.
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D6A6C7-FDD2-4011-9F16-8266461645C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06905E4-24CD-4569-A413-494C0077B95A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="860" activeTab="13" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="31200" yWindow="2160" windowWidth="21600" windowHeight="12735" tabRatio="860" firstSheet="6" activeTab="14" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="ATC" sheetId="3" r:id="rId12"/>
     <sheet name="KM" sheetId="4" r:id="rId13"/>
     <sheet name="potentials" sheetId="19" r:id="rId14"/>
+    <sheet name="AIR_POLLUTION" sheetId="20" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -639,8 +640,43 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sebastian</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2C3BF732-EB70-4318-A3DC-57E3173C0EC6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lifecycle air pollution cost of state-of-the-art (in around 2009) electricity generation technologies in € of 2015. 
+Total of health impacts, crop yield losses, and material damage.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="259">
   <si>
     <t>year</t>
   </si>
@@ -1089,9 +1125,6 @@
     <t>total installed cost</t>
   </si>
   <si>
-    <t>annuity of total installed cost</t>
-  </si>
-  <si>
     <t>zone</t>
   </si>
   <si>
@@ -1315,22 +1348,129 @@
   </si>
   <si>
     <t>1, 8</t>
+  </si>
+  <si>
+    <t>equivalent annual cost</t>
+  </si>
+  <si>
+    <t>Sascha Samadi</t>
+  </si>
+  <si>
+    <t>The Social Costs of Electricity Generation - Categorizing Different Types of Costs and Evaluating Their Respective Relevance</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/1996-1073/10/3/356</t>
+  </si>
+  <si>
+    <t>NEEDS Project</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D7.2%20Final%20report%20on%20advanced%20fossil%20power%20plants.pdf</t>
+  </si>
+  <si>
+    <t>Final report on technical data, costs, and life cycle inventories of advanced fossil power generation systems</t>
+  </si>
+  <si>
+    <t>Final report on technical data, costs and life cycle inventories of biomass CHP plants</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D13.2%20Final%20report%20on%20Biomass%20technologies.pdf</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D11.2%20Final%20report%20on%20PV%20technology.pdf</t>
+  </si>
+  <si>
+    <t>Table 16, page 51</t>
+  </si>
+  <si>
+    <t>Final report on technical data, costs and life cycle inventories of PV applications</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D10.2.pdf</t>
+  </si>
+  <si>
+    <t>Table 5.3, page 39</t>
+  </si>
+  <si>
+    <t>Final report on offshore wind technology</t>
+  </si>
+  <si>
+    <t>Table 7, page 16</t>
+  </si>
+  <si>
+    <t>10, 11</t>
+  </si>
+  <si>
+    <t>10, 14</t>
+  </si>
+  <si>
+    <t>10, 13</t>
+  </si>
+  <si>
+    <t>10, 12</t>
+  </si>
+  <si>
+    <t>10, 8</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>fixed cost</t>
+  </si>
+  <si>
+    <t>wind offshore in soure; 4044 full-load hours</t>
+  </si>
+  <si>
+    <t>utility scale pv, 838 full-load hours</t>
+  </si>
+  <si>
+    <t>avg of lignite and nat gas due to lack of data</t>
+  </si>
+  <si>
+    <t>no data available</t>
+  </si>
+  <si>
+    <t>Syngas</t>
+  </si>
+  <si>
+    <t>43.2% net efficiency</t>
+  </si>
+  <si>
+    <t>45.0% net efficiency</t>
+  </si>
+  <si>
+    <t>57.5% net efficiency</t>
+  </si>
+  <si>
+    <t>20.0% net efficiency</t>
+  </si>
+  <si>
+    <t>34.0% net efficiency</t>
+  </si>
+  <si>
+    <t>variable cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="170" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="169" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1387,6 +1527,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1416,7 +1569,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1449,8 +1602,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1460,9 +1613,11 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1779,10 +1934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3387BF03-EDC5-4C83-AB6F-3B95A2E59024}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,22 +1949,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,16 +1972,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2">
         <v>2016</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,16 +1989,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1851,16 +2006,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4">
         <v>2013</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,16 +2023,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5">
         <v>2014</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,16 +2040,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,16 +2057,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7">
         <v>2014</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1919,16 +2074,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1936,16 +2091,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1953,16 +2108,115 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C10">
         <v>2017</v>
       </c>
       <c r="D10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>220</v>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C11">
+        <v>2017</v>
+      </c>
+      <c r="D11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12">
+        <v>2007</v>
+      </c>
+      <c r="D12" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13">
+        <v>2008</v>
+      </c>
+      <c r="D13" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14">
+        <v>2008</v>
+      </c>
+      <c r="D14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15">
+        <v>2008</v>
+      </c>
+      <c r="D15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="F15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1974,6 +2228,9 @@
     <hyperlink ref="E7" r:id="rId5" xr:uid="{D9995BB9-537F-4F22-BB62-7F47B6A20D25}"/>
     <hyperlink ref="E3" r:id="rId6" xr:uid="{B3ADECFE-DF4D-4251-89D4-973E831A4DC5}"/>
     <hyperlink ref="E10" r:id="rId7" xr:uid="{FE90C9A5-8CAA-4399-9D7F-A79798808E4E}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{FA159502-D871-48B6-BF13-936603692024}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{E9DA7171-DCDC-459E-9319-AD7D4C4C193D}"/>
+    <hyperlink ref="E15" r:id="rId10" xr:uid="{A12914E5-AF85-4EA9-814D-4FC82B75214B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4367,7 +4624,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
@@ -5273,7 +5530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E1761F-2504-4C8D-8040-F9E9B5E3E6FE}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -5410,6 +5667,248 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE718DA-91F3-45FB-AD2F-2A0676B90C2D}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0.27</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4">
+        <v>6.12</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5">
+        <v>2.36</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <f>(B5+B3)/2</f>
+        <v>3.21</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>4.04</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>5028</v>
+      </c>
+      <c r="D9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>2831</v>
+      </c>
+      <c r="D10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5418,8 +5917,8 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37:C38"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6066,7 +6565,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>63</v>
@@ -6095,20 +6594,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A9BE73-D660-402D-8ABC-7BC4E42D221F}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -6134,7 +6633,7 @@
         <v>2012</v>
       </c>
       <c r="C2">
-        <v>0.36299999999999999</v>
+        <v>0.36288500000000001</v>
       </c>
       <c r="D2">
         <v>5.5190000000000001</v>
@@ -6154,7 +6653,7 @@
         <v>2013</v>
       </c>
       <c r="C3">
-        <v>0.621</v>
+        <v>0.62597400000000003</v>
       </c>
       <c r="D3">
         <v>5.5730000000000004</v>
@@ -6174,7 +6673,7 @@
         <v>2014</v>
       </c>
       <c r="C4">
-        <v>0.78</v>
+        <v>0.785246</v>
       </c>
       <c r="D4">
         <v>5.6150000000000002</v>
@@ -6194,7 +6693,7 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0.93700000000000006</v>
+        <v>0.93709799999999999</v>
       </c>
       <c r="D5">
         <v>5.6559999999999997</v>
@@ -6214,7 +6713,7 @@
         <v>2016</v>
       </c>
       <c r="C6">
-        <v>1.0960000000000001</v>
+        <v>1.0960160000000001</v>
       </c>
       <c r="D6">
         <v>5.7</v>
@@ -6234,7 +6733,7 @@
         <v>2017</v>
       </c>
       <c r="C7">
-        <v>1.2689999999999999</v>
+        <v>1.2689710000000001</v>
       </c>
       <c r="D7">
         <v>5.7140000000000004</v>
@@ -6254,7 +6753,10 @@
         <v>2018</v>
       </c>
       <c r="C8">
-        <v>1.4</v>
+        <v>1.4376409999999999</v>
+      </c>
+      <c r="D8">
+        <v>5.7220000000000004</v>
       </c>
       <c r="E8">
         <v>3.0449999999999999</v>
@@ -6265,42 +6767,24 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>2012</v>
-      </c>
-      <c r="C9">
-        <v>34.076999999999998</v>
-      </c>
-      <c r="D9">
-        <v>4.5179999999999998</v>
-      </c>
-      <c r="E9">
-        <v>30.710999999999999</v>
+        <v>2019</v>
       </c>
       <c r="F9">
-        <v>0.26800000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>2013</v>
-      </c>
-      <c r="C10">
-        <v>36.71</v>
-      </c>
-      <c r="D10">
-        <v>4.5009999999999994</v>
-      </c>
-      <c r="E10">
-        <v>32.969000000000001</v>
+        <v>2020</v>
       </c>
       <c r="F10">
-        <v>0.50800000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -6308,19 +6792,19 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C11">
-        <v>37.9</v>
+        <v>34.076999999999998</v>
       </c>
       <c r="D11">
-        <v>4.4909999999999997</v>
+        <v>4.5179999999999998</v>
       </c>
       <c r="E11">
-        <v>37.619999999999997</v>
+        <v>30.710999999999999</v>
       </c>
       <c r="F11">
-        <v>0.99399999999999999</v>
+        <v>0.26800000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -6328,19 +6812,19 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="C12">
-        <v>39.223999999999997</v>
+        <v>36.71</v>
       </c>
       <c r="D12">
-        <v>4.5</v>
+        <v>4.5009999999999994</v>
       </c>
       <c r="E12">
-        <v>41.296999999999997</v>
+        <v>32.969000000000001</v>
       </c>
       <c r="F12">
-        <v>3.2829999999999999</v>
+        <v>0.50800000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -6348,19 +6832,19 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="C13">
-        <v>40.679000000000002</v>
+        <v>37.9</v>
       </c>
       <c r="D13">
-        <v>4.5</v>
+        <v>4.4909999999999997</v>
       </c>
       <c r="E13">
-        <v>45.283000000000001</v>
+        <v>37.619999999999997</v>
       </c>
       <c r="F13">
-        <v>4.1520000000000001</v>
+        <v>0.99399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -6368,19 +6852,19 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="C14">
-        <v>42.338999999999999</v>
+        <v>39.223999999999997</v>
       </c>
       <c r="D14">
         <v>4.5</v>
       </c>
       <c r="E14">
-        <v>50.290999999999997</v>
+        <v>41.296999999999997</v>
       </c>
       <c r="F14">
-        <v>5.4269999999999996</v>
+        <v>3.2829999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -6388,19 +6872,75 @@
         <v>2</v>
       </c>
       <c r="B15">
+        <v>2016</v>
+      </c>
+      <c r="C15">
+        <v>40.679000000000002</v>
+      </c>
+      <c r="D15">
+        <v>4.5</v>
+      </c>
+      <c r="E15">
+        <v>45.283000000000001</v>
+      </c>
+      <c r="F15">
+        <v>4.1520000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2017</v>
+      </c>
+      <c r="C16">
+        <v>42.338999999999999</v>
+      </c>
+      <c r="D16">
+        <v>4.5</v>
+      </c>
+      <c r="E16">
+        <v>50.290999999999997</v>
+      </c>
+      <c r="F16">
+        <v>5.4269999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
         <v>2018</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>45.277000000000001</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>4.5069999999999997</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>52.564999999999998</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>6.4169999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -6416,14 +6956,17 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>147</v>
@@ -6441,7 +6984,7 @@
         <v>146</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>149</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6452,7 +6995,6 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <f>C6</f>
         <v>40</v>
       </c>
       <c r="D2" s="20">
@@ -6468,10 +7010,11 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
-        <f>ROUND($D2*(WACC!$B$2*(1+WACC!$B$2)^$C2)/((1+WACC!$B$2)^$C2-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C2)/((1+WACC!$B$2)^$C2-1)*$D2,0)</f>
         <v>36715</v>
       </c>
-      <c r="I2" s="25"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -6497,7 +7040,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <f>ROUND($D3*(WACC!$B$2*(1+WACC!$B$2)^$C3)/((1+WACC!$B$2)^$C3-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C3)/((1+WACC!$B$2)^$C3-1)*$D3,0)</f>
         <v>153375</v>
       </c>
       <c r="I3" s="25"/>
@@ -6526,7 +7069,7 @@
         <v>1.35</v>
       </c>
       <c r="G4" s="1">
-        <f>ROUND($D4*(WACC!$B$2*(1+WACC!$B$2)^$C4)/((1+WACC!$B$2)^$C4-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C4)/((1+WACC!$B$2)^$C4-1)*$D4,0)</f>
         <v>67653</v>
       </c>
       <c r="I4" s="25"/>
@@ -6555,7 +7098,7 @@
         <v>2.7</v>
       </c>
       <c r="G5" s="1">
-        <f>ROUND($D5*(WACC!$B$2*(1+WACC!$B$2)^$C5)/((1+WACC!$B$2)^$C5-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C5)/((1+WACC!$B$2)^$C5-1)*$D5,0)</f>
         <v>125549</v>
       </c>
       <c r="I5" s="25"/>
@@ -6580,7 +7123,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <f>ROUND($D6*(WACC!$B$3*(1+WACC!$B$3)^$C6)/((1+WACC!$B$3)^$C6-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C6)/((1+WACC!$B$3)^$C6-1)*$D6,0)</f>
         <v>27255</v>
       </c>
       <c r="I6" s="25"/>
@@ -6605,7 +7148,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f>ROUND($D7*(WACC!$B$3*(1+WACC!$B$3)^$C7)/((1+WACC!$B$3)^$C7-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C7)/((1+WACC!$B$3)^$C7-1)*$D7,0)</f>
         <v>108823</v>
       </c>
       <c r="I7" s="25"/>
@@ -6630,7 +7173,7 @@
         <v>1.35</v>
       </c>
       <c r="G8" s="1">
-        <f>ROUND($D8*(WACC!$B$3*(1+WACC!$B$3)^$C8)/((1+WACC!$B$3)^$C8-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C8)/((1+WACC!$B$3)^$C8-1)*$D8,0)</f>
         <v>53060</v>
       </c>
       <c r="I8" s="25"/>
@@ -6655,7 +7198,7 @@
         <v>2.7</v>
       </c>
       <c r="G9" s="1">
-        <f>ROUND($D9*(WACC!$B$3*(1+WACC!$B$3)^$C9)/((1+WACC!$B$3)^$C9-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C9)/((1+WACC!$B$3)^$C9-1)*$D9,0)</f>
         <v>98467</v>
       </c>
       <c r="I9" s="25"/>
@@ -6684,7 +7227,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>147</v>
@@ -9239,7 +9782,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="O27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="S36" sqref="S36"/>
@@ -9263,64 +9806,64 @@
         <v>65</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="S1" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="R1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="S1" s="14" t="s">
+      <c r="T1" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="V1" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="V1" s="14" t="s">
-        <v>194</v>
-      </c>
       <c r="W1" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X1" s="14"/>
       <c r="Y1" s="14"/>
@@ -9335,28 +9878,28 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2" t="s">
         <v>195</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>196</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>197</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>198</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>199</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>200</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>201</v>
-      </c>
-      <c r="L2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -9376,31 +9919,31 @@
         <v>0.34</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -9454,31 +9997,31 @@
         <v>0.35199999999999998</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -9567,7 +10110,7 @@
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S5">
         <v>1700</v>
@@ -9614,31 +10157,31 @@
         <v>0.439</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -9728,7 +10271,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S7">
         <f>ROUND(S6/0.95,0)</f>
@@ -9745,7 +10288,7 @@
         <v>40</v>
       </c>
       <c r="W7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
@@ -9777,31 +10320,31 @@
         <v>0.375</v>
       </c>
       <c r="G8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -9822,7 +10365,7 @@
         <v>40</v>
       </c>
       <c r="W8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
@@ -9890,7 +10433,7 @@
         <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S9">
         <f>ROUND(S8/0.95,0)</f>
@@ -9906,7 +10449,7 @@
         <v>40</v>
       </c>
       <c r="W9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
@@ -9938,31 +10481,31 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="G10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -9983,7 +10526,7 @@
         <v>40</v>
       </c>
       <c r="W10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
@@ -10051,7 +10594,7 @@
         <v>1</v>
       </c>
       <c r="Q11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S11">
         <f>ROUND(S10/0.95,0)</f>
@@ -10067,7 +10610,7 @@
         <v>40</v>
       </c>
       <c r="W11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
@@ -10099,31 +10642,31 @@
         <v>0.48499999999999999</v>
       </c>
       <c r="G12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P12">
         <v>1</v>
@@ -10144,7 +10687,7 @@
         <v>40</v>
       </c>
       <c r="W12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
@@ -10260,31 +10803,31 @@
         <v>0.46</v>
       </c>
       <c r="G14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -10338,31 +10881,31 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="G15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q15">
         <v>4</v>
@@ -10445,7 +10988,7 @@
         <v>0.8</v>
       </c>
       <c r="Q16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S16">
         <v>400</v>
@@ -10477,7 +11020,7 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C17" t="s">
         <v>94</v>
@@ -10492,31 +11035,31 @@
         <v>0.32800000000000001</v>
       </c>
       <c r="G17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -10554,7 +11097,7 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
         <v>96</v>
@@ -10652,31 +11195,31 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -10697,7 +11240,7 @@
         <v>30</v>
       </c>
       <c r="W19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
@@ -10781,7 +11324,7 @@
         <v>30</v>
       </c>
       <c r="W20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
@@ -10813,31 +11356,31 @@
         <v>0.61</v>
       </c>
       <c r="G21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P21">
         <v>1</v>
@@ -10977,31 +11520,31 @@
         <v>0.47</v>
       </c>
       <c r="G23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q23">
         <v>1</v>
@@ -11123,7 +11666,7 @@
         <v>49.5</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25" t="s">
         <v>104</v>
@@ -11138,31 +11681,31 @@
         <v>0.95</v>
       </c>
       <c r="G25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P25">
         <v>1</v>
@@ -11215,31 +11758,31 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="G26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q26">
         <v>4</v>
@@ -11322,7 +11865,7 @@
         <v>0.8</v>
       </c>
       <c r="Q27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S27">
         <v>400</v>
@@ -11354,7 +11897,7 @@
         <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C28" t="s">
         <v>107</v>
@@ -11369,31 +11912,31 @@
         <v>0.41</v>
       </c>
       <c r="G28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P28">
         <v>1</v>
@@ -11446,31 +11989,31 @@
         <v>0.47</v>
       </c>
       <c r="G29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q29">
         <v>4</v>
@@ -11553,7 +12096,7 @@
         <v>0.8</v>
       </c>
       <c r="Q30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S30">
         <f>ROUND(S29/0.95,0)</f>
@@ -11569,7 +12112,7 @@
         <v>25</v>
       </c>
       <c r="W30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
@@ -11595,34 +12138,34 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S31">
         <v>3000</v>
@@ -11637,7 +12180,7 @@
         <v>60</v>
       </c>
       <c r="W31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
@@ -11654,7 +12197,7 @@
         <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C32" t="s">
         <v>112</v>
@@ -11663,34 +12206,34 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S32">
         <v>2000</v>
@@ -11705,7 +12248,7 @@
         <v>60</v>
       </c>
       <c r="W32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
@@ -11731,34 +12274,34 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S33">
         <v>2000</v>
@@ -11773,7 +12316,7 @@
         <v>60</v>
       </c>
       <c r="W33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
@@ -11805,31 +12348,31 @@
         <v>0.29599999999999999</v>
       </c>
       <c r="G34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q34">
         <v>1</v>
@@ -11948,7 +12491,7 @@
         <v>100</v>
       </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C36" t="s">
         <v>116</v>
@@ -11963,31 +12506,31 @@
         <v>3.6</v>
       </c>
       <c r="G36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P36">
         <v>1</v>
@@ -12025,10 +12568,10 @@
         <v>101</v>
       </c>
       <c r="B37" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" t="s">
         <v>213</v>
-      </c>
-      <c r="C37" t="s">
-        <v>214</v>
       </c>
       <c r="D37">
         <v>2020</v>
@@ -12040,31 +12583,31 @@
         <v>1.71</v>
       </c>
       <c r="G37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P37">
         <v>1</v>
@@ -12102,10 +12645,10 @@
         <v>102</v>
       </c>
       <c r="B38" t="s">
+        <v>214</v>
+      </c>
+      <c r="C38" t="s">
         <v>215</v>
-      </c>
-      <c r="C38" t="s">
-        <v>216</v>
       </c>
       <c r="D38">
         <v>2020</v>
@@ -12117,31 +12660,31 @@
         <v>0.99</v>
       </c>
       <c r="G38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P38">
         <v>1</v>

</xml_diff>

<commit_message>
* updates data_static.xlsx * updates medea_regional_timeseries.csv
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D6A6C7-FDD2-4011-9F16-8266461645C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06905E4-24CD-4569-A413-494C0077B95A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="860" activeTab="13" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="31200" yWindow="2160" windowWidth="21600" windowHeight="12735" tabRatio="860" firstSheet="6" activeTab="14" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="ATC" sheetId="3" r:id="rId12"/>
     <sheet name="KM" sheetId="4" r:id="rId13"/>
     <sheet name="potentials" sheetId="19" r:id="rId14"/>
+    <sheet name="AIR_POLLUTION" sheetId="20" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -639,8 +640,43 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sebastian</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2C3BF732-EB70-4318-A3DC-57E3173C0EC6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lifecycle air pollution cost of state-of-the-art (in around 2009) electricity generation technologies in € of 2015. 
+Total of health impacts, crop yield losses, and material damage.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="259">
   <si>
     <t>year</t>
   </si>
@@ -1089,9 +1125,6 @@
     <t>total installed cost</t>
   </si>
   <si>
-    <t>annuity of total installed cost</t>
-  </si>
-  <si>
     <t>zone</t>
   </si>
   <si>
@@ -1315,22 +1348,129 @@
   </si>
   <si>
     <t>1, 8</t>
+  </si>
+  <si>
+    <t>equivalent annual cost</t>
+  </si>
+  <si>
+    <t>Sascha Samadi</t>
+  </si>
+  <si>
+    <t>The Social Costs of Electricity Generation - Categorizing Different Types of Costs and Evaluating Their Respective Relevance</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/1996-1073/10/3/356</t>
+  </si>
+  <si>
+    <t>NEEDS Project</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D7.2%20Final%20report%20on%20advanced%20fossil%20power%20plants.pdf</t>
+  </si>
+  <si>
+    <t>Final report on technical data, costs, and life cycle inventories of advanced fossil power generation systems</t>
+  </si>
+  <si>
+    <t>Final report on technical data, costs and life cycle inventories of biomass CHP plants</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D13.2%20Final%20report%20on%20Biomass%20technologies.pdf</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D11.2%20Final%20report%20on%20PV%20technology.pdf</t>
+  </si>
+  <si>
+    <t>Table 16, page 51</t>
+  </si>
+  <si>
+    <t>Final report on technical data, costs and life cycle inventories of PV applications</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D10.2.pdf</t>
+  </si>
+  <si>
+    <t>Table 5.3, page 39</t>
+  </si>
+  <si>
+    <t>Final report on offshore wind technology</t>
+  </si>
+  <si>
+    <t>Table 7, page 16</t>
+  </si>
+  <si>
+    <t>10, 11</t>
+  </si>
+  <si>
+    <t>10, 14</t>
+  </si>
+  <si>
+    <t>10, 13</t>
+  </si>
+  <si>
+    <t>10, 12</t>
+  </si>
+  <si>
+    <t>10, 8</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>fixed cost</t>
+  </si>
+  <si>
+    <t>wind offshore in soure; 4044 full-load hours</t>
+  </si>
+  <si>
+    <t>utility scale pv, 838 full-load hours</t>
+  </si>
+  <si>
+    <t>avg of lignite and nat gas due to lack of data</t>
+  </si>
+  <si>
+    <t>no data available</t>
+  </si>
+  <si>
+    <t>Syngas</t>
+  </si>
+  <si>
+    <t>43.2% net efficiency</t>
+  </si>
+  <si>
+    <t>45.0% net efficiency</t>
+  </si>
+  <si>
+    <t>57.5% net efficiency</t>
+  </si>
+  <si>
+    <t>20.0% net efficiency</t>
+  </si>
+  <si>
+    <t>34.0% net efficiency</t>
+  </si>
+  <si>
+    <t>variable cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="170" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="169" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1387,6 +1527,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1416,7 +1569,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1449,8 +1602,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1460,9 +1613,11 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1779,10 +1934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3387BF03-EDC5-4C83-AB6F-3B95A2E59024}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,22 +1949,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,16 +1972,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2">
         <v>2016</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,16 +1989,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1851,16 +2006,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4">
         <v>2013</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,16 +2023,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5">
         <v>2014</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,16 +2040,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,16 +2057,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7">
         <v>2014</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1919,16 +2074,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1936,16 +2091,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1953,16 +2108,115 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C10">
         <v>2017</v>
       </c>
       <c r="D10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>220</v>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C11">
+        <v>2017</v>
+      </c>
+      <c r="D11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12">
+        <v>2007</v>
+      </c>
+      <c r="D12" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13">
+        <v>2008</v>
+      </c>
+      <c r="D13" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14">
+        <v>2008</v>
+      </c>
+      <c r="D14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15">
+        <v>2008</v>
+      </c>
+      <c r="D15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="F15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1974,6 +2228,9 @@
     <hyperlink ref="E7" r:id="rId5" xr:uid="{D9995BB9-537F-4F22-BB62-7F47B6A20D25}"/>
     <hyperlink ref="E3" r:id="rId6" xr:uid="{B3ADECFE-DF4D-4251-89D4-973E831A4DC5}"/>
     <hyperlink ref="E10" r:id="rId7" xr:uid="{FE90C9A5-8CAA-4399-9D7F-A79798808E4E}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{FA159502-D871-48B6-BF13-936603692024}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{E9DA7171-DCDC-459E-9319-AD7D4C4C193D}"/>
+    <hyperlink ref="E15" r:id="rId10" xr:uid="{A12914E5-AF85-4EA9-814D-4FC82B75214B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4367,7 +4624,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
@@ -5273,7 +5530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E1761F-2504-4C8D-8040-F9E9B5E3E6FE}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -5410,6 +5667,248 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE718DA-91F3-45FB-AD2F-2A0676B90C2D}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0.27</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4">
+        <v>6.12</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5">
+        <v>2.36</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <f>(B5+B3)/2</f>
+        <v>3.21</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>4.04</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>5028</v>
+      </c>
+      <c r="D9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>2831</v>
+      </c>
+      <c r="D10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5418,8 +5917,8 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37:C38"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6066,7 +6565,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>63</v>
@@ -6095,20 +6594,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A9BE73-D660-402D-8ABC-7BC4E42D221F}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -6134,7 +6633,7 @@
         <v>2012</v>
       </c>
       <c r="C2">
-        <v>0.36299999999999999</v>
+        <v>0.36288500000000001</v>
       </c>
       <c r="D2">
         <v>5.5190000000000001</v>
@@ -6154,7 +6653,7 @@
         <v>2013</v>
       </c>
       <c r="C3">
-        <v>0.621</v>
+        <v>0.62597400000000003</v>
       </c>
       <c r="D3">
         <v>5.5730000000000004</v>
@@ -6174,7 +6673,7 @@
         <v>2014</v>
       </c>
       <c r="C4">
-        <v>0.78</v>
+        <v>0.785246</v>
       </c>
       <c r="D4">
         <v>5.6150000000000002</v>
@@ -6194,7 +6693,7 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0.93700000000000006</v>
+        <v>0.93709799999999999</v>
       </c>
       <c r="D5">
         <v>5.6559999999999997</v>
@@ -6214,7 +6713,7 @@
         <v>2016</v>
       </c>
       <c r="C6">
-        <v>1.0960000000000001</v>
+        <v>1.0960160000000001</v>
       </c>
       <c r="D6">
         <v>5.7</v>
@@ -6234,7 +6733,7 @@
         <v>2017</v>
       </c>
       <c r="C7">
-        <v>1.2689999999999999</v>
+        <v>1.2689710000000001</v>
       </c>
       <c r="D7">
         <v>5.7140000000000004</v>
@@ -6254,7 +6753,10 @@
         <v>2018</v>
       </c>
       <c r="C8">
-        <v>1.4</v>
+        <v>1.4376409999999999</v>
+      </c>
+      <c r="D8">
+        <v>5.7220000000000004</v>
       </c>
       <c r="E8">
         <v>3.0449999999999999</v>
@@ -6265,42 +6767,24 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>2012</v>
-      </c>
-      <c r="C9">
-        <v>34.076999999999998</v>
-      </c>
-      <c r="D9">
-        <v>4.5179999999999998</v>
-      </c>
-      <c r="E9">
-        <v>30.710999999999999</v>
+        <v>2019</v>
       </c>
       <c r="F9">
-        <v>0.26800000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>2013</v>
-      </c>
-      <c r="C10">
-        <v>36.71</v>
-      </c>
-      <c r="D10">
-        <v>4.5009999999999994</v>
-      </c>
-      <c r="E10">
-        <v>32.969000000000001</v>
+        <v>2020</v>
       </c>
       <c r="F10">
-        <v>0.50800000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -6308,19 +6792,19 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C11">
-        <v>37.9</v>
+        <v>34.076999999999998</v>
       </c>
       <c r="D11">
-        <v>4.4909999999999997</v>
+        <v>4.5179999999999998</v>
       </c>
       <c r="E11">
-        <v>37.619999999999997</v>
+        <v>30.710999999999999</v>
       </c>
       <c r="F11">
-        <v>0.99399999999999999</v>
+        <v>0.26800000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -6328,19 +6812,19 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="C12">
-        <v>39.223999999999997</v>
+        <v>36.71</v>
       </c>
       <c r="D12">
-        <v>4.5</v>
+        <v>4.5009999999999994</v>
       </c>
       <c r="E12">
-        <v>41.296999999999997</v>
+        <v>32.969000000000001</v>
       </c>
       <c r="F12">
-        <v>3.2829999999999999</v>
+        <v>0.50800000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -6348,19 +6832,19 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="C13">
-        <v>40.679000000000002</v>
+        <v>37.9</v>
       </c>
       <c r="D13">
-        <v>4.5</v>
+        <v>4.4909999999999997</v>
       </c>
       <c r="E13">
-        <v>45.283000000000001</v>
+        <v>37.619999999999997</v>
       </c>
       <c r="F13">
-        <v>4.1520000000000001</v>
+        <v>0.99399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -6368,19 +6852,19 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="C14">
-        <v>42.338999999999999</v>
+        <v>39.223999999999997</v>
       </c>
       <c r="D14">
         <v>4.5</v>
       </c>
       <c r="E14">
-        <v>50.290999999999997</v>
+        <v>41.296999999999997</v>
       </c>
       <c r="F14">
-        <v>5.4269999999999996</v>
+        <v>3.2829999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -6388,19 +6872,75 @@
         <v>2</v>
       </c>
       <c r="B15">
+        <v>2016</v>
+      </c>
+      <c r="C15">
+        <v>40.679000000000002</v>
+      </c>
+      <c r="D15">
+        <v>4.5</v>
+      </c>
+      <c r="E15">
+        <v>45.283000000000001</v>
+      </c>
+      <c r="F15">
+        <v>4.1520000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2017</v>
+      </c>
+      <c r="C16">
+        <v>42.338999999999999</v>
+      </c>
+      <c r="D16">
+        <v>4.5</v>
+      </c>
+      <c r="E16">
+        <v>50.290999999999997</v>
+      </c>
+      <c r="F16">
+        <v>5.4269999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
         <v>2018</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>45.277000000000001</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>4.5069999999999997</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>52.564999999999998</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>6.4169999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -6416,14 +6956,17 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>147</v>
@@ -6441,7 +6984,7 @@
         <v>146</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>149</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6452,7 +6995,6 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <f>C6</f>
         <v>40</v>
       </c>
       <c r="D2" s="20">
@@ -6468,10 +7010,11 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
-        <f>ROUND($D2*(WACC!$B$2*(1+WACC!$B$2)^$C2)/((1+WACC!$B$2)^$C2-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C2)/((1+WACC!$B$2)^$C2-1)*$D2,0)</f>
         <v>36715</v>
       </c>
-      <c r="I2" s="25"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -6497,7 +7040,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <f>ROUND($D3*(WACC!$B$2*(1+WACC!$B$2)^$C3)/((1+WACC!$B$2)^$C3-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C3)/((1+WACC!$B$2)^$C3-1)*$D3,0)</f>
         <v>153375</v>
       </c>
       <c r="I3" s="25"/>
@@ -6526,7 +7069,7 @@
         <v>1.35</v>
       </c>
       <c r="G4" s="1">
-        <f>ROUND($D4*(WACC!$B$2*(1+WACC!$B$2)^$C4)/((1+WACC!$B$2)^$C4-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C4)/((1+WACC!$B$2)^$C4-1)*$D4,0)</f>
         <v>67653</v>
       </c>
       <c r="I4" s="25"/>
@@ -6555,7 +7098,7 @@
         <v>2.7</v>
       </c>
       <c r="G5" s="1">
-        <f>ROUND($D5*(WACC!$B$2*(1+WACC!$B$2)^$C5)/((1+WACC!$B$2)^$C5-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C5)/((1+WACC!$B$2)^$C5-1)*$D5,0)</f>
         <v>125549</v>
       </c>
       <c r="I5" s="25"/>
@@ -6580,7 +7123,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <f>ROUND($D6*(WACC!$B$3*(1+WACC!$B$3)^$C6)/((1+WACC!$B$3)^$C6-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C6)/((1+WACC!$B$3)^$C6-1)*$D6,0)</f>
         <v>27255</v>
       </c>
       <c r="I6" s="25"/>
@@ -6605,7 +7148,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f>ROUND($D7*(WACC!$B$3*(1+WACC!$B$3)^$C7)/((1+WACC!$B$3)^$C7-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C7)/((1+WACC!$B$3)^$C7-1)*$D7,0)</f>
         <v>108823</v>
       </c>
       <c r="I7" s="25"/>
@@ -6630,7 +7173,7 @@
         <v>1.35</v>
       </c>
       <c r="G8" s="1">
-        <f>ROUND($D8*(WACC!$B$3*(1+WACC!$B$3)^$C8)/((1+WACC!$B$3)^$C8-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C8)/((1+WACC!$B$3)^$C8-1)*$D8,0)</f>
         <v>53060</v>
       </c>
       <c r="I8" s="25"/>
@@ -6655,7 +7198,7 @@
         <v>2.7</v>
       </c>
       <c r="G9" s="1">
-        <f>ROUND($D9*(WACC!$B$3*(1+WACC!$B$3)^$C9)/((1+WACC!$B$3)^$C9-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C9)/((1+WACC!$B$3)^$C9-1)*$D9,0)</f>
         <v>98467</v>
       </c>
       <c r="I9" s="25"/>
@@ -6684,7 +7227,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>147</v>
@@ -9239,7 +9782,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="O27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="S36" sqref="S36"/>
@@ -9263,64 +9806,64 @@
         <v>65</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="S1" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="R1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="S1" s="14" t="s">
+      <c r="T1" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="V1" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="V1" s="14" t="s">
-        <v>194</v>
-      </c>
       <c r="W1" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X1" s="14"/>
       <c r="Y1" s="14"/>
@@ -9335,28 +9878,28 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2" t="s">
         <v>195</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>196</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>197</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>198</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>199</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>200</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>201</v>
-      </c>
-      <c r="L2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -9376,31 +9919,31 @@
         <v>0.34</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -9454,31 +9997,31 @@
         <v>0.35199999999999998</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -9567,7 +10110,7 @@
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S5">
         <v>1700</v>
@@ -9614,31 +10157,31 @@
         <v>0.439</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -9728,7 +10271,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S7">
         <f>ROUND(S6/0.95,0)</f>
@@ -9745,7 +10288,7 @@
         <v>40</v>
       </c>
       <c r="W7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
@@ -9777,31 +10320,31 @@
         <v>0.375</v>
       </c>
       <c r="G8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -9822,7 +10365,7 @@
         <v>40</v>
       </c>
       <c r="W8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
@@ -9890,7 +10433,7 @@
         <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S9">
         <f>ROUND(S8/0.95,0)</f>
@@ -9906,7 +10449,7 @@
         <v>40</v>
       </c>
       <c r="W9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
@@ -9938,31 +10481,31 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="G10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -9983,7 +10526,7 @@
         <v>40</v>
       </c>
       <c r="W10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
@@ -10051,7 +10594,7 @@
         <v>1</v>
       </c>
       <c r="Q11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S11">
         <f>ROUND(S10/0.95,0)</f>
@@ -10067,7 +10610,7 @@
         <v>40</v>
       </c>
       <c r="W11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
@@ -10099,31 +10642,31 @@
         <v>0.48499999999999999</v>
       </c>
       <c r="G12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P12">
         <v>1</v>
@@ -10144,7 +10687,7 @@
         <v>40</v>
       </c>
       <c r="W12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
@@ -10260,31 +10803,31 @@
         <v>0.46</v>
       </c>
       <c r="G14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -10338,31 +10881,31 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="G15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q15">
         <v>4</v>
@@ -10445,7 +10988,7 @@
         <v>0.8</v>
       </c>
       <c r="Q16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S16">
         <v>400</v>
@@ -10477,7 +11020,7 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C17" t="s">
         <v>94</v>
@@ -10492,31 +11035,31 @@
         <v>0.32800000000000001</v>
       </c>
       <c r="G17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -10554,7 +11097,7 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
         <v>96</v>
@@ -10652,31 +11195,31 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -10697,7 +11240,7 @@
         <v>30</v>
       </c>
       <c r="W19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
@@ -10781,7 +11324,7 @@
         <v>30</v>
       </c>
       <c r="W20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
@@ -10813,31 +11356,31 @@
         <v>0.61</v>
       </c>
       <c r="G21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P21">
         <v>1</v>
@@ -10977,31 +11520,31 @@
         <v>0.47</v>
       </c>
       <c r="G23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q23">
         <v>1</v>
@@ -11123,7 +11666,7 @@
         <v>49.5</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25" t="s">
         <v>104</v>
@@ -11138,31 +11681,31 @@
         <v>0.95</v>
       </c>
       <c r="G25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P25">
         <v>1</v>
@@ -11215,31 +11758,31 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="G26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q26">
         <v>4</v>
@@ -11322,7 +11865,7 @@
         <v>0.8</v>
       </c>
       <c r="Q27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S27">
         <v>400</v>
@@ -11354,7 +11897,7 @@
         <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C28" t="s">
         <v>107</v>
@@ -11369,31 +11912,31 @@
         <v>0.41</v>
       </c>
       <c r="G28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P28">
         <v>1</v>
@@ -11446,31 +11989,31 @@
         <v>0.47</v>
       </c>
       <c r="G29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q29">
         <v>4</v>
@@ -11553,7 +12096,7 @@
         <v>0.8</v>
       </c>
       <c r="Q30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S30">
         <f>ROUND(S29/0.95,0)</f>
@@ -11569,7 +12112,7 @@
         <v>25</v>
       </c>
       <c r="W30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
@@ -11595,34 +12138,34 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S31">
         <v>3000</v>
@@ -11637,7 +12180,7 @@
         <v>60</v>
       </c>
       <c r="W31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
@@ -11654,7 +12197,7 @@
         <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C32" t="s">
         <v>112</v>
@@ -11663,34 +12206,34 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S32">
         <v>2000</v>
@@ -11705,7 +12248,7 @@
         <v>60</v>
       </c>
       <c r="W32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
@@ -11731,34 +12274,34 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S33">
         <v>2000</v>
@@ -11773,7 +12316,7 @@
         <v>60</v>
       </c>
       <c r="W33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
@@ -11805,31 +12348,31 @@
         <v>0.29599999999999999</v>
       </c>
       <c r="G34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q34">
         <v>1</v>
@@ -11948,7 +12491,7 @@
         <v>100</v>
       </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C36" t="s">
         <v>116</v>
@@ -11963,31 +12506,31 @@
         <v>3.6</v>
       </c>
       <c r="G36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P36">
         <v>1</v>
@@ -12025,10 +12568,10 @@
         <v>101</v>
       </c>
       <c r="B37" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" t="s">
         <v>213</v>
-      </c>
-      <c r="C37" t="s">
-        <v>214</v>
       </c>
       <c r="D37">
         <v>2020</v>
@@ -12040,31 +12583,31 @@
         <v>1.71</v>
       </c>
       <c r="G37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P37">
         <v>1</v>
@@ -12102,10 +12645,10 @@
         <v>102</v>
       </c>
       <c r="B38" t="s">
+        <v>214</v>
+      </c>
+      <c r="C38" t="s">
         <v>215</v>
-      </c>
-      <c r="C38" t="s">
-        <v>216</v>
       </c>
       <c r="D38">
         <v>2020</v>
@@ -12117,31 +12660,31 @@
         <v>0.99</v>
       </c>
       <c r="G38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P38">
         <v>1</v>

</xml_diff>

<commit_message>
adds draft of undisturbed landscapes-paper
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seb/git_repos/medea/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06905E4-24CD-4569-A413-494C0077B95A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE7B8B6-FD6E-5749-86A4-B7B64E0B36E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31200" yWindow="2160" windowWidth="21600" windowHeight="12735" tabRatio="860" firstSheet="6" activeTab="14" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" tabRatio="860" activeTab="7" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -676,7 +676,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="259">
   <si>
     <t>year</t>
   </si>
@@ -1290,9 +1290,6 @@
     <t>3, 1, 8</t>
   </si>
   <si>
-    <t>6, 1</t>
-  </si>
-  <si>
     <t>4, 7, 8</t>
   </si>
   <si>
@@ -1453,6 +1450,9 @@
   </si>
   <si>
     <t>variable cost</t>
+  </si>
+  <si>
+    <t>6, 9</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1470,7 @@
     <numFmt numFmtId="171" formatCode="#,##0.0000"/>
     <numFmt numFmtId="172" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1940,14 +1940,14 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="90.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>151</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2103,118 +2103,118 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C10">
         <v>2017</v>
       </c>
       <c r="D10" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C11">
         <v>2017</v>
       </c>
       <c r="D11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" t="s">
         <v>226</v>
       </c>
-      <c r="E11" t="s">
-        <v>227</v>
-      </c>
       <c r="F11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C12">
         <v>2007</v>
       </c>
       <c r="D12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E12" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="F12" t="s">
         <v>233</v>
       </c>
-      <c r="F12" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C13">
         <v>2008</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14">
         <v>2008</v>
       </c>
       <c r="D14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" t="s">
         <v>231</v>
       </c>
-      <c r="E14" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C15">
         <v>2008</v>
       </c>
       <c r="D15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E15" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="F15" t="s">
         <v>236</v>
       </c>
-      <c r="F15" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2247,13 +2247,13 @@
       <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="11.42578125" style="5"/>
-    <col min="5" max="5" width="11.42578125" style="17"/>
+    <col min="1" max="4" width="11.5" style="5"/>
+    <col min="5" max="5" width="11.5" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2271,7 +2271,7 @@
       </c>
       <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="4">
         <v>10</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>10</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>0.83330000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="4">
         <v>10</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>0.54049999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="4">
         <v>10</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="4">
         <v>20</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="4">
         <v>20</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>0.90629999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="4">
         <v>20</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>0.59460000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="4">
         <v>20</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="4">
         <v>20.5</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="4">
         <v>20.5</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="4">
         <v>20.5</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="4">
         <v>20.5</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="4">
         <v>21</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="4">
         <v>21</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>0.92710000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="4">
         <v>21</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>0.37840000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="4">
         <v>21</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="4">
         <v>21.5</v>
       </c>
@@ -2564,7 +2564,7 @@
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="4">
         <v>21.5</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="4">
         <v>21.5</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="4">
         <v>21.5</v>
       </c>
@@ -2619,7 +2619,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="4">
         <v>30</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="4">
         <v>30</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>0.9375</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="4">
         <v>30</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>0.56759999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="4">
         <v>30</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="4">
         <v>30.5</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="4">
         <v>30.5</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="4">
         <v>30.5</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="4">
         <v>30.5</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="4">
         <v>31</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="4">
         <v>31</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>0.91149999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>0.43240000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="4">
         <v>31.5</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="4">
         <v>31.5</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="4">
         <v>31.5</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="4">
         <v>31.5</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="4">
         <v>32</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="4">
         <v>32</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>0.88539999999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="4">
         <v>32</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>0.37840000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="4">
         <v>32</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="4">
         <v>32.5</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="4">
         <v>32.5</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="4">
         <v>32.5</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="4">
         <v>32.5</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="4">
         <v>33</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="4">
         <v>33</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0.83330000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="4">
         <v>33</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>0.32429999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="4">
         <v>33</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="4">
         <v>40</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="4">
         <v>40</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>0.91669999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="4">
         <v>40</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>0.64859999999999995</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="4">
         <v>40</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="4">
         <v>40.5</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="4">
         <v>40.5</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="4">
         <v>40.5</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="4">
         <v>40.5</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="4">
         <v>41</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="4">
         <v>41</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>0.83330000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" s="4">
         <v>41</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>0.75680000000000003</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="4">
         <v>41</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="4">
         <v>41.5</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="4">
         <v>41.5</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="4">
         <v>41.5</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="4">
         <v>41.5</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="4">
         <v>42</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="4">
         <v>42</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>0.78129999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="4">
         <v>42</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>0.70269999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="4">
         <v>42</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="4">
         <v>42.5</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="4">
         <v>42.5</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="4">
         <v>42.5</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="4">
         <v>42.5</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="4">
         <v>43</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="A75" s="4">
         <v>43</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>0.88539999999999996</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="4">
         <v>43</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>0.40539999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="4">
         <v>43</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="4">
         <v>43.5</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="4">
         <v>43.5</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="4">
         <v>43.5</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="4">
         <v>43.5</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" s="4">
         <v>44</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="4">
         <v>44</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>0.85940000000000005</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84" s="4">
         <v>44</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>0.29730000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="4">
         <v>44</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="4">
         <v>44.5</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="4">
         <v>44.5</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="4">
         <v>44.5</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="4">
         <v>44.5</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="4">
         <v>45</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="4">
         <v>45</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>0.84379999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="4">
         <v>45</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>0.28110000000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="4">
         <v>45</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="4">
         <v>45.5</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="4">
         <v>45.5</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="4">
         <v>45.5</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="4">
         <v>45.5</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="4">
         <v>49.5</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="4">
         <v>49.5</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>0.72600000000000009</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="4">
         <v>49.5</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>0.34350000000000003</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5">
       <c r="A101" s="4">
         <v>49.5</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="4">
         <v>50</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="4">
         <v>50</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>0.91669999999999996</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="4">
         <v>50</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>0.54049999999999998</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="4">
         <v>50</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="4">
         <v>50.5</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="4">
         <v>50.5</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="4">
         <v>50.5</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5">
       <c r="A109" s="4">
         <v>50.5</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="4">
         <v>51</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="4">
         <v>51</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>0.80730000000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="4">
         <v>51</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>0.64859999999999995</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="4">
         <v>51</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5">
       <c r="A114" s="4">
         <v>51.5</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="4">
         <v>51.5</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="4">
         <v>51.5</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="4">
         <v>51.5</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="4">
         <v>52</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="4">
         <v>52</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>0.88539999999999996</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="4">
         <v>52</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>0.51349999999999996</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="4">
         <v>52</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="4">
         <v>52.5</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="4">
         <v>52.5</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="4">
         <v>52.5</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="4">
         <v>52.5</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="4">
         <v>70</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="4">
         <v>70</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>0.85419999999999996</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="4">
         <v>70</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>0.54049999999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" s="4">
         <v>70</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" s="4">
         <v>70.5</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" s="4">
         <v>70.5</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" s="4">
         <v>70.5</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" s="4">
         <v>70.5</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5">
       <c r="A134" s="4">
         <v>100</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5">
       <c r="A135" s="4">
         <v>100</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" s="4">
         <v>100</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" s="4">
         <v>100</v>
       </c>
@@ -4620,9 +4620,9 @@
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>149</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4752,9 +4752,9 @@
       <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -4849,7 +4849,7 @@
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -4871,7 +4871,7 @@
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -4926,7 +4926,7 @@
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -4948,7 +4948,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -4976,7 +4976,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -4996,7 +4996,7 @@
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -5018,7 +5018,7 @@
       <c r="L10" s="18"/>
       <c r="N10" s="18"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5039,7 +5039,7 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5082,7 +5082,7 @@
       </c>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -5117,9 +5117,9 @@
       <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5220,7 +5220,7 @@
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -5248,7 +5248,7 @@
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -5312,7 +5312,7 @@
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -5334,7 +5334,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -5362,7 +5362,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -5416,7 +5416,7 @@
       </c>
       <c r="N10" s="18"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5440,7 +5440,7 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5492,7 +5492,7 @@
       </c>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -5534,9 +5534,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>126</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>127</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -5674,33 +5674,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE718DA-91F3-45FB-AD2F-2A0676B90C2D}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -5711,13 +5711,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -5728,13 +5728,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -5745,13 +5745,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -5762,13 +5762,13 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -5780,13 +5780,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -5797,13 +5797,13 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E7">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -5814,13 +5814,13 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E8" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -5831,13 +5831,13 @@
         <v>5028</v>
       </c>
       <c r="D9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -5848,13 +5848,13 @@
         <v>2831</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -5865,13 +5865,13 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -5882,15 +5882,15 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -5899,7 +5899,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E13">
         <v>8</v>
@@ -5921,15 +5921,15 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="15" customFormat="1" ht="32">
       <c r="A1" s="13" t="s">
         <v>18</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>10</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>20.5</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>0.70175438596491224</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3">
         <v>21</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>21.5</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>0.67567567567567566</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="3">
         <v>30</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="3">
         <v>30.5</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>0.70175438596491224</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="3">
         <v>31</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="3">
         <v>31.5</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>0.68965517241379315</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="3">
         <v>32</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="3">
         <v>32.5</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>0.67567567567567566</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="3">
         <v>33</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="3">
         <v>40</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="3">
         <v>40.5</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="3">
         <v>41</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="3">
         <v>41.5</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="3">
         <v>42</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="3">
         <v>42.5</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>0.5494505494505495</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="3">
         <v>43</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="3">
         <v>43.5</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>0.75471698113207553</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="3">
         <v>44</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="3">
         <v>44.5</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>0.63492063492063489</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="3">
         <v>45</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="3">
         <v>45.5</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>0.86956521739130443</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="3">
         <v>49.5</v>
       </c>
@@ -6356,7 +6356,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="3">
         <v>50</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="3">
         <v>50.5</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>0.68965517241379304</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="3">
         <v>51</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="3">
         <v>51.5</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="3">
         <v>52</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="3">
         <v>52.5</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>0.70175438596491235</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="3">
         <v>60</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="3">
         <v>61</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="3">
         <v>62</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="3">
         <v>63</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="3">
         <v>70</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="3">
         <v>70.5</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>0.70175438596491224</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="3">
         <v>100</v>
       </c>
@@ -6561,9 +6561,9 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>149</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6579,7 +6579,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6603,9 +6603,9 @@
       <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>149</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6645,7 +6645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -6745,7 +6745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -6807,7 +6807,7 @@
         <v>0.26800000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>0.99399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -6867,7 +6867,7 @@
         <v>3.2829999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>4.1520000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -6907,7 +6907,7 @@
         <v>5.4269999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>6.4169999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -6959,12 +6959,12 @@
       <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="48">
       <c r="A1" s="2" t="s">
         <v>149</v>
       </c>
@@ -6984,10 +6984,10 @@
         <v>146</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" customHeight="1">
       <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
@@ -7016,7 +7016,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="31"/>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" customHeight="1">
       <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
@@ -7045,7 +7045,7 @@
       </c>
       <c r="I3" s="25"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -7074,7 +7074,7 @@
       </c>
       <c r="I4" s="25"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -7103,7 +7103,7 @@
       </c>
       <c r="I5" s="25"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -7128,7 +7128,7 @@
       </c>
       <c r="I6" s="25"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -7153,7 +7153,7 @@
       </c>
       <c r="I7" s="25"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -7220,12 +7220,12 @@
       <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="7" width="11.42578125" customWidth="1"/>
+    <col min="4" max="7" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="15" customFormat="1" ht="32">
       <c r="A1" s="14" t="s">
         <v>149</v>
       </c>
@@ -7254,7 +7254,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7287,7 +7287,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7320,7 +7320,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -7353,7 +7353,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -7386,7 +7386,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>252.62571387089088</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>252.62571387089088</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -7479,34 +7479,34 @@
         <v>8154.7576875561499</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="D15" s="8"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -7527,15 +7527,15 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
+      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>10</v>
       </c>
@@ -7647,7 +7647,7 @@
       </c>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>20</v>
       </c>
@@ -7706,7 +7706,7 @@
       </c>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>20.5</v>
       </c>
@@ -7765,7 +7765,7 @@
       </c>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>21</v>
       </c>
@@ -7804,11 +7804,11 @@
       </c>
       <c r="M5" s="8">
         <f>LOOKUP($A5,tech_full!$A$3:$A$38,tech_full!$T$3:$T$38)</f>
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="N5" s="1">
         <f>LOOKUP($A5,tech_full!$A$3:$A$38,tech_full!$U$3:$U$38)</f>
-        <v>50000</v>
+        <v>40500</v>
       </c>
       <c r="O5" s="1">
         <f>LOOKUP($A5,tech_full!$A$3:$A$38,tech_full!$V$3:$V$38)</f>
@@ -7824,7 +7824,7 @@
       </c>
       <c r="S5" s="7"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>21.5</v>
       </c>
@@ -7863,11 +7863,11 @@
       </c>
       <c r="M6" s="8">
         <f>LOOKUP($A6,tech_full!$A$3:$A$38,tech_full!$T$3:$T$38)</f>
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="N6" s="1">
         <f>LOOKUP($A6,tech_full!$A$3:$A$38,tech_full!$U$3:$U$38)</f>
-        <v>52625</v>
+        <v>40500</v>
       </c>
       <c r="O6" s="1">
         <f>LOOKUP($A6,tech_full!$A$3:$A$38,tech_full!$V$3:$V$38)</f>
@@ -7883,7 +7883,7 @@
       </c>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>30</v>
       </c>
@@ -7942,7 +7942,7 @@
       </c>
       <c r="S7" s="7"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>30.5</v>
       </c>
@@ -8001,7 +8001,7 @@
       </c>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>31</v>
       </c>
@@ -8060,7 +8060,7 @@
       </c>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>31.5</v>
       </c>
@@ -8119,7 +8119,7 @@
       </c>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>32</v>
       </c>
@@ -8178,7 +8178,7 @@
       </c>
       <c r="S11" s="7"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>32.5</v>
       </c>
@@ -8237,7 +8237,7 @@
       </c>
       <c r="S12" s="7"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>33</v>
       </c>
@@ -8296,7 +8296,7 @@
       </c>
       <c r="S13" s="7"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>40</v>
       </c>
@@ -8355,7 +8355,7 @@
       </c>
       <c r="S14" s="7"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>40.5</v>
       </c>
@@ -8414,7 +8414,7 @@
       </c>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>41</v>
       </c>
@@ -8473,7 +8473,7 @@
       </c>
       <c r="S16" s="7"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>41.5</v>
       </c>
@@ -8532,7 +8532,7 @@
       </c>
       <c r="S17" s="7"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>42</v>
       </c>
@@ -8591,7 +8591,7 @@
       </c>
       <c r="S18" s="7"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>42.5</v>
       </c>
@@ -8650,7 +8650,7 @@
       </c>
       <c r="S19" s="7"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>43</v>
       </c>
@@ -8709,7 +8709,7 @@
       </c>
       <c r="S20" s="7"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>43.5</v>
       </c>
@@ -8768,7 +8768,7 @@
       </c>
       <c r="S21" s="7"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>44</v>
       </c>
@@ -8827,7 +8827,7 @@
       </c>
       <c r="S22" s="7"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>44.5</v>
       </c>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="S23" s="7"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>45</v>
       </c>
@@ -8945,7 +8945,7 @@
       </c>
       <c r="S24" s="7"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>45.5</v>
       </c>
@@ -9004,7 +9004,7 @@
       </c>
       <c r="S25" s="7"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>49.5</v>
       </c>
@@ -9063,7 +9063,7 @@
       </c>
       <c r="S26" s="7"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>50</v>
       </c>
@@ -9122,7 +9122,7 @@
       </c>
       <c r="S27" s="7"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>50.5</v>
       </c>
@@ -9181,7 +9181,7 @@
       </c>
       <c r="S28" s="7"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29">
         <v>51</v>
       </c>
@@ -9240,7 +9240,7 @@
       </c>
       <c r="S29" s="7"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19">
       <c r="A30">
         <v>51.5</v>
       </c>
@@ -9299,7 +9299,7 @@
       </c>
       <c r="S30" s="7"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>52</v>
       </c>
@@ -9358,7 +9358,7 @@
       </c>
       <c r="S31" s="7"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>52.5</v>
       </c>
@@ -9417,7 +9417,7 @@
       </c>
       <c r="S32" s="7"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>60</v>
       </c>
@@ -9476,7 +9476,7 @@
       </c>
       <c r="S33" s="7"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>61</v>
       </c>
@@ -9535,7 +9535,7 @@
       </c>
       <c r="S34" s="7"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>62</v>
       </c>
@@ -9594,7 +9594,7 @@
       </c>
       <c r="S35" s="7"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>70</v>
       </c>
@@ -9653,7 +9653,7 @@
       </c>
       <c r="S36" s="7"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19">
       <c r="A37">
         <v>70.5</v>
       </c>
@@ -9712,7 +9712,7 @@
       </c>
       <c r="S37" s="7"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19">
       <c r="A38">
         <v>100</v>
       </c>
@@ -9781,21 +9781,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC309567-9A6C-4187-BA34-43941F9E27B4}">
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="O27" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S36" sqref="S36"/>
+      <selection pane="bottomRight" activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="80">
       <c r="A1" s="13" t="s">
         <v>18</v>
       </c>
@@ -9848,7 +9848,7 @@
         <v>189</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S1" s="14" t="s">
         <v>190</v>
@@ -9876,7 +9876,7 @@
       <c r="AF1" s="14"/>
       <c r="AG1" s="14"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="E2" t="s">
         <v>194</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="A3">
         <v>10</v>
       </c>
@@ -9977,7 +9977,7 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33">
       <c r="A4">
         <v>20</v>
       </c>
@@ -10054,7 +10054,7 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33">
       <c r="A5">
         <v>20.5</v>
       </c>
@@ -10137,7 +10137,7 @@
       <c r="AF5" s="6"/>
       <c r="AG5" s="6"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33">
       <c r="A6">
         <v>21</v>
       </c>
@@ -10193,17 +10193,16 @@
         <v>2000</v>
       </c>
       <c r="T6">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="U6">
-        <f>2.5%*S6*1000</f>
-        <v>50000</v>
+        <v>40500</v>
       </c>
       <c r="V6">
         <v>40</v>
       </c>
-      <c r="W6">
-        <v>6</v>
+      <c r="W6" t="s">
+        <v>258</v>
       </c>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
@@ -10215,7 +10214,7 @@
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="16">
       <c r="A7">
         <v>21.5</v>
       </c>
@@ -10278,17 +10277,16 @@
         <v>2105</v>
       </c>
       <c r="T7">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="U7">
-        <f>2.5%*S7*1000</f>
-        <v>52625</v>
+        <v>40500</v>
       </c>
       <c r="V7" s="29">
         <v>40</v>
       </c>
       <c r="W7" t="s">
-        <v>204</v>
+        <v>258</v>
       </c>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
@@ -10300,7 +10298,7 @@
       <c r="AF7" s="6"/>
       <c r="AG7" s="6"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33">
       <c r="A8">
         <v>30</v>
       </c>
@@ -10365,7 +10363,7 @@
         <v>40</v>
       </c>
       <c r="W8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
@@ -10377,7 +10375,7 @@
       <c r="AF8" s="6"/>
       <c r="AG8" s="6"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33">
       <c r="A9">
         <v>30.5</v>
       </c>
@@ -10449,7 +10447,7 @@
         <v>40</v>
       </c>
       <c r="W9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
@@ -10461,7 +10459,7 @@
       <c r="AF9" s="6"/>
       <c r="AG9" s="6"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="A10">
         <v>31</v>
       </c>
@@ -10526,7 +10524,7 @@
         <v>40</v>
       </c>
       <c r="W10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
@@ -10538,7 +10536,7 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33">
       <c r="A11">
         <v>31.5</v>
       </c>
@@ -10610,7 +10608,7 @@
         <v>40</v>
       </c>
       <c r="W11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
@@ -10622,7 +10620,7 @@
       <c r="AF11" s="6"/>
       <c r="AG11" s="6"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33">
       <c r="A12">
         <v>32</v>
       </c>
@@ -10687,7 +10685,7 @@
         <v>40</v>
       </c>
       <c r="W12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
@@ -10699,7 +10697,7 @@
       <c r="AF12" s="6"/>
       <c r="AG12" s="6"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33">
       <c r="A13">
         <v>32.5</v>
       </c>
@@ -10783,7 +10781,7 @@
       <c r="AF13" s="6"/>
       <c r="AG13" s="6"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33">
       <c r="A14">
         <v>33</v>
       </c>
@@ -10861,7 +10859,7 @@
       <c r="AF14" s="6"/>
       <c r="AG14" s="6"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33">
       <c r="A15">
         <v>40</v>
       </c>
@@ -10935,7 +10933,7 @@
       <c r="AF15" s="6"/>
       <c r="AG15" s="6"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33">
       <c r="A16">
         <v>40.5</v>
       </c>
@@ -10988,7 +10986,7 @@
         <v>0.8</v>
       </c>
       <c r="Q16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="S16">
         <v>400</v>
@@ -11015,12 +11013,12 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33">
       <c r="A17">
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C17" t="s">
         <v>94</v>
@@ -11092,12 +11090,12 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33">
       <c r="A18">
         <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C18" t="s">
         <v>96</v>
@@ -11175,7 +11173,7 @@
       <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33">
       <c r="A19">
         <v>43</v>
       </c>
@@ -11240,7 +11238,7 @@
         <v>30</v>
       </c>
       <c r="W19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
@@ -11252,7 +11250,7 @@
       <c r="AF19" s="6"/>
       <c r="AG19" s="6"/>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33">
       <c r="A20">
         <v>43.5</v>
       </c>
@@ -11324,7 +11322,7 @@
         <v>30</v>
       </c>
       <c r="W20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
@@ -11336,7 +11334,7 @@
       <c r="AF20" s="6"/>
       <c r="AG20" s="6"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33">
       <c r="A21">
         <v>44</v>
       </c>
@@ -11417,7 +11415,7 @@
       <c r="AF21" s="6"/>
       <c r="AG21" s="6"/>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33">
       <c r="A22">
         <v>44.5</v>
       </c>
@@ -11500,7 +11498,7 @@
       <c r="AF22" s="6"/>
       <c r="AG22" s="6"/>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33">
       <c r="A23">
         <v>45</v>
       </c>
@@ -11578,7 +11576,7 @@
       <c r="AF23" s="6"/>
       <c r="AG23" s="6"/>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33">
       <c r="A24">
         <v>45.5</v>
       </c>
@@ -11661,12 +11659,12 @@
       <c r="AF24" s="6"/>
       <c r="AG24" s="6"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33">
       <c r="A25">
         <v>49.5</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C25" t="s">
         <v>104</v>
@@ -11738,7 +11736,7 @@
       <c r="AF25" s="6"/>
       <c r="AG25" s="6"/>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33">
       <c r="A26">
         <v>50</v>
       </c>
@@ -11812,7 +11810,7 @@
       <c r="AF26" s="6"/>
       <c r="AG26" s="6"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33">
       <c r="A27">
         <v>50.5</v>
       </c>
@@ -11865,7 +11863,7 @@
         <v>0.8</v>
       </c>
       <c r="Q27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="S27">
         <v>400</v>
@@ -11892,12 +11890,12 @@
       <c r="AF27" s="6"/>
       <c r="AG27" s="6"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33">
       <c r="A28">
         <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C28" t="s">
         <v>107</v>
@@ -11969,7 +11967,7 @@
       <c r="AF28" s="6"/>
       <c r="AG28" s="6"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33">
       <c r="A29">
         <v>52</v>
       </c>
@@ -12043,7 +12041,7 @@
       <c r="AF29" s="6"/>
       <c r="AG29" s="6"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33">
       <c r="A30">
         <v>52.5</v>
       </c>
@@ -12096,7 +12094,7 @@
         <v>0.8</v>
       </c>
       <c r="Q30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="S30">
         <f>ROUND(S29/0.95,0)</f>
@@ -12112,7 +12110,7 @@
         <v>25</v>
       </c>
       <c r="W30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
@@ -12124,7 +12122,7 @@
       <c r="AF30" s="6"/>
       <c r="AG30" s="6"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33">
       <c r="A31">
         <v>60</v>
       </c>
@@ -12180,7 +12178,7 @@
         <v>60</v>
       </c>
       <c r="W31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
@@ -12192,12 +12190,12 @@
       <c r="AF31" s="6"/>
       <c r="AG31" s="6"/>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33">
       <c r="A32">
         <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C32" t="s">
         <v>112</v>
@@ -12248,7 +12246,7 @@
         <v>60</v>
       </c>
       <c r="W32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
@@ -12260,7 +12258,7 @@
       <c r="AF32" s="6"/>
       <c r="AG32" s="6"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33">
       <c r="A33">
         <v>63</v>
       </c>
@@ -12316,7 +12314,7 @@
         <v>60</v>
       </c>
       <c r="W33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
@@ -12328,7 +12326,7 @@
       <c r="AF33" s="6"/>
       <c r="AG33" s="6"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33">
       <c r="A34">
         <v>70</v>
       </c>
@@ -12406,7 +12404,7 @@
       <c r="AF34" s="6"/>
       <c r="AG34" s="6"/>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33">
       <c r="A35">
         <v>70.5</v>
       </c>
@@ -12486,12 +12484,12 @@
       <c r="AF35" s="6"/>
       <c r="AG35" s="6"/>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33">
       <c r="A36">
         <v>100</v>
       </c>
       <c r="B36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C36" t="s">
         <v>116</v>
@@ -12563,15 +12561,15 @@
       <c r="AF36" s="6"/>
       <c r="AG36" s="6"/>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33">
       <c r="A37">
         <v>101</v>
       </c>
       <c r="B37" t="s">
+        <v>211</v>
+      </c>
+      <c r="C37" t="s">
         <v>212</v>
-      </c>
-      <c r="C37" t="s">
-        <v>213</v>
       </c>
       <c r="D37">
         <v>2020</v>
@@ -12640,15 +12638,15 @@
       <c r="AF37" s="6"/>
       <c r="AG37" s="6"/>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33">
       <c r="A38">
         <v>102</v>
       </c>
       <c r="B38" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" t="s">
         <v>214</v>
-      </c>
-      <c r="C38" t="s">
-        <v>215</v>
       </c>
       <c r="D38">
         <v>2020</v>
@@ -12728,13 +12726,13 @@
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="16">
       <c r="A1" s="13" t="s">
         <v>18</v>
       </c>
@@ -12751,7 +12749,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="3">
         <v>20.5</v>
       </c>
@@ -12770,7 +12768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <v>20.5</v>
       </c>
@@ -12790,7 +12788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <v>20.5</v>
       </c>
@@ -12810,7 +12808,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <v>20.5</v>
       </c>
@@ -12827,7 +12825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="3">
         <v>21.5</v>
       </c>
@@ -12846,7 +12844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <v>21.5</v>
       </c>
@@ -12866,7 +12864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <v>21.5</v>
       </c>
@@ -12886,7 +12884,7 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <v>21.5</v>
       </c>
@@ -12903,7 +12901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <v>30.5</v>
       </c>
@@ -12922,7 +12920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>30.5</v>
       </c>
@@ -12942,7 +12940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="3">
         <v>30.5</v>
       </c>
@@ -12962,7 +12960,7 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <v>30.5</v>
       </c>
@@ -12979,7 +12977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <v>31.5</v>
       </c>
@@ -12998,7 +12996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <v>31.5</v>
       </c>
@@ -13018,7 +13016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="3">
         <v>31.5</v>
       </c>
@@ -13038,7 +13036,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="3">
         <v>31.5</v>
       </c>
@@ -13055,7 +13053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="3">
         <v>32.5</v>
       </c>
@@ -13074,7 +13072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="3">
         <v>32.5</v>
       </c>
@@ -13094,7 +13092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="3">
         <v>32.5</v>
       </c>
@@ -13114,7 +13112,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="3">
         <v>32.5</v>
       </c>
@@ -13131,7 +13129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="3">
         <v>40.5</v>
       </c>
@@ -13150,7 +13148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="3">
         <v>40.5</v>
       </c>
@@ -13170,7 +13168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="3">
         <v>40.5</v>
       </c>
@@ -13190,7 +13188,7 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="3">
         <v>40.5</v>
       </c>
@@ -13207,7 +13205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="3">
         <v>43.5</v>
       </c>
@@ -13226,7 +13224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="3">
         <v>43.5</v>
       </c>
@@ -13246,7 +13244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="3">
         <v>43.5</v>
       </c>
@@ -13266,7 +13264,7 @@
         <v>0.80000000000000016</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="3">
         <v>43.5</v>
       </c>
@@ -13283,7 +13281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="3">
         <v>44.5</v>
       </c>
@@ -13302,7 +13300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="3">
         <v>44.5</v>
       </c>
@@ -13322,7 +13320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="3">
         <v>44.5</v>
       </c>
@@ -13342,7 +13340,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="3">
         <v>44.5</v>
       </c>
@@ -13359,7 +13357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="3">
         <v>45.5</v>
       </c>
@@ -13378,7 +13376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="3">
         <v>45.5</v>
       </c>
@@ -13398,7 +13396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="3">
         <v>45.5</v>
       </c>
@@ -13418,7 +13416,7 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="3">
         <v>45.5</v>
       </c>
@@ -13435,7 +13433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="3">
         <v>50.5</v>
       </c>
@@ -13454,7 +13452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="3">
         <v>50.5</v>
       </c>
@@ -13474,7 +13472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="3">
         <v>50.5</v>
       </c>
@@ -13494,7 +13492,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="3">
         <v>50.5</v>
       </c>
@@ -13511,7 +13509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="3">
         <v>52.5</v>
       </c>
@@ -13530,7 +13528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="3">
         <v>52.5</v>
       </c>
@@ -13550,7 +13548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="3">
         <v>52.5</v>
       </c>
@@ -13570,7 +13568,7 @@
         <v>0.80000000000000016</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="3">
         <v>52.5</v>
       </c>
@@ -13587,7 +13585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="3">
         <v>70.5</v>
       </c>
@@ -13606,7 +13604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="3">
         <v>70.5</v>
       </c>
@@ -13626,7 +13624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="3">
         <v>70.5</v>
       </c>
@@ -13646,7 +13644,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="3">
         <v>70.5</v>
       </c>

</xml_diff>

<commit_message>
updated asparagus demand assumption;
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D6A6C7-FDD2-4011-9F16-8266461645C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846E2146-1BD2-4BEC-97E8-867C68C919BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="860" activeTab="13" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="860" firstSheet="6" activeTab="14" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="ATC" sheetId="3" r:id="rId12"/>
     <sheet name="KM" sheetId="4" r:id="rId13"/>
     <sheet name="potentials" sheetId="19" r:id="rId14"/>
+    <sheet name="AIR_POLLUTION" sheetId="20" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -639,8 +640,43 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sebastian</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2C3BF732-EB70-4318-A3DC-57E3173C0EC6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lifecycle air pollution cost of state-of-the-art (in around 2009) electricity generation technologies in € of 2015. 
+Total of health impacts, crop yield losses, and material damage.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="259">
   <si>
     <t>year</t>
   </si>
@@ -1089,9 +1125,6 @@
     <t>total installed cost</t>
   </si>
   <si>
-    <t>annuity of total installed cost</t>
-  </si>
-  <si>
     <t>zone</t>
   </si>
   <si>
@@ -1315,22 +1348,129 @@
   </si>
   <si>
     <t>1, 8</t>
+  </si>
+  <si>
+    <t>equivalent annual cost</t>
+  </si>
+  <si>
+    <t>Sascha Samadi</t>
+  </si>
+  <si>
+    <t>The Social Costs of Electricity Generation - Categorizing Different Types of Costs and Evaluating Their Respective Relevance</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/1996-1073/10/3/356</t>
+  </si>
+  <si>
+    <t>NEEDS Project</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D7.2%20Final%20report%20on%20advanced%20fossil%20power%20plants.pdf</t>
+  </si>
+  <si>
+    <t>Final report on technical data, costs, and life cycle inventories of advanced fossil power generation systems</t>
+  </si>
+  <si>
+    <t>Final report on technical data, costs and life cycle inventories of biomass CHP plants</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D13.2%20Final%20report%20on%20Biomass%20technologies.pdf</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D11.2%20Final%20report%20on%20PV%20technology.pdf</t>
+  </si>
+  <si>
+    <t>Table 16, page 51</t>
+  </si>
+  <si>
+    <t>Final report on technical data, costs and life cycle inventories of PV applications</t>
+  </si>
+  <si>
+    <t>http://www.needs-project.org/2009/Deliverables/RS1a%20D10.2.pdf</t>
+  </si>
+  <si>
+    <t>Table 5.3, page 39</t>
+  </si>
+  <si>
+    <t>Final report on offshore wind technology</t>
+  </si>
+  <si>
+    <t>Table 7, page 16</t>
+  </si>
+  <si>
+    <t>10, 11</t>
+  </si>
+  <si>
+    <t>10, 14</t>
+  </si>
+  <si>
+    <t>10, 13</t>
+  </si>
+  <si>
+    <t>10, 12</t>
+  </si>
+  <si>
+    <t>10, 8</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>fixed cost</t>
+  </si>
+  <si>
+    <t>wind offshore in soure; 4044 full-load hours</t>
+  </si>
+  <si>
+    <t>utility scale pv, 838 full-load hours</t>
+  </si>
+  <si>
+    <t>avg of lignite and nat gas due to lack of data</t>
+  </si>
+  <si>
+    <t>no data available</t>
+  </si>
+  <si>
+    <t>Syngas</t>
+  </si>
+  <si>
+    <t>43.2% net efficiency</t>
+  </si>
+  <si>
+    <t>45.0% net efficiency</t>
+  </si>
+  <si>
+    <t>57.5% net efficiency</t>
+  </si>
+  <si>
+    <t>20.0% net efficiency</t>
+  </si>
+  <si>
+    <t>34.0% net efficiency</t>
+  </si>
+  <si>
+    <t>variable cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="170" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="169" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1387,6 +1527,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1416,7 +1569,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1449,8 +1602,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1460,9 +1613,11 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1779,10 +1934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3387BF03-EDC5-4C83-AB6F-3B95A2E59024}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,22 +1949,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,16 +1972,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2">
         <v>2016</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,16 +1989,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1851,16 +2006,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4">
         <v>2013</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,16 +2023,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5">
         <v>2014</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,16 +2040,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,16 +2057,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7">
         <v>2014</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1919,16 +2074,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1936,16 +2091,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1953,16 +2108,115 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C10">
         <v>2017</v>
       </c>
       <c r="D10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>220</v>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C11">
+        <v>2017</v>
+      </c>
+      <c r="D11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12">
+        <v>2007</v>
+      </c>
+      <c r="D12" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13">
+        <v>2008</v>
+      </c>
+      <c r="D13" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14">
+        <v>2008</v>
+      </c>
+      <c r="D14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15">
+        <v>2008</v>
+      </c>
+      <c r="D15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="F15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1974,6 +2228,9 @@
     <hyperlink ref="E7" r:id="rId5" xr:uid="{D9995BB9-537F-4F22-BB62-7F47B6A20D25}"/>
     <hyperlink ref="E3" r:id="rId6" xr:uid="{B3ADECFE-DF4D-4251-89D4-973E831A4DC5}"/>
     <hyperlink ref="E10" r:id="rId7" xr:uid="{FE90C9A5-8CAA-4399-9D7F-A79798808E4E}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{FA159502-D871-48B6-BF13-936603692024}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{E9DA7171-DCDC-459E-9319-AD7D4C4C193D}"/>
+    <hyperlink ref="E15" r:id="rId10" xr:uid="{A12914E5-AF85-4EA9-814D-4FC82B75214B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4367,7 +4624,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
@@ -5273,7 +5530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E1761F-2504-4C8D-8040-F9E9B5E3E6FE}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -5410,6 +5667,248 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE718DA-91F3-45FB-AD2F-2A0676B90C2D}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0.27</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4">
+        <v>6.12</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5">
+        <v>2.36</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <f>(B5+B3)/2</f>
+        <v>3.21</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>4.04</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>5028</v>
+      </c>
+      <c r="D9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>2831</v>
+      </c>
+      <c r="D10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5418,8 +5917,8 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37:C38"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6066,7 +6565,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>63</v>
@@ -6095,20 +6594,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A9BE73-D660-402D-8ABC-7BC4E42D221F}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -6134,7 +6633,7 @@
         <v>2012</v>
       </c>
       <c r="C2">
-        <v>0.36299999999999999</v>
+        <v>0.36288500000000001</v>
       </c>
       <c r="D2">
         <v>5.5190000000000001</v>
@@ -6154,7 +6653,7 @@
         <v>2013</v>
       </c>
       <c r="C3">
-        <v>0.621</v>
+        <v>0.62597400000000003</v>
       </c>
       <c r="D3">
         <v>5.5730000000000004</v>
@@ -6174,7 +6673,7 @@
         <v>2014</v>
       </c>
       <c r="C4">
-        <v>0.78</v>
+        <v>0.785246</v>
       </c>
       <c r="D4">
         <v>5.6150000000000002</v>
@@ -6194,7 +6693,7 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0.93700000000000006</v>
+        <v>0.93709799999999999</v>
       </c>
       <c r="D5">
         <v>5.6559999999999997</v>
@@ -6214,7 +6713,7 @@
         <v>2016</v>
       </c>
       <c r="C6">
-        <v>1.0960000000000001</v>
+        <v>1.0960160000000001</v>
       </c>
       <c r="D6">
         <v>5.7</v>
@@ -6234,7 +6733,7 @@
         <v>2017</v>
       </c>
       <c r="C7">
-        <v>1.2689999999999999</v>
+        <v>1.2689710000000001</v>
       </c>
       <c r="D7">
         <v>5.7140000000000004</v>
@@ -6254,7 +6753,10 @@
         <v>2018</v>
       </c>
       <c r="C8">
-        <v>1.4</v>
+        <v>1.4376409999999999</v>
+      </c>
+      <c r="D8">
+        <v>5.7220000000000004</v>
       </c>
       <c r="E8">
         <v>3.0449999999999999</v>
@@ -6265,42 +6767,24 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>2012</v>
-      </c>
-      <c r="C9">
-        <v>34.076999999999998</v>
-      </c>
-      <c r="D9">
-        <v>4.5179999999999998</v>
-      </c>
-      <c r="E9">
-        <v>30.710999999999999</v>
+        <v>2019</v>
       </c>
       <c r="F9">
-        <v>0.26800000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>2013</v>
-      </c>
-      <c r="C10">
-        <v>36.71</v>
-      </c>
-      <c r="D10">
-        <v>4.5009999999999994</v>
-      </c>
-      <c r="E10">
-        <v>32.969000000000001</v>
+        <v>2020</v>
       </c>
       <c r="F10">
-        <v>0.50800000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -6308,19 +6792,19 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C11">
-        <v>37.9</v>
+        <v>34.076999999999998</v>
       </c>
       <c r="D11">
-        <v>4.4909999999999997</v>
+        <v>4.5179999999999998</v>
       </c>
       <c r="E11">
-        <v>37.619999999999997</v>
+        <v>30.710999999999999</v>
       </c>
       <c r="F11">
-        <v>0.99399999999999999</v>
+        <v>0.26800000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -6328,19 +6812,19 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="C12">
-        <v>39.223999999999997</v>
+        <v>36.71</v>
       </c>
       <c r="D12">
-        <v>4.5</v>
+        <v>4.5009999999999994</v>
       </c>
       <c r="E12">
-        <v>41.296999999999997</v>
+        <v>32.969000000000001</v>
       </c>
       <c r="F12">
-        <v>3.2829999999999999</v>
+        <v>0.50800000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -6348,19 +6832,19 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="C13">
-        <v>40.679000000000002</v>
+        <v>37.9</v>
       </c>
       <c r="D13">
-        <v>4.5</v>
+        <v>4.4909999999999997</v>
       </c>
       <c r="E13">
-        <v>45.283000000000001</v>
+        <v>37.619999999999997</v>
       </c>
       <c r="F13">
-        <v>4.1520000000000001</v>
+        <v>0.99399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -6368,19 +6852,19 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="C14">
-        <v>42.338999999999999</v>
+        <v>39.223999999999997</v>
       </c>
       <c r="D14">
         <v>4.5</v>
       </c>
       <c r="E14">
-        <v>50.290999999999997</v>
+        <v>41.296999999999997</v>
       </c>
       <c r="F14">
-        <v>5.4269999999999996</v>
+        <v>3.2829999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -6388,19 +6872,75 @@
         <v>2</v>
       </c>
       <c r="B15">
+        <v>2016</v>
+      </c>
+      <c r="C15">
+        <v>40.679000000000002</v>
+      </c>
+      <c r="D15">
+        <v>4.5</v>
+      </c>
+      <c r="E15">
+        <v>45.283000000000001</v>
+      </c>
+      <c r="F15">
+        <v>4.1520000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2017</v>
+      </c>
+      <c r="C16">
+        <v>42.338999999999999</v>
+      </c>
+      <c r="D16">
+        <v>4.5</v>
+      </c>
+      <c r="E16">
+        <v>50.290999999999997</v>
+      </c>
+      <c r="F16">
+        <v>5.4269999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
         <v>2018</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>45.277000000000001</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>4.5069999999999997</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>52.564999999999998</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>6.4169999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -6416,14 +6956,17 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>147</v>
@@ -6441,7 +6984,7 @@
         <v>146</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>149</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6452,7 +6995,6 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <f>C6</f>
         <v>40</v>
       </c>
       <c r="D2" s="20">
@@ -6468,10 +7010,11 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
-        <f>ROUND($D2*(WACC!$B$2*(1+WACC!$B$2)^$C2)/((1+WACC!$B$2)^$C2-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C2)/((1+WACC!$B$2)^$C2-1)*$D2,0)</f>
         <v>36715</v>
       </c>
-      <c r="I2" s="25"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -6497,7 +7040,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <f>ROUND($D3*(WACC!$B$2*(1+WACC!$B$2)^$C3)/((1+WACC!$B$2)^$C3-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C3)/((1+WACC!$B$2)^$C3-1)*$D3,0)</f>
         <v>153375</v>
       </c>
       <c r="I3" s="25"/>
@@ -6526,7 +7069,7 @@
         <v>1.35</v>
       </c>
       <c r="G4" s="1">
-        <f>ROUND($D4*(WACC!$B$2*(1+WACC!$B$2)^$C4)/((1+WACC!$B$2)^$C4-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C4)/((1+WACC!$B$2)^$C4-1)*$D4,0)</f>
         <v>67653</v>
       </c>
       <c r="I4" s="25"/>
@@ -6555,7 +7098,7 @@
         <v>2.7</v>
       </c>
       <c r="G5" s="1">
-        <f>ROUND($D5*(WACC!$B$2*(1+WACC!$B$2)^$C5)/((1+WACC!$B$2)^$C5-1),0)</f>
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$C5)/((1+WACC!$B$2)^$C5-1)*$D5,0)</f>
         <v>125549</v>
       </c>
       <c r="I5" s="25"/>
@@ -6580,7 +7123,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <f>ROUND($D6*(WACC!$B$3*(1+WACC!$B$3)^$C6)/((1+WACC!$B$3)^$C6-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C6)/((1+WACC!$B$3)^$C6-1)*$D6,0)</f>
         <v>27255</v>
       </c>
       <c r="I6" s="25"/>
@@ -6605,7 +7148,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f>ROUND($D7*(WACC!$B$3*(1+WACC!$B$3)^$C7)/((1+WACC!$B$3)^$C7-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C7)/((1+WACC!$B$3)^$C7-1)*$D7,0)</f>
         <v>108823</v>
       </c>
       <c r="I7" s="25"/>
@@ -6630,7 +7173,7 @@
         <v>1.35</v>
       </c>
       <c r="G8" s="1">
-        <f>ROUND($D8*(WACC!$B$3*(1+WACC!$B$3)^$C8)/((1+WACC!$B$3)^$C8-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C8)/((1+WACC!$B$3)^$C8-1)*$D8,0)</f>
         <v>53060</v>
       </c>
       <c r="I8" s="25"/>
@@ -6655,7 +7198,7 @@
         <v>2.7</v>
       </c>
       <c r="G9" s="1">
-        <f>ROUND($D9*(WACC!$B$3*(1+WACC!$B$3)^$C9)/((1+WACC!$B$3)^$C9-1),0)</f>
+        <f>ROUND((WACC!$B$3*(1+WACC!$B$3)^$C9)/((1+WACC!$B$3)^$C9-1)*$D9,0)</f>
         <v>98467</v>
       </c>
       <c r="I9" s="25"/>
@@ -6684,7 +7227,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>147</v>
@@ -9239,7 +9782,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="O27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="S36" sqref="S36"/>
@@ -9263,64 +9806,64 @@
         <v>65</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="S1" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="R1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="S1" s="14" t="s">
+      <c r="T1" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="V1" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="V1" s="14" t="s">
-        <v>194</v>
-      </c>
       <c r="W1" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X1" s="14"/>
       <c r="Y1" s="14"/>
@@ -9335,28 +9878,28 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2" t="s">
         <v>195</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>196</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>197</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>198</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>199</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>200</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>201</v>
-      </c>
-      <c r="L2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -9376,31 +9919,31 @@
         <v>0.34</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -9454,31 +9997,31 @@
         <v>0.35199999999999998</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -9567,7 +10110,7 @@
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S5">
         <v>1700</v>
@@ -9614,31 +10157,31 @@
         <v>0.439</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -9728,7 +10271,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S7">
         <f>ROUND(S6/0.95,0)</f>
@@ -9745,7 +10288,7 @@
         <v>40</v>
       </c>
       <c r="W7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
@@ -9777,31 +10320,31 @@
         <v>0.375</v>
       </c>
       <c r="G8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -9822,7 +10365,7 @@
         <v>40</v>
       </c>
       <c r="W8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
@@ -9890,7 +10433,7 @@
         <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S9">
         <f>ROUND(S8/0.95,0)</f>
@@ -9906,7 +10449,7 @@
         <v>40</v>
       </c>
       <c r="W9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
@@ -9938,31 +10481,31 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="G10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -9983,7 +10526,7 @@
         <v>40</v>
       </c>
       <c r="W10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
@@ -10051,7 +10594,7 @@
         <v>1</v>
       </c>
       <c r="Q11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S11">
         <f>ROUND(S10/0.95,0)</f>
@@ -10067,7 +10610,7 @@
         <v>40</v>
       </c>
       <c r="W11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
@@ -10099,31 +10642,31 @@
         <v>0.48499999999999999</v>
       </c>
       <c r="G12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P12">
         <v>1</v>
@@ -10144,7 +10687,7 @@
         <v>40</v>
       </c>
       <c r="W12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
@@ -10260,31 +10803,31 @@
         <v>0.46</v>
       </c>
       <c r="G14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -10338,31 +10881,31 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="G15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q15">
         <v>4</v>
@@ -10445,7 +10988,7 @@
         <v>0.8</v>
       </c>
       <c r="Q16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S16">
         <v>400</v>
@@ -10477,7 +11020,7 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C17" t="s">
         <v>94</v>
@@ -10492,31 +11035,31 @@
         <v>0.32800000000000001</v>
       </c>
       <c r="G17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -10554,7 +11097,7 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
         <v>96</v>
@@ -10652,31 +11195,31 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -10697,7 +11240,7 @@
         <v>30</v>
       </c>
       <c r="W19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
@@ -10781,7 +11324,7 @@
         <v>30</v>
       </c>
       <c r="W20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
@@ -10813,31 +11356,31 @@
         <v>0.61</v>
       </c>
       <c r="G21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P21">
         <v>1</v>
@@ -10977,31 +11520,31 @@
         <v>0.47</v>
       </c>
       <c r="G23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q23">
         <v>1</v>
@@ -11123,7 +11666,7 @@
         <v>49.5</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25" t="s">
         <v>104</v>
@@ -11138,31 +11681,31 @@
         <v>0.95</v>
       </c>
       <c r="G25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P25">
         <v>1</v>
@@ -11215,31 +11758,31 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="G26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q26">
         <v>4</v>
@@ -11322,7 +11865,7 @@
         <v>0.8</v>
       </c>
       <c r="Q27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S27">
         <v>400</v>
@@ -11354,7 +11897,7 @@
         <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C28" t="s">
         <v>107</v>
@@ -11369,31 +11912,31 @@
         <v>0.41</v>
       </c>
       <c r="G28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P28">
         <v>1</v>
@@ -11446,31 +11989,31 @@
         <v>0.47</v>
       </c>
       <c r="G29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q29">
         <v>4</v>
@@ -11553,7 +12096,7 @@
         <v>0.8</v>
       </c>
       <c r="Q30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="S30">
         <f>ROUND(S29/0.95,0)</f>
@@ -11569,7 +12112,7 @@
         <v>25</v>
       </c>
       <c r="W30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
@@ -11595,34 +12138,34 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S31">
         <v>3000</v>
@@ -11637,7 +12180,7 @@
         <v>60</v>
       </c>
       <c r="W31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
@@ -11654,7 +12197,7 @@
         <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C32" t="s">
         <v>112</v>
@@ -11663,34 +12206,34 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S32">
         <v>2000</v>
@@ -11705,7 +12248,7 @@
         <v>60</v>
       </c>
       <c r="W32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
@@ -11731,34 +12274,34 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S33">
         <v>2000</v>
@@ -11773,7 +12316,7 @@
         <v>60</v>
       </c>
       <c r="W33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
@@ -11805,31 +12348,31 @@
         <v>0.29599999999999999</v>
       </c>
       <c r="G34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q34">
         <v>1</v>
@@ -11948,7 +12491,7 @@
         <v>100</v>
       </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C36" t="s">
         <v>116</v>
@@ -11963,31 +12506,31 @@
         <v>3.6</v>
       </c>
       <c r="G36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P36">
         <v>1</v>
@@ -12025,10 +12568,10 @@
         <v>101</v>
       </c>
       <c r="B37" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" t="s">
         <v>213</v>
-      </c>
-      <c r="C37" t="s">
-        <v>214</v>
       </c>
       <c r="D37">
         <v>2020</v>
@@ -12040,31 +12583,31 @@
         <v>1.71</v>
       </c>
       <c r="G37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M37" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P37">
         <v>1</v>
@@ -12102,10 +12645,10 @@
         <v>102</v>
       </c>
       <c r="B38" t="s">
+        <v>214</v>
+      </c>
+      <c r="C38" t="s">
         <v>215</v>
-      </c>
-      <c r="C38" t="s">
-        <v>216</v>
       </c>
       <c r="D38">
         <v>2020</v>
@@ -12117,31 +12660,31 @@
         <v>0.99</v>
       </c>
       <c r="G38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P38">
         <v>1</v>

</xml_diff>

<commit_message>
fixes and improvements in project asparagus
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846E2146-1BD2-4BEC-97E8-867C68C919BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4A2B9E-FF56-4D03-9D5A-43C1D8F2DE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="860" firstSheet="6" activeTab="14" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="860" firstSheet="6" activeTab="11" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -4745,11 +4745,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4160F9D6-85F4-409B-B165-F3480400FC38}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4810,7 +4810,7 @@
         <v>700</v>
       </c>
       <c r="F2">
-        <v>4500</v>
+        <v>4900</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -4904,7 +4904,7 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>4500</v>
+        <v>4900</v>
       </c>
       <c r="E6">
         <v>1750</v>
@@ -5674,7 +5674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE718DA-91F3-45FB-AD2F-2A0676B90C2D}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
continued to rewrite data export to gdx
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seb/git_repos/medea/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD771F90-2FDA-7A4F-849B-AA8557F69D4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED005999-E05C-F94C-928C-FADCD4358D12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="1520" windowWidth="22540" windowHeight="14300" tabRatio="860" activeTab="2" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="860" activeTab="3" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -22,14 +22,16 @@
     <sheet name="ATC" sheetId="3" r:id="rId7"/>
     <sheet name="KM" sheetId="4" r:id="rId8"/>
     <sheet name="COST_TRANSPORT" sheetId="11" r:id="rId9"/>
-    <sheet name="WACC" sheetId="7" r:id="rId10"/>
-    <sheet name="INITIAL_CAP_R" sheetId="2" r:id="rId11"/>
-    <sheet name="CAPITALCOST_R" sheetId="8" r:id="rId12"/>
-    <sheet name="CAPITALCOST_S" sheetId="10" r:id="rId13"/>
-    <sheet name="parameters_G" sheetId="9" r:id="rId14"/>
-    <sheet name="tech_full" sheetId="17" r:id="rId15"/>
-    <sheet name="FEASIBLE_INPUT-OUTPUT_BAK" sheetId="6" r:id="rId16"/>
-    <sheet name="potentials" sheetId="19" r:id="rId17"/>
+    <sheet name="ESTIMATES" sheetId="23" r:id="rId10"/>
+    <sheet name="CO2_INTENSITY" sheetId="24" r:id="rId11"/>
+    <sheet name="WACC" sheetId="7" r:id="rId12"/>
+    <sheet name="INITIAL_CAP_R" sheetId="2" r:id="rId13"/>
+    <sheet name="CAPITALCOST_R" sheetId="8" r:id="rId14"/>
+    <sheet name="CAPITALCOST_S" sheetId="10" r:id="rId15"/>
+    <sheet name="parameters_G" sheetId="9" r:id="rId16"/>
+    <sheet name="tech_full" sheetId="17" r:id="rId17"/>
+    <sheet name="FEASIBLE_INPUT-OUTPUT_BAK" sheetId="6" r:id="rId18"/>
+    <sheet name="potentials" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -120,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA10" authorId="0" shapeId="0" xr:uid="{2BF3154B-BA64-E342-BA77-8DD512F08E6D}">
+    <comment ref="AC10" authorId="0" shapeId="0" xr:uid="{2BF3154B-BA64-E342-BA77-8DD512F08E6D}">
       <text>
         <r>
           <rPr>
@@ -913,7 +915,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="345">
   <si>
     <t>year</t>
   </si>
@@ -1891,6 +1893,64 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>LAMBDA</t>
+  </si>
+  <si>
+    <t>SIGMA</t>
+  </si>
+  <si>
+    <t>VALUE_NSE</t>
+  </si>
+  <si>
+    <t>CO2_intensity</t>
+  </si>
+  <si>
+    <t>Transmission grid expansion</t>
+  </si>
+  <si>
+    <t>transmission</t>
+  </si>
+  <si>
+    <t>Hagspiel et al.</t>
+  </si>
+  <si>
+    <t>Cost-optimal power system extension under flow-based market coupling. Energy 66, 654-666</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.
+energy.2014.01.025</t>
+  </si>
+  <si>
+    <t>Brown et al.</t>
+  </si>
+  <si>
+    <t>Synergies of sector coupling and transmission reinforcement in a cost-optimised, highly renewable European energy system. Energy 160, 720-739</t>
+  </si>
+  <si>
+    <t>https: //doi.org/10.1016/j.energy.2018.06.222</t>
+  </si>
+  <si>
+    <t>16, 17</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
+    <t>Conventional generation</t>
+  </si>
+  <si>
+    <t>conventional</t>
+  </si>
+  <si>
+    <t>Nat Gas - Old OCGT CoGen</t>
+  </si>
+  <si>
+    <t>Nat Gas - New OCGT CoGen</t>
+  </si>
+  <si>
+    <t>Oil - OCGT CoGen</t>
   </si>
 </sst>
 </file>
@@ -2011,7 +2071,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2048,6 +2108,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2063,7 +2129,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2134,6 +2200,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -2450,10 +2518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3387BF03-EDC5-4C83-AB6F-3B95A2E59024}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2744,6 +2812,40 @@
         <v>259</v>
       </c>
     </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>332</v>
+      </c>
+      <c r="C17">
+        <v>2014</v>
+      </c>
+      <c r="D17" t="s">
+        <v>333</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>335</v>
+      </c>
+      <c r="C18">
+        <v>2018</v>
+      </c>
+      <c r="D18" t="s">
+        <v>336</v>
+      </c>
+      <c r="E18" t="s">
+        <v>337</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{646F59EA-8517-4A9D-A362-14E775EE0CCE}"/>
@@ -2756,12 +2858,185 @@
     <hyperlink ref="E13" r:id="rId8" xr:uid="{FA159502-D871-48B6-BF13-936603692024}"/>
     <hyperlink ref="E12" r:id="rId9" xr:uid="{E9DA7171-DCDC-459E-9319-AD7D4C4C193D}"/>
     <hyperlink ref="E15" r:id="rId10" xr:uid="{A12914E5-AF85-4EA9-814D-4FC82B75214B}"/>
+    <hyperlink ref="E17" r:id="rId11" xr:uid="{4B4C06FA-2FD6-DC43-A7E2-EBC6BBE17244}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC364A5-0555-C645-8A12-2533612BB966}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2">
+        <v>0.125</v>
+      </c>
+      <c r="C2">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4">
+        <v>12500</v>
+      </c>
+      <c r="C4">
+        <v>12500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758C487E-D7D8-8746-BC28-E4CE13A03946}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4">
+        <v>0.20100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36A1418A-DD29-4863-849D-DF62091CC750}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2803,7 +3078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A9BE73-D660-402D-8ABC-7BC4E42D221F}">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -3159,7 +3434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9B5A1D-EA9B-421F-AC28-39B233C76782}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -3420,7 +3695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F321D5C-F791-46AF-9A23-F1D5D185B926}">
   <dimension ref="A1:O15"/>
   <sheetViews>
@@ -3754,7 +4029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262E26B0-C129-4904-8AA9-F9E48EA6FD9F}">
   <dimension ref="A1:S38"/>
   <sheetViews>
@@ -6012,7 +6287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC309567-9A6C-4187-BA34-43941F9E27B4}">
   <dimension ref="A1:AG38"/>
   <sheetViews>
@@ -8955,7 +9230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CDD314-E06C-4AC0-8DDE-77CC4444BECC}">
   <dimension ref="A1:I137"/>
   <sheetViews>
@@ -11328,7 +11603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E1761F-2504-4C8D-8040-F9E9B5E3E6FE}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -12114,8 +12389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33D813E-78BA-D24A-A7D9-6241E48D080F}">
   <dimension ref="A1:AR58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="E33" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
@@ -17417,11 +17692,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D7635-111A-D442-BE0C-35A2D3A6DC99}">
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:AC53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17430,7 +17705,7 @@
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="15" customFormat="1" ht="80">
+    <row r="1" spans="1:29" s="15" customFormat="1" ht="80">
       <c r="A1" s="15" t="s">
         <v>261</v>
       </c>
@@ -17480,40 +17755,46 @@
         <v>288</v>
       </c>
       <c r="Q1" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="S1" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="15" customFormat="1" ht="16">
+    <row r="2" spans="1:29" s="15" customFormat="1" ht="16">
       <c r="E2" s="15" t="s">
         <v>278</v>
       </c>
@@ -17547,8 +17828,14 @@
       <c r="P2" s="15" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="3" spans="1:27">
+      <c r="Q2" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>292</v>
       </c>
@@ -17598,40 +17885,46 @@
         <v>306</v>
       </c>
       <c r="Q3" t="s">
+        <v>331</v>
+      </c>
+      <c r="R3" t="s">
+        <v>341</v>
+      </c>
+      <c r="S3" t="s">
         <v>194</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>196</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>197</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>198</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>199</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>200</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>201</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>303</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>304</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>305</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>0</v>
       </c>
@@ -17680,13 +17973,14 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f>1-SUM(O4:Q4)</f>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>155</v>
@@ -17712,8 +18006,14 @@
       <c r="AA4" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="5" spans="1:27">
+      <c r="AB4" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC4" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>1</v>
       </c>
@@ -17762,13 +18062,14 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R52" si="0">1-SUM(O5:Q5)</f>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
       </c>
       <c r="T5" s="7" t="s">
         <v>155</v>
@@ -17794,8 +18095,14 @@
       <c r="AA5" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="6" spans="1:27">
+      <c r="AB5" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC5" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>2</v>
       </c>
@@ -17844,13 +18151,14 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
       </c>
       <c r="T6" s="7" t="s">
         <v>155</v>
@@ -17876,8 +18184,14 @@
       <c r="AA6" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="7" spans="1:27">
+      <c r="AB6" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>3</v>
       </c>
@@ -17926,13 +18240,14 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
       </c>
       <c r="T7" s="7" t="s">
         <v>155</v>
@@ -17958,8 +18273,14 @@
       <c r="AA7" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="8" spans="1:27">
+      <c r="AB7" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC7" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>4</v>
       </c>
@@ -18010,13 +18331,14 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S8" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
       </c>
       <c r="T8" s="7" t="s">
         <v>155</v>
@@ -18039,11 +18361,17 @@
       <c r="Z8" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27">
+      <c r="AA8" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>5</v>
       </c>
@@ -18094,40 +18422,47 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9" s="7">
-        <v>1</v>
-      </c>
-      <c r="S9" s="7">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9" s="7">
+        <v>1</v>
+      </c>
+      <c r="U9" s="7">
         <v>0.36</v>
       </c>
-      <c r="T9" s="7">
+      <c r="V9" s="7">
         <v>0.58823529411764708</v>
       </c>
-      <c r="U9" s="7">
+      <c r="W9" s="7">
         <v>0.73529411764705888</v>
       </c>
-      <c r="V9" s="7">
+      <c r="X9" s="7">
         <v>0.41176470588235292</v>
       </c>
-      <c r="W9" s="7">
+      <c r="Y9" s="7">
         <v>0.26470588235294112</v>
       </c>
-      <c r="X9" s="7">
+      <c r="Z9" s="7">
         <v>5.3656597774244839</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="AA9" s="7">
         <v>0.29599999999999999</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="AB9" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27">
+      <c r="AC9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>6</v>
       </c>
@@ -18178,13 +18513,14 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
       </c>
       <c r="T10" s="7" t="s">
         <v>155</v>
@@ -18207,11 +18543,17 @@
       <c r="Z10" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27">
+      <c r="AA10" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB10" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11">
         <v>7</v>
       </c>
@@ -18262,13 +18604,14 @@
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>1</v>
-      </c>
-      <c r="R11" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
       </c>
       <c r="T11" s="7" t="s">
         <v>155</v>
@@ -18291,11 +18634,17 @@
       <c r="Z11" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27">
+      <c r="AA11" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB11" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>8</v>
       </c>
@@ -18346,40 +18695,47 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>1</v>
-      </c>
-      <c r="R12" s="7">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12" s="7">
         <v>0.15</v>
       </c>
-      <c r="S12" s="7">
+      <c r="U12" s="7">
         <v>0.52500000000000002</v>
       </c>
-      <c r="T12" s="7">
+      <c r="V12" s="7">
         <v>1.1851851851851851</v>
       </c>
-      <c r="U12" s="7">
+      <c r="W12" s="7">
         <v>1.4814814814814814</v>
       </c>
-      <c r="V12" s="7">
+      <c r="X12" s="7">
         <v>0.82222222222222219</v>
       </c>
-      <c r="W12" s="7">
+      <c r="Y12" s="7">
         <v>0.77777777777777779</v>
       </c>
-      <c r="X12" s="7">
+      <c r="Z12" s="7">
         <v>3.3459595959595965</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="AA12" s="7">
         <v>0.70660740740740724</v>
       </c>
-      <c r="Z12" s="7">
+      <c r="AB12" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AC12" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>9</v>
       </c>
@@ -18430,13 +18786,14 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
       </c>
       <c r="T13" s="7" t="s">
         <v>155</v>
@@ -18459,11 +18816,17 @@
       <c r="Z13" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27">
+      <c r="AA13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>10</v>
       </c>
@@ -18514,40 +18877,47 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>1</v>
-      </c>
-      <c r="R14" s="7">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14" s="7">
         <v>0.15</v>
       </c>
-      <c r="S14" s="7">
+      <c r="U14" s="7">
         <v>0.66</v>
       </c>
-      <c r="T14" s="7">
+      <c r="V14" s="7">
         <v>0.98765432098765427</v>
       </c>
-      <c r="U14" s="7">
+      <c r="W14" s="7">
         <v>1.2345679012345678</v>
       </c>
-      <c r="V14" s="7">
+      <c r="X14" s="7">
         <v>0.85185185185185186</v>
       </c>
-      <c r="W14" s="7">
+      <c r="Y14" s="7">
         <v>0.81481481481481488</v>
       </c>
-      <c r="X14" s="7">
+      <c r="Z14" s="7">
         <v>2.615371635872775</v>
       </c>
-      <c r="Y14" s="7">
+      <c r="AA14" s="7">
         <v>0.80754320987654327</v>
       </c>
-      <c r="Z14" s="7">
+      <c r="AB14" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AC14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:29">
       <c r="A15">
         <v>11</v>
       </c>
@@ -18598,13 +18968,14 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
       </c>
       <c r="T15" s="7" t="s">
         <v>155</v>
@@ -18627,11 +18998,17 @@
       <c r="Z15" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27">
+      <c r="AA15" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB15" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>12</v>
       </c>
@@ -18682,40 +19059,47 @@
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>1</v>
-      </c>
-      <c r="R16" s="7">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16" s="7">
         <v>0.15</v>
       </c>
-      <c r="S16" s="7">
+      <c r="U16" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="T16" s="7">
+      <c r="V16" s="7">
         <v>1.1428571428571428</v>
       </c>
-      <c r="U16" s="7">
+      <c r="W16" s="7">
         <v>1.4285714285714284</v>
       </c>
-      <c r="V16" s="7">
+      <c r="X16" s="7">
         <v>0.82857142857142863</v>
       </c>
-      <c r="W16" s="7">
+      <c r="Y16" s="7">
         <v>0.78571428571428581</v>
       </c>
-      <c r="X16" s="7">
+      <c r="Z16" s="7">
         <v>3.1238095238095238</v>
       </c>
-      <c r="Y16" s="7">
+      <c r="AA16" s="7">
         <v>0.73928571428571432</v>
       </c>
-      <c r="Z16" s="7">
+      <c r="AB16" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AC16" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>13</v>
       </c>
@@ -18766,13 +19150,14 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
       </c>
       <c r="T17" s="7" t="s">
         <v>155</v>
@@ -18795,11 +19180,17 @@
       <c r="Z17" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27">
+      <c r="AA17" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB17" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>14</v>
       </c>
@@ -18850,40 +19241,47 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>1</v>
-      </c>
-      <c r="R18" s="7">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18" s="7">
         <v>0.15</v>
       </c>
-      <c r="S18" s="7">
+      <c r="U18" s="7">
         <v>0.6</v>
       </c>
-      <c r="T18" s="7">
+      <c r="V18" s="7">
         <v>1.0666666666666667</v>
       </c>
-      <c r="U18" s="7">
+      <c r="W18" s="7">
         <v>1.3333333333333333</v>
       </c>
-      <c r="V18" s="7">
+      <c r="X18" s="7">
         <v>0.84</v>
       </c>
-      <c r="W18" s="7">
+      <c r="Y18" s="7">
         <v>0.8</v>
       </c>
-      <c r="X18" s="7">
+      <c r="Z18" s="7">
         <v>2.7294117647058824</v>
       </c>
-      <c r="Y18" s="7">
+      <c r="AA18" s="7">
         <v>0.81033333333333335</v>
       </c>
-      <c r="Z18" s="7">
+      <c r="AB18" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AC18" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>15</v>
       </c>
@@ -18934,13 +19332,14 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>1</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S19" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
       </c>
       <c r="T19" s="7" t="s">
         <v>155</v>
@@ -18963,11 +19362,17 @@
       <c r="Z19" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
+      <c r="AA19" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>16</v>
       </c>
@@ -19018,40 +19423,47 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>1</v>
-      </c>
-      <c r="R20" s="7">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20" s="7">
         <v>0.15</v>
       </c>
-      <c r="S20" s="7">
+      <c r="U20" s="7">
         <v>0.84</v>
       </c>
-      <c r="T20" s="7">
+      <c r="V20" s="7">
         <v>0.80808080808080818</v>
       </c>
-      <c r="U20" s="7">
+      <c r="W20" s="7">
         <v>1.0101010101010102</v>
       </c>
-      <c r="V20" s="7">
+      <c r="X20" s="7">
         <v>0.87878787878787878</v>
       </c>
-      <c r="W20" s="7">
+      <c r="Y20" s="7">
         <v>0.84848484848484851</v>
       </c>
-      <c r="X20" s="7">
+      <c r="Z20" s="7">
         <v>2.3117775695095282</v>
       </c>
-      <c r="Y20" s="7">
+      <c r="AA20" s="7">
         <v>0.81813131313131315</v>
       </c>
-      <c r="Z20" s="7">
+      <c r="AB20" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
+      <c r="AC20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>17</v>
       </c>
@@ -19102,13 +19514,14 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="R21" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S21" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
       </c>
       <c r="T21" s="7" t="s">
         <v>155</v>
@@ -19131,11 +19544,17 @@
       <c r="Z21" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
+      <c r="AA21" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB21" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>18</v>
       </c>
@@ -19186,13 +19605,14 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>1</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S22" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
       </c>
       <c r="T22" s="7" t="s">
         <v>155</v>
@@ -19215,11 +19635,17 @@
       <c r="Z22" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA22" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27">
+      <c r="AA22" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB22" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>19</v>
       </c>
@@ -19270,40 +19696,47 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="R23" s="7">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23" s="7">
         <v>0.15</v>
       </c>
-      <c r="S23" s="7">
+      <c r="U23" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="T23" s="7">
+      <c r="V23" s="7">
         <v>1.1428571428571428</v>
       </c>
-      <c r="U23" s="7">
+      <c r="W23" s="7">
         <v>1.4285714285714284</v>
       </c>
-      <c r="V23" s="7">
+      <c r="X23" s="7">
         <v>0.82857142857142863</v>
       </c>
-      <c r="W23" s="7">
+      <c r="Y23" s="7">
         <v>0.78571428571428581</v>
       </c>
-      <c r="X23" s="7">
+      <c r="Z23" s="7">
         <v>2.8782028782028783</v>
       </c>
-      <c r="Y23" s="7">
+      <c r="AA23" s="7">
         <v>0.80237142857142851</v>
       </c>
-      <c r="Z23" s="7">
+      <c r="AB23" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AC23" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>20</v>
       </c>
@@ -19354,13 +19787,14 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S24" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
       </c>
       <c r="T24" s="7" t="s">
         <v>155</v>
@@ -19383,134 +19817,80 @@
       <c r="Z24" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27">
+      <c r="AA24" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB24" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>21</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>207</v>
+        <v>342</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
         <v>130</v>
       </c>
-      <c r="E25">
-        <v>590</v>
-      </c>
-      <c r="F25" t="s">
-        <v>155</v>
-      </c>
-      <c r="G25" s="1">
-        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K25)/((1+WACC!$B$2)^$K25-1)*$E25,0)</f>
-        <v>42</v>
-      </c>
-      <c r="H25" t="s">
-        <v>155</v>
-      </c>
-      <c r="I25">
-        <v>19500</v>
-      </c>
-      <c r="J25">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K25">
-        <v>25</v>
-      </c>
-      <c r="L25">
-        <v>0.42</v>
-      </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="R25" s="7">
-        <v>0</v>
-      </c>
-      <c r="S25" s="7">
-        <v>0.96</v>
-      </c>
-      <c r="T25" s="7">
-        <v>0.83333333333333348</v>
-      </c>
-      <c r="U25" s="7">
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="V25" s="7">
-        <v>1</v>
-      </c>
-      <c r="W25" s="7">
-        <v>1</v>
-      </c>
-      <c r="X25" s="7">
-        <v>2.3809523809523809</v>
-      </c>
-      <c r="Y25" s="7">
-        <v>0.77</v>
-      </c>
-      <c r="Z25" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="AA25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27">
+      <c r="G25" s="1"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+    </row>
+    <row r="26" spans="1:29">
       <c r="A26">
         <v>22</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>38</v>
+        <v>207</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
         <v>130</v>
       </c>
       <c r="E26">
-        <v>800</v>
+        <v>590</v>
       </c>
       <c r="F26" t="s">
         <v>155</v>
       </c>
       <c r="G26" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K26)/((1+WACC!$B$2)^$K26-1)*$E26,0)</f>
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="H26" t="s">
         <v>155</v>
       </c>
       <c r="I26">
-        <v>20000</v>
+        <v>19500</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K26">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L26">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="M26" t="s">
-        <v>222</v>
+        <v>0.42</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -19522,163 +19902,110 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>1</v>
-      </c>
-      <c r="R26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="T26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="U26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="V26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="W26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="X26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26" s="7">
+        <v>0</v>
+      </c>
+      <c r="U26" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="V26" s="7">
+        <v>0.83333333333333348</v>
+      </c>
+      <c r="W26" s="7">
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="X26" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="7">
+        <v>2.3809523809523809</v>
+      </c>
+      <c r="AA26" s="7">
+        <v>0.77</v>
+      </c>
+      <c r="AB26" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AC26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29">
       <c r="A27">
         <v>23</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>39</v>
+        <v>343</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
         <v>130</v>
       </c>
-      <c r="E27">
-        <v>842</v>
-      </c>
-      <c r="F27" t="s">
-        <v>155</v>
-      </c>
-      <c r="G27" s="1">
-        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K27)/((1+WACC!$B$2)^$K27-1)*$E27,0)</f>
-        <v>55</v>
-      </c>
-      <c r="H27" t="s">
-        <v>155</v>
-      </c>
-      <c r="I27">
-        <v>20000</v>
-      </c>
-      <c r="J27">
-        <v>4</v>
-      </c>
-      <c r="K27">
-        <v>30</v>
-      </c>
-      <c r="L27">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="M27" t="s">
-        <v>221</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-      <c r="R27" s="7">
-        <v>0.15</v>
-      </c>
-      <c r="S27" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="T27" s="7">
-        <v>0.41025641025641035</v>
-      </c>
-      <c r="U27" s="7">
-        <v>0.51282051282051289</v>
-      </c>
-      <c r="V27" s="7">
-        <v>0.93846153846153846</v>
-      </c>
-      <c r="W27" s="7">
-        <v>0.92307692307692313</v>
-      </c>
-      <c r="X27" s="7">
-        <v>1.8956043956043955</v>
-      </c>
-      <c r="Y27" s="7">
-        <v>0.75528205128205139</v>
-      </c>
-      <c r="Z27" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="AA27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27">
+      <c r="G27" s="1"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7"/>
+    </row>
+    <row r="28" spans="1:29">
       <c r="A28">
         <v>24</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
         <v>130</v>
       </c>
       <c r="E28">
-        <v>836</v>
+        <v>800</v>
       </c>
       <c r="F28" t="s">
         <v>155</v>
       </c>
       <c r="G28" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K28)/((1+WACC!$B$2)^$K28-1)*$E28,0)</f>
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H28" t="s">
         <v>155</v>
       </c>
       <c r="I28">
-        <v>27835</v>
+        <v>20000</v>
       </c>
       <c r="J28">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="K28">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L28">
-        <v>0.61</v>
-      </c>
-      <c r="M28">
-        <v>1</v>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M28" t="s">
+        <v>222</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -19690,13 +20017,14 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>1</v>
-      </c>
-      <c r="R28" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S28" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
       </c>
       <c r="T28" s="7" t="s">
         <v>155</v>
@@ -19719,50 +20047,56 @@
       <c r="Z28" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA28" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27">
+      <c r="AA28" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB28" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29">
       <c r="A29">
         <v>25</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
         <v>130</v>
       </c>
       <c r="E29">
-        <v>880</v>
+        <v>842</v>
       </c>
       <c r="F29" t="s">
         <v>155</v>
       </c>
       <c r="G29" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K29)/((1+WACC!$B$2)^$K29-1)*$E29,0)</f>
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
         <v>155</v>
       </c>
       <c r="I29">
-        <v>29300</v>
+        <v>20000</v>
       </c>
       <c r="J29">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="K29">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L29">
-        <v>0.61</v>
-      </c>
-      <c r="M29">
-        <v>1</v>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M29" t="s">
+        <v>221</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -19774,76 +20108,83 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>1</v>
-      </c>
-      <c r="R29" s="7">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29" s="7">
         <v>0.15</v>
       </c>
-      <c r="S29" s="7">
-        <v>2</v>
-      </c>
-      <c r="T29" s="7">
-        <v>0.37209302325581395</v>
-      </c>
       <c r="U29" s="7">
-        <v>0.46511627906976744</v>
+        <v>1.8</v>
       </c>
       <c r="V29" s="7">
-        <v>0.94418604651162785</v>
+        <v>0.41025641025641035</v>
       </c>
       <c r="W29" s="7">
-        <v>0.93023255813953487</v>
+        <v>0.51282051282051289</v>
       </c>
       <c r="X29" s="7">
-        <v>1.7308425467022495</v>
+        <v>0.93846153846153846</v>
       </c>
       <c r="Y29" s="7">
-        <v>0.80293023255813945</v>
+        <v>0.92307692307692313</v>
       </c>
       <c r="Z29" s="7">
+        <v>1.8956043956043955</v>
+      </c>
+      <c r="AA29" s="7">
+        <v>0.75528205128205139</v>
+      </c>
+      <c r="AB29" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27">
+      <c r="AC29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29">
       <c r="A30">
         <v>26</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D30" t="s">
         <v>130</v>
       </c>
       <c r="E30">
-        <v>902.5</v>
+        <v>836</v>
       </c>
       <c r="F30" t="s">
         <v>155</v>
       </c>
       <c r="G30" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K30)/((1+WACC!$B$2)^$K30-1)*$E30,0)</f>
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H30" t="s">
         <v>155</v>
       </c>
       <c r="I30">
-        <v>9262.5</v>
+        <v>27835</v>
       </c>
       <c r="J30">
-        <v>5.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K30">
         <v>25</v>
       </c>
       <c r="L30">
-        <v>0.47</v>
+        <v>0.61</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -19858,13 +20199,14 @@
         <v>0</v>
       </c>
       <c r="Q30">
-        <v>1</v>
-      </c>
-      <c r="R30" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S30" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
       </c>
       <c r="T30" s="7" t="s">
         <v>155</v>
@@ -19887,47 +20229,53 @@
       <c r="Z30" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AA30" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27">
+      <c r="AA30" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB30" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29">
       <c r="A31">
         <v>27</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
         <v>130</v>
       </c>
       <c r="E31">
-        <v>950</v>
+        <v>880</v>
       </c>
       <c r="F31" t="s">
         <v>155</v>
       </c>
       <c r="G31" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K31)/((1+WACC!$B$2)^$K31-1)*$E31,0)</f>
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H31" t="s">
         <v>155</v>
       </c>
       <c r="I31">
-        <v>9750</v>
+        <v>29300</v>
       </c>
       <c r="J31">
-        <v>5.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K31">
         <v>25</v>
       </c>
       <c r="L31">
-        <v>0.47</v>
+        <v>0.61</v>
       </c>
       <c r="M31">
         <v>1</v>
@@ -19942,82 +20290,89 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>1</v>
-      </c>
-      <c r="R31" s="7">
-        <v>0</v>
-      </c>
-      <c r="S31" s="7">
-        <v>0.95</v>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
       </c>
       <c r="T31" s="7">
-        <v>0.84210526315789469</v>
+        <v>0.15</v>
       </c>
       <c r="U31" s="7">
-        <v>1.0526315789473684</v>
+        <v>2</v>
       </c>
       <c r="V31" s="7">
-        <v>1</v>
+        <v>0.37209302325581395</v>
       </c>
       <c r="W31" s="7">
-        <v>1</v>
+        <v>0.46511627906976744</v>
       </c>
       <c r="X31" s="7">
-        <v>2.1276595744680851</v>
+        <v>0.94418604651162785</v>
       </c>
       <c r="Y31" s="7">
-        <v>0.86578947368421044</v>
+        <v>0.93023255813953487</v>
       </c>
       <c r="Z31" s="7">
+        <v>1.7308425467022495</v>
+      </c>
+      <c r="AA31" s="7">
+        <v>0.80293023255813945</v>
+      </c>
+      <c r="AB31" s="7">
         <v>0.8</v>
       </c>
-      <c r="AA31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27">
+      <c r="AC31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29">
       <c r="A32">
         <v>28</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>208</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
         <v>130</v>
       </c>
       <c r="E32">
-        <v>60</v>
+        <v>902.5</v>
       </c>
       <c r="F32" t="s">
         <v>155</v>
       </c>
       <c r="G32" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K32)/((1+WACC!$B$2)^$K32-1)*$E32,0)</f>
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="H32" t="s">
         <v>155</v>
       </c>
       <c r="I32">
-        <v>1950</v>
+        <v>9262.5</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="K32">
         <v>25</v>
       </c>
       <c r="L32">
-        <v>0.95</v>
+        <v>0.47</v>
       </c>
       <c r="M32">
         <v>1</v>
       </c>
       <c r="N32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32">
         <v>0</v>
@@ -20026,13 +20381,14 @@
         <v>0</v>
       </c>
       <c r="Q32">
-        <v>1</v>
-      </c>
-      <c r="R32" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S32" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
       </c>
       <c r="T32" s="7" t="s">
         <v>155</v>
@@ -20058,50 +20414,56 @@
       <c r="AA32" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="33" spans="1:27">
+      <c r="AB32" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29">
       <c r="A33">
         <v>29</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E33">
-        <v>400</v>
+        <v>950</v>
       </c>
       <c r="F33" t="s">
         <v>155</v>
       </c>
       <c r="G33" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K33)/((1+WACC!$B$2)^$K33-1)*$E33,0)</f>
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="H33" t="s">
         <v>155</v>
       </c>
       <c r="I33">
-        <v>6000</v>
+        <v>9750</v>
       </c>
       <c r="J33">
-        <v>3</v>
+        <v>5.4</v>
       </c>
       <c r="K33">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L33">
-        <v>0.39600000000000002</v>
+        <v>0.47</v>
       </c>
       <c r="M33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O33">
         <v>0</v>
@@ -20110,79 +20472,86 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <v>1</v>
-      </c>
-      <c r="R33" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S33" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="T33" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="U33" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="V33" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="W33" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="X33" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y33" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z33" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA33" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33" s="7">
+        <v>0</v>
+      </c>
+      <c r="U33" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="V33" s="7">
+        <v>0.84210526315789469</v>
+      </c>
+      <c r="W33" s="7">
+        <v>1.0526315789473684</v>
+      </c>
+      <c r="X33" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="7">
+        <v>2.1276595744680851</v>
+      </c>
+      <c r="AA33" s="7">
+        <v>0.86578947368421044</v>
+      </c>
+      <c r="AB33" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AC33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29">
       <c r="A34">
         <v>30</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>46</v>
+        <v>208</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E34">
-        <v>400</v>
+        <v>60</v>
       </c>
       <c r="F34" t="s">
         <v>155</v>
       </c>
       <c r="G34" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K34)/((1+WACC!$B$2)^$K34-1)*$E34,0)</f>
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="H34" t="s">
         <v>155</v>
       </c>
       <c r="I34">
-        <v>6000</v>
+        <v>1950</v>
       </c>
       <c r="J34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K34">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L34">
-        <v>0.39600000000000002</v>
+        <v>0.95</v>
       </c>
       <c r="M34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N34">
         <v>1</v>
@@ -20194,79 +20563,86 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <v>1</v>
-      </c>
-      <c r="R34" s="7">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="S34" s="7">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="T34" s="7">
-        <v>1.103448275862069</v>
-      </c>
-      <c r="U34" s="7">
-        <v>1.3793103448275861</v>
-      </c>
-      <c r="V34" s="7">
-        <v>0.80689655172413799</v>
-      </c>
-      <c r="W34" s="7">
-        <v>0.75862068965517249</v>
-      </c>
-      <c r="X34" s="7">
-        <v>3.0128874956461162</v>
-      </c>
-      <c r="Y34" s="7">
-        <v>0.75649655172413799</v>
-      </c>
-      <c r="Z34" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="V34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="W34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="X34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC34" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
       <c r="A35">
         <v>31</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>209</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
         <v>131</v>
       </c>
       <c r="E35">
-        <v>378</v>
+        <v>400</v>
       </c>
       <c r="F35" t="s">
         <v>155</v>
       </c>
       <c r="G35" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K35)/((1+WACC!$B$2)^$K35-1)*$E35,0)</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H35" t="s">
         <v>155</v>
       </c>
       <c r="I35">
-        <v>8068</v>
+        <v>6000</v>
       </c>
       <c r="J35">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="K35">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L35">
-        <v>0.41</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N35">
         <v>0</v>
@@ -20278,13 +20654,14 @@
         <v>0</v>
       </c>
       <c r="Q35">
-        <v>1</v>
-      </c>
-      <c r="R35" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S35" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
       </c>
       <c r="T35" s="7" t="s">
         <v>155</v>
@@ -20310,50 +20687,56 @@
       <c r="AA35" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="36" spans="1:27">
+      <c r="AB35" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC35" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29">
       <c r="A36">
         <v>32</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
         <v>131</v>
       </c>
       <c r="E36">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="F36" t="s">
         <v>155</v>
       </c>
       <c r="G36" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K36)/((1+WACC!$B$2)^$K36-1)*$E36,0)</f>
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="H36" t="s">
         <v>155</v>
       </c>
       <c r="I36">
-        <v>25000</v>
+        <v>6000</v>
       </c>
       <c r="J36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K36">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L36">
-        <v>0.47</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="M36">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -20362,82 +20745,89 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>1</v>
-      </c>
-      <c r="R36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="T36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="U36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="V36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="W36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="X36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA36" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36" s="7">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="U36" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="V36" s="7">
+        <v>1.103448275862069</v>
+      </c>
+      <c r="W36" s="7">
+        <v>1.3793103448275861</v>
+      </c>
+      <c r="X36" s="7">
+        <v>0.80689655172413799</v>
+      </c>
+      <c r="Y36" s="7">
+        <v>0.75862068965517249</v>
+      </c>
+      <c r="Z36" s="7">
+        <v>3.0128874956461162</v>
+      </c>
+      <c r="AA36" s="7">
+        <v>0.75649655172413799</v>
+      </c>
+      <c r="AB36" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29">
       <c r="A37">
         <v>33</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>141</v>
+        <v>209</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D37" t="s">
         <v>131</v>
       </c>
       <c r="E37">
-        <v>842</v>
+        <v>378</v>
       </c>
       <c r="F37" t="s">
         <v>155</v>
       </c>
       <c r="G37" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K37)/((1+WACC!$B$2)^$K37-1)*$E37,0)</f>
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="H37" t="s">
         <v>155</v>
       </c>
       <c r="I37">
-        <v>25000</v>
+        <v>8068</v>
       </c>
       <c r="J37">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="K37">
         <v>25</v>
       </c>
       <c r="L37">
-        <v>0.47</v>
-      </c>
-      <c r="M37" t="s">
-        <v>223</v>
+        <v>0.41</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
       </c>
       <c r="N37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O37">
         <v>0</v>
@@ -20446,166 +20836,114 @@
         <v>0</v>
       </c>
       <c r="Q37">
-        <v>1</v>
-      </c>
-      <c r="R37" s="7">
-        <v>0.187</v>
-      </c>
-      <c r="S37" s="7">
-        <v>0.65</v>
-      </c>
-      <c r="T37" s="7">
-        <v>0.95579450418160106</v>
-      </c>
-      <c r="U37" s="7">
-        <v>1.1947431302270013</v>
-      </c>
-      <c r="V37" s="7">
-        <v>0.82126642771804059</v>
-      </c>
-      <c r="W37" s="7">
-        <v>0.77658303464755074</v>
-      </c>
-      <c r="X37" s="7">
-        <v>2.5079437708126799</v>
-      </c>
-      <c r="Y37" s="7">
-        <v>0.83521863799283147</v>
-      </c>
-      <c r="Z37" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+      <c r="T37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="X37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC37" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29">
       <c r="A38">
         <v>34</v>
       </c>
-      <c r="B38" s="35" t="s">
-        <v>211</v>
+      <c r="B38" s="33" t="s">
+        <v>344</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
-      </c>
-      <c r="E38">
-        <v>660</v>
-      </c>
-      <c r="F38" t="s">
-        <v>155</v>
-      </c>
-      <c r="G38" s="1">
-        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K38)/((1+WACC!$B$2)^$K38-1)*$E38,0)</f>
-        <v>47</v>
-      </c>
-      <c r="H38" t="s">
-        <v>155</v>
-      </c>
-      <c r="I38">
-        <v>2000</v>
-      </c>
-      <c r="J38">
-        <v>1.8</v>
-      </c>
-      <c r="K38">
-        <v>25</v>
-      </c>
-      <c r="L38">
-        <v>3.6</v>
-      </c>
-      <c r="M38">
-        <v>1</v>
-      </c>
-      <c r="N38">
-        <v>1</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38">
-        <v>0</v>
-      </c>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-      <c r="R38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="T38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="U38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="V38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="W38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="X38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA38" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27">
+        <v>131</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+    </row>
+    <row r="39" spans="1:29">
       <c r="A39">
         <v>35</v>
       </c>
-      <c r="B39" s="35" t="s">
-        <v>212</v>
+      <c r="B39" s="33" t="s">
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>213</v>
+        <v>109</v>
       </c>
       <c r="D39" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E39">
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="F39" t="s">
         <v>155</v>
       </c>
       <c r="G39" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K39)/((1+WACC!$B$2)^$K39-1)*$E39,0)</f>
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="H39" t="s">
         <v>155</v>
       </c>
       <c r="I39">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="J39">
-        <v>0.28000000000000003</v>
+        <v>4</v>
       </c>
       <c r="K39">
         <v>25</v>
       </c>
       <c r="L39">
-        <v>1.71</v>
+        <v>0.47</v>
       </c>
       <c r="M39">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="N39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O39">
         <v>0</v>
@@ -20614,13 +20952,14 @@
         <v>0</v>
       </c>
       <c r="Q39">
-        <v>1</v>
-      </c>
-      <c r="R39" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S39" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
       </c>
       <c r="T39" s="7" t="s">
         <v>155</v>
@@ -20646,47 +20985,53 @@
       <c r="AA39" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="40" spans="1:27">
+      <c r="AB39" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC39" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29">
       <c r="A40">
         <v>36</v>
       </c>
-      <c r="B40" s="35" t="s">
-        <v>214</v>
+      <c r="B40" s="33" t="s">
+        <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>215</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E40">
-        <v>150</v>
+        <v>842</v>
       </c>
       <c r="F40" t="s">
         <v>155</v>
       </c>
       <c r="G40" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K40)/((1+WACC!$B$2)^$K40-1)*$E40,0)</f>
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="H40" t="s">
         <v>155</v>
       </c>
       <c r="I40">
-        <v>1070</v>
+        <v>25000</v>
       </c>
       <c r="J40">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="K40">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L40">
-        <v>0.99</v>
-      </c>
-      <c r="M40">
-        <v>1</v>
+        <v>0.47</v>
+      </c>
+      <c r="M40" t="s">
+        <v>223</v>
       </c>
       <c r="N40">
         <v>1</v>
@@ -20698,96 +21043,105 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <v>1</v>
-      </c>
-      <c r="R40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="T40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="U40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="V40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="W40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="X40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA40" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+      <c r="T40" s="7">
+        <v>0.187</v>
+      </c>
+      <c r="U40" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="V40" s="7">
+        <v>0.95579450418160106</v>
+      </c>
+      <c r="W40" s="7">
+        <v>1.1947431302270013</v>
+      </c>
+      <c r="X40" s="7">
+        <v>0.82126642771804059</v>
+      </c>
+      <c r="Y40" s="7">
+        <v>0.77658303464755074</v>
+      </c>
+      <c r="Z40" s="7">
+        <v>2.5079437708126799</v>
+      </c>
+      <c r="AA40" s="7">
+        <v>0.83521863799283147</v>
+      </c>
+      <c r="AB40" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29">
       <c r="A41">
         <v>37</v>
       </c>
-      <c r="B41" s="34" t="s">
-        <v>281</v>
+      <c r="B41" s="35" t="s">
+        <v>211</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D41" t="s">
         <v>136</v>
       </c>
       <c r="E41">
-        <v>320</v>
-      </c>
-      <c r="F41" s="1">
-        <v>302</v>
+        <v>660</v>
+      </c>
+      <c r="F41" t="s">
+        <v>155</v>
       </c>
       <c r="G41" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K41)/((1+WACC!$B$2)^$K41-1)*$E41,0)</f>
-        <v>23</v>
-      </c>
-      <c r="H41" s="1">
-        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K41)/((1+WACC!$B$2)^$K41-1)*$F41,0)</f>
-        <v>21</v>
-      </c>
-      <c r="I41" s="1">
-        <v>540</v>
-      </c>
-      <c r="J41" s="8">
+        <v>47</v>
+      </c>
+      <c r="H41" t="s">
+        <v>155</v>
+      </c>
+      <c r="I41">
+        <v>2000</v>
+      </c>
+      <c r="J41">
         <v>1.8</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41">
         <v>25</v>
       </c>
-      <c r="L41" s="1">
-        <v>1</v>
-      </c>
-      <c r="M41" s="35"/>
-      <c r="N41" s="29">
-        <v>0</v>
-      </c>
-      <c r="O41" s="1">
+      <c r="L41">
+        <v>3.6</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
         <v>0</v>
       </c>
       <c r="P41">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="1">
-        <v>1</v>
-      </c>
-      <c r="R41" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S41" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
       </c>
       <c r="T41" s="7" t="s">
         <v>155</v>
@@ -20813,65 +21167,72 @@
       <c r="AA41" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="42" spans="1:27">
+      <c r="AB41" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC41" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29">
       <c r="A42">
         <v>38</v>
       </c>
-      <c r="B42" s="34" t="s">
-        <v>316</v>
+      <c r="B42" s="35" t="s">
+        <v>212</v>
       </c>
       <c r="C42" t="s">
-        <v>307</v>
+        <v>213</v>
       </c>
       <c r="D42" t="s">
-        <v>287</v>
+        <v>136</v>
       </c>
       <c r="E42">
-        <v>2400</v>
-      </c>
-      <c r="F42">
-        <v>6.5</v>
+        <v>560</v>
+      </c>
+      <c r="F42" t="s">
+        <v>155</v>
       </c>
       <c r="G42" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K42)/((1+WACC!$B$2)^$K42-1)*$E42,0)</f>
-        <v>131</v>
+        <v>40</v>
       </c>
       <c r="H42" t="s">
         <v>155</v>
       </c>
       <c r="I42">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="J42">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K42">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="L42">
-        <v>0.9</v>
-      </c>
-      <c r="M42" t="s">
-        <v>283</v>
+        <v>1.71</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
       </c>
       <c r="N42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O42">
         <v>0</v>
       </c>
       <c r="P42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42">
-        <v>1</v>
-      </c>
-      <c r="R42" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S42" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
       </c>
       <c r="T42" s="7" t="s">
         <v>155</v>
@@ -20897,65 +21258,72 @@
       <c r="AA42" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="43" spans="1:27">
+      <c r="AB42" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC42" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29">
       <c r="A43">
         <v>39</v>
       </c>
-      <c r="B43" s="34" t="s">
-        <v>317</v>
+      <c r="B43" s="35" t="s">
+        <v>214</v>
       </c>
       <c r="C43" t="s">
-        <v>308</v>
+        <v>215</v>
       </c>
       <c r="D43" t="s">
-        <v>287</v>
+        <v>136</v>
       </c>
       <c r="E43">
-        <v>2400</v>
-      </c>
-      <c r="F43">
-        <v>6.5</v>
+        <v>150</v>
+      </c>
+      <c r="F43" t="s">
+        <v>155</v>
       </c>
       <c r="G43" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K43)/((1+WACC!$B$2)^$K43-1)*$E43,0)</f>
-        <v>131</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
         <v>155</v>
       </c>
       <c r="I43">
-        <v>20000</v>
+        <v>1070</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K43">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="L43">
-        <v>0.9</v>
-      </c>
-      <c r="M43" t="s">
-        <v>283</v>
+        <v>0.99</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
       </c>
       <c r="N43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O43">
         <v>0</v>
       </c>
       <c r="P43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q43">
-        <v>1</v>
-      </c>
-      <c r="R43" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S43" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
       </c>
       <c r="T43" s="7" t="s">
         <v>155</v>
@@ -20981,65 +21349,71 @@
       <c r="AA43" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="44" spans="1:27">
+      <c r="AB43" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC43" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29">
       <c r="A44">
         <v>40</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>318</v>
+        <v>281</v>
       </c>
       <c r="C44" t="s">
-        <v>309</v>
+        <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>287</v>
+        <v>136</v>
       </c>
       <c r="E44">
-        <v>2400</v>
-      </c>
-      <c r="F44">
-        <v>6.5</v>
+        <v>320</v>
+      </c>
+      <c r="F44" s="1">
+        <v>302</v>
       </c>
       <c r="G44" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K44)/((1+WACC!$B$2)^$K44-1)*$E44,0)</f>
-        <v>131</v>
-      </c>
-      <c r="H44" t="s">
-        <v>155</v>
-      </c>
-      <c r="I44">
-        <v>20000</v>
-      </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44">
-        <v>50</v>
-      </c>
-      <c r="L44">
-        <v>0.9</v>
-      </c>
-      <c r="M44" t="s">
-        <v>283</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
-      </c>
-      <c r="O44">
+        <v>23</v>
+      </c>
+      <c r="H44" s="1">
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K44)/((1+WACC!$B$2)^$K44-1)*$F44,0)</f>
+        <v>21</v>
+      </c>
+      <c r="I44" s="1">
+        <v>540</v>
+      </c>
+      <c r="J44" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="K44" s="1">
+        <v>25</v>
+      </c>
+      <c r="L44" s="1">
+        <v>1</v>
+      </c>
+      <c r="M44" s="35"/>
+      <c r="N44" s="29">
+        <v>0</v>
+      </c>
+      <c r="O44" s="1">
         <v>0</v>
       </c>
       <c r="P44">
         <v>1</v>
       </c>
       <c r="Q44">
-        <v>1</v>
-      </c>
-      <c r="R44" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S44" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S44" s="1">
+        <v>1</v>
       </c>
       <c r="T44" s="7" t="s">
         <v>155</v>
@@ -21065,29 +21439,35 @@
       <c r="AA44" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="45" spans="1:27">
+      <c r="AB44" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC44" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29">
       <c r="A45">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C45" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D45" t="s">
         <v>287</v>
       </c>
       <c r="E45">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="F45">
         <v>6.5</v>
       </c>
       <c r="G45" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K45)/((1+WACC!$B$2)^$K45-1)*$E45,0)</f>
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="H45" t="s">
         <v>155</v>
@@ -21102,10 +21482,10 @@
         <v>50</v>
       </c>
       <c r="L45">
-        <v>0.81</v>
+        <v>0.9</v>
       </c>
       <c r="M45" t="s">
-        <v>222</v>
+        <v>283</v>
       </c>
       <c r="N45">
         <v>0</v>
@@ -21117,13 +21497,14 @@
         <v>1</v>
       </c>
       <c r="Q45">
-        <v>1</v>
-      </c>
-      <c r="R45" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S45" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
       </c>
       <c r="T45" s="7" t="s">
         <v>155</v>
@@ -21149,29 +21530,35 @@
       <c r="AA45" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="46" spans="1:27">
+      <c r="AB45" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC45" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29">
       <c r="A46">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C46" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D46" t="s">
         <v>287</v>
       </c>
       <c r="E46">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="F46">
         <v>6.5</v>
       </c>
       <c r="G46" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K46)/((1+WACC!$B$2)^$K46-1)*$E46,0)</f>
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="H46" t="s">
         <v>155</v>
@@ -21186,10 +21573,10 @@
         <v>50</v>
       </c>
       <c r="L46">
-        <v>0.81</v>
+        <v>0.9</v>
       </c>
       <c r="M46" t="s">
-        <v>222</v>
+        <v>283</v>
       </c>
       <c r="N46">
         <v>0</v>
@@ -21201,13 +21588,14 @@
         <v>1</v>
       </c>
       <c r="Q46">
-        <v>1</v>
-      </c>
-      <c r="R46" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S46" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
       </c>
       <c r="T46" s="7" t="s">
         <v>155</v>
@@ -21233,29 +21621,35 @@
       <c r="AA46" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="47" spans="1:27">
+      <c r="AB46" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC46" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29">
       <c r="A47">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C47" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D47" t="s">
         <v>287</v>
       </c>
       <c r="E47">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="F47">
         <v>6.5</v>
       </c>
       <c r="G47" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K47)/((1+WACC!$B$2)^$K47-1)*$E47,0)</f>
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="H47" t="s">
         <v>155</v>
@@ -21270,10 +21664,10 @@
         <v>50</v>
       </c>
       <c r="L47">
-        <v>0.81</v>
+        <v>0.9</v>
       </c>
       <c r="M47" t="s">
-        <v>222</v>
+        <v>283</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -21285,13 +21679,14 @@
         <v>1</v>
       </c>
       <c r="Q47">
-        <v>1</v>
-      </c>
-      <c r="R47" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S47" s="7" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>1</v>
       </c>
       <c r="T47" s="7" t="s">
         <v>155</v>
@@ -21317,108 +21712,478 @@
       <c r="AA47" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="48" spans="1:27">
+      <c r="AB47" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC47" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29">
       <c r="A48">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B48" s="34" t="s">
-        <v>282</v>
+        <v>313</v>
       </c>
       <c r="C48" t="s">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="D48" t="s">
-        <v>136</v>
+        <v>287</v>
       </c>
       <c r="E48">
-        <v>2575</v>
-      </c>
-      <c r="F48" s="1">
-        <v>2</v>
+        <v>3000</v>
+      </c>
+      <c r="F48">
+        <v>6.5</v>
       </c>
       <c r="G48" s="1">
         <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K48)/((1+WACC!$B$2)^$K48-1)*$E48,0)</f>
+        <v>164</v>
+      </c>
+      <c r="H48" t="s">
+        <v>155</v>
+      </c>
+      <c r="I48">
+        <v>20000</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>50</v>
+      </c>
+      <c r="L48">
+        <v>0.81</v>
+      </c>
+      <c r="M48" t="s">
+        <v>222</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>1</v>
+      </c>
+      <c r="T48" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="U48" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="V48" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="W48" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="X48" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y48" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z48" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA48" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB48" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC48" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="C49" t="s">
+        <v>311</v>
+      </c>
+      <c r="D49" t="s">
+        <v>287</v>
+      </c>
+      <c r="E49">
+        <v>3000</v>
+      </c>
+      <c r="F49">
+        <v>6.5</v>
+      </c>
+      <c r="G49" s="1">
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K49)/((1+WACC!$B$2)^$K49-1)*$E49,0)</f>
+        <v>164</v>
+      </c>
+      <c r="H49" t="s">
+        <v>155</v>
+      </c>
+      <c r="I49">
+        <v>20000</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>50</v>
+      </c>
+      <c r="L49">
+        <v>0.81</v>
+      </c>
+      <c r="M49" t="s">
+        <v>222</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>1</v>
+      </c>
+      <c r="T49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="U49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="V49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="W49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="X49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC49" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29">
+      <c r="A50">
+        <v>46</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="C50" t="s">
+        <v>312</v>
+      </c>
+      <c r="D50" t="s">
+        <v>287</v>
+      </c>
+      <c r="E50">
+        <v>3000</v>
+      </c>
+      <c r="F50">
+        <v>6.5</v>
+      </c>
+      <c r="G50" s="1">
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K50)/((1+WACC!$B$2)^$K50-1)*$E50,0)</f>
+        <v>164</v>
+      </c>
+      <c r="H50" t="s">
+        <v>155</v>
+      </c>
+      <c r="I50">
+        <v>20000</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>50</v>
+      </c>
+      <c r="L50">
+        <v>0.81</v>
+      </c>
+      <c r="M50" t="s">
+        <v>222</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>1</v>
+      </c>
+      <c r="T50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="U50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="V50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="W50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="X50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC50" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29">
+      <c r="A51">
+        <v>47</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="C51" t="s">
+        <v>260</v>
+      </c>
+      <c r="D51" t="s">
+        <v>136</v>
+      </c>
+      <c r="E51">
+        <v>2575</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2</v>
+      </c>
+      <c r="G51" s="1">
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K51)/((1+WACC!$B$2)^$K51-1)*$E51,0)</f>
         <v>183</v>
       </c>
-      <c r="H48" s="1">
-        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K48)/((1+WACC!$B$2)^$K48-1)*$F48,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I48">
+      <c r="H51" s="1">
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K51)/((1+WACC!$B$2)^$K51-1)*$F51,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I51">
         <v>82500</v>
       </c>
-      <c r="J48" s="1">
-        <v>0</v>
-      </c>
-      <c r="K48" s="1">
+      <c r="J51" s="1">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1">
         <v>25</v>
       </c>
-      <c r="L48" s="6">
+      <c r="L51" s="6">
         <f>0.5*0.79</f>
         <v>0.39500000000000002</v>
       </c>
-      <c r="M48" t="s">
+      <c r="M51" t="s">
         <v>284</v>
       </c>
-      <c r="N48">
-        <v>0</v>
-      </c>
-      <c r="O48">
-        <v>0</v>
-      </c>
-      <c r="P48">
-        <v>1</v>
-      </c>
-      <c r="Q48">
-        <v>1</v>
-      </c>
-      <c r="R48" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S48" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="T48" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="U48" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="V48" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="W48" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="X48" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y48" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z48" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA48" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="49" spans="6:11">
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-    </row>
-    <row r="50" spans="6:11">
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>1</v>
+      </c>
+      <c r="T51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="U51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="V51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="W51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="X51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC51" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29">
+      <c r="A52">
+        <v>48</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="C52" t="s">
+        <v>331</v>
+      </c>
+      <c r="D52" t="s">
+        <v>136</v>
+      </c>
+      <c r="E52" s="42">
+        <f>ROUND(455/0.9,0)</f>
+        <v>506</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G52" s="1">
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$K52)/((1+WACC!$B$2)^$K52-1)*$E52,0)</f>
+        <v>29</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I52" s="1">
+        <v>9</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1">
+        <v>40</v>
+      </c>
+      <c r="L52" s="1">
+        <v>1</v>
+      </c>
+      <c r="M52" t="s">
+        <v>338</v>
+      </c>
+      <c r="N52" s="1">
+        <v>0</v>
+      </c>
+      <c r="O52" s="1">
+        <v>0</v>
+      </c>
+      <c r="P52" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>1</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S52" s="1">
+        <v>0</v>
+      </c>
+      <c r="T52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="U52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="V52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="W52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="X52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC52" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29">
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
@@ -22527,7 +23292,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22640,7 +23405,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>287</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -23557,7 +24322,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -23582,7 +24347,7 @@
         <v>131</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>132</v>
+        <v>287</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
fixed bug in export2gdx.py that resulted in duplication of an empty line in data_static.xlsx
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44B2A6E-0007-4BC9-91BA-5F8FD719DF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E863CFB-F082-4427-AB9F-836C51926466}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="750" windowWidth="27555" windowHeight="14985" tabRatio="860" firstSheet="1" activeTab="5" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="29745" yWindow="885" windowWidth="27450" windowHeight="15510" tabRatio="860" firstSheet="1" activeTab="3" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="FEASIBLE_INPUT-OUTPUT_BAK" sheetId="6" r:id="rId18"/>
     <sheet name="potentials" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -15625,13 +15625,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D7635-111A-D442-BE0C-35A2D3A6DC99}">
-  <dimension ref="A1:AD54"/>
+  <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="S22" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W38" sqref="W38"/>
+      <selection pane="bottomRight" activeCell="D60" sqref="D59:D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20547,14 +20547,6 @@
       <c r="AD53" s="7" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="54" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -23505,7 +23497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF42A340-82E7-43E3-8839-0FF1CC25A011}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
temporarily introduces simulated future wind power generation profiles
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73E2719-EB88-446C-A894-7B9883738F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5DEE75-44B1-4FC1-A2A3-6FBB4BA640C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30900" yWindow="2265" windowWidth="24375" windowHeight="12735" tabRatio="860" activeTab="3" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="4515" yWindow="1350" windowWidth="23985" windowHeight="13995" tabRatio="860" activeTab="2" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -62,6 +62,78 @@
     <author>Sebastian</author>
   </authors>
   <commentList>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{9EBCF03B-BA74-4058-87E7-1808BBBFC360}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1,033 (e-control Bestandsstatistik Strom, Jahresreihen)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{93FF72D7-EE86-4585-AEB5-52ED06000142}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+5,7</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{4D0951C0-E14D-4F4F-A7BF-F0E433F2F78F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+2,73</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I18" authorId="0" shapeId="0" xr:uid="{4B4B343C-8F14-4655-876B-5A6C3757947C}">
       <text>
         <r>
@@ -1114,7 +1186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="369">
   <si>
     <t>year</t>
   </si>
@@ -2512,6 +2584,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3970,7 +4046,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4054,7 +4130,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>368</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -10486,11 +10562,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33D813E-78BA-D24A-A7D9-6241E48D080F}">
   <dimension ref="A1:AZ74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D62" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G78" sqref="G78"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11610,13 +11686,13 @@
         <v>2014</v>
       </c>
       <c r="D12">
-        <v>0.785246</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="E12">
         <v>5.6150000000000002</v>
       </c>
       <c r="F12">
-        <v>2.0960000000000001</v>
+        <v>2.11</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -11901,13 +11977,13 @@
         <v>2015</v>
       </c>
       <c r="D15">
-        <v>0.93709799999999999</v>
+        <v>0.872</v>
       </c>
       <c r="E15">
         <v>5.6559999999999997</v>
       </c>
       <c r="F15">
-        <v>2.4209999999999998</v>
+        <v>2.4889999999999999</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -12192,13 +12268,13 @@
         <v>2016</v>
       </c>
       <c r="D18">
-        <v>1.0960160000000001</v>
+        <v>1.976</v>
       </c>
       <c r="E18">
-        <v>5.7</v>
+        <v>5796</v>
       </c>
       <c r="F18">
-        <v>2.649</v>
+        <v>3.1640000000000001</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -12666,13 +12742,13 @@
         <v>2017</v>
       </c>
       <c r="D21">
-        <v>1.2689710000000001</v>
+        <v>1.1930000000000001</v>
       </c>
       <c r="E21">
         <v>5.7140000000000004</v>
       </c>
       <c r="F21">
-        <v>2.8439999999999999</v>
+        <v>2.887</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -12957,13 +13033,13 @@
         <v>2018</v>
       </c>
       <c r="D24">
-        <v>1.4376409999999999</v>
+        <v>1.371</v>
       </c>
       <c r="E24">
-        <v>5.7220000000000004</v>
+        <v>5.7229999999999999</v>
       </c>
       <c r="F24">
-        <v>3.0449999999999999</v>
+        <v>3.133</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -13247,6 +13323,15 @@
       <c r="C27">
         <v>2019</v>
       </c>
+      <c r="D27">
+        <v>1.615</v>
+      </c>
+      <c r="E27">
+        <v>5.7969999999999997</v>
+      </c>
+      <c r="F27">
+        <v>3.2080000000000002</v>
+      </c>
       <c r="G27">
         <v>0</v>
       </c>
@@ -13528,6 +13613,15 @@
       </c>
       <c r="C30">
         <v>2020</v>
+      </c>
+      <c r="D30">
+        <v>1.976</v>
+      </c>
+      <c r="E30">
+        <v>5.7960000000000003</v>
+      </c>
+      <c r="F30">
+        <v>3.1640000000000001</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -17163,13 +17257,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D7635-111A-D442-BE0C-35A2D3A6DC99}">
-  <dimension ref="A1:AD52"/>
+  <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="L37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomRight" activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17545,7 +17639,7 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S52" si="0">1-SUM(P5:R5)</f>
+        <f t="shared" ref="S5:S53" si="0">1-SUM(P5:R5)</f>
         <v>0</v>
       </c>
       <c r="T5">
@@ -20927,7 +21021,7 @@
         <v>116</v>
       </c>
       <c r="D42" t="s">
-        <v>137</v>
+        <v>368</v>
       </c>
       <c r="E42" t="s">
         <v>138</v>
@@ -21904,11 +21998,11 @@
       </c>
     </row>
     <row r="52" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B52" s="43" t="s">
-        <v>327</v>
+      <c r="B52" s="34" t="s">
+        <v>279</v>
       </c>
       <c r="C52" t="s">
-        <v>328</v>
+        <v>257</v>
       </c>
       <c r="D52" t="s">
         <v>368</v>
@@ -21916,80 +22010,172 @@
       <c r="E52" t="s">
         <v>137</v>
       </c>
-      <c r="F52" s="42">
+      <c r="F52">
+        <v>2575</v>
+      </c>
+      <c r="G52" s="1">
+        <v>2</v>
+      </c>
+      <c r="H52" s="1">
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$L52)/((1+WACC!$B$2)^$L52-1)*$F52,0)</f>
+        <v>183</v>
+      </c>
+      <c r="I52" s="1">
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$L52)/((1+WACC!$B$2)^$L52-1)*$G52,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>82500</v>
+      </c>
+      <c r="K52" s="1">
+        <v>0</v>
+      </c>
+      <c r="L52" s="1">
+        <v>25</v>
+      </c>
+      <c r="M52" s="6">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="N52" t="s">
+        <v>281</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>1</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T52">
+        <v>1</v>
+      </c>
+      <c r="U52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="V52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="W52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="X52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD52" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B53" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="C53" t="s">
+        <v>328</v>
+      </c>
+      <c r="D53" t="s">
+        <v>368</v>
+      </c>
+      <c r="E53" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" s="42">
         <f>ROUND(455/0.9,0)</f>
         <v>506</v>
       </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1">
-        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$L52)/((1+WACC!$B$2)^$L52-1)*$F52,0)</f>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1">
+        <f>ROUND((WACC!$B$2*(1+WACC!$B$2)^$L53)/((1+WACC!$B$2)^$L53-1)*$F53,0)</f>
         <v>29</v>
       </c>
-      <c r="I52" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J52" s="1">
+      <c r="I53" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J53" s="1">
         <v>9</v>
       </c>
-      <c r="K52" s="1">
-        <v>0</v>
-      </c>
-      <c r="L52" s="1">
+      <c r="K53" s="1">
+        <v>0</v>
+      </c>
+      <c r="L53" s="1">
         <v>40</v>
       </c>
-      <c r="M52" s="1">
-        <v>0</v>
-      </c>
-      <c r="N52" t="s">
+      <c r="M53" s="1">
+        <v>0</v>
+      </c>
+      <c r="N53" t="s">
         <v>335</v>
       </c>
-      <c r="O52" s="1">
-        <v>0</v>
-      </c>
-      <c r="P52" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="1">
-        <v>0</v>
-      </c>
-      <c r="R52">
-        <v>1</v>
-      </c>
-      <c r="S52">
+      <c r="O53" s="1">
+        <v>0</v>
+      </c>
+      <c r="P53" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+      <c r="S53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T52" s="1">
-        <v>0</v>
-      </c>
-      <c r="U52" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="V52" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="W52" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="X52" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y52" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z52" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AA52" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB52" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AC52" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AD52" s="7" t="s">
+      <c r="T53" s="1">
+        <v>0</v>
+      </c>
+      <c r="U53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="V53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="W53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="X53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD53" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -22005,10 +22191,10 @@
   <dimension ref="A1:AD57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
+      <selection pane="bottomRight" activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31476,7 +31662,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31657,7 +31843,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>368</v>
       </c>
       <c r="B11">
         <v>0</v>

</xml_diff>

<commit_message>
updates to project asparagus
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5DEE75-44B1-4FC1-A2A3-6FBB4BA640C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8775C4-75BA-445A-939E-47429332C1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="1350" windowWidth="23985" windowHeight="13995" tabRatio="860" activeTab="2" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="3375" yWindow="2235" windowWidth="23985" windowHeight="13995" tabRatio="860" activeTab="2" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -155,6 +155,174 @@
           </rPr>
           <t xml:space="preserve">
 0,355 in 2016</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D45" authorId="0" shapeId="0" xr:uid="{6A97567A-D5DD-44A0-A9B7-67C63EEF75E3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+40,679</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E45" authorId="0" shapeId="0" xr:uid="{048582FC-3DC9-4483-8C81-1436EA10C25D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+4,5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{1BE10ECF-326E-4604-B10F-99E84F18F438}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+45,283</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G45" authorId="0" shapeId="0" xr:uid="{62BB9CA3-0A1F-4C6B-8BF8-E7652ECCD6D2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+4,152</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H45" authorId="0" shapeId="0" xr:uid="{2775EA62-55DE-47C6-B37C-28FF3CC13FF5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+2,504</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I45" authorId="0" shapeId="0" xr:uid="{799E24EC-1D12-47D8-8937-29DD0434E82E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J45" authorId="0" shapeId="0" xr:uid="{66A437AC-A5B3-420B-B6C5-3A1DBA71C86B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+2</t>
         </r>
       </text>
     </comment>
@@ -2586,10 +2754,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -10563,10 +10727,10 @@
   <dimension ref="A1:AZ74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12264,28 +12428,28 @@
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="35">
         <v>2016</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="35">
         <v>1.976</v>
       </c>
-      <c r="E18">
-        <v>5796</v>
-      </c>
-      <c r="F18">
+      <c r="E18" s="35">
+        <v>5.7960000000000003</v>
+      </c>
+      <c r="F18" s="35">
         <v>3.1640000000000001</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
+      <c r="G18" s="35">
+        <v>0</v>
+      </c>
+      <c r="H18" s="35">
         <v>0.20949999999999999</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="35">
         <v>0.47699999999999998</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="35">
         <v>0.8</v>
       </c>
       <c r="K18">
@@ -15066,28 +15230,28 @@
       <c r="B45" t="s">
         <v>2</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="35">
         <v>2016</v>
       </c>
-      <c r="D45">
-        <v>40.679000000000002</v>
-      </c>
-      <c r="E45">
+      <c r="D45" s="35">
+        <v>53.847999999999999</v>
+      </c>
+      <c r="E45" s="35">
         <v>4.5</v>
       </c>
-      <c r="F45">
-        <v>45.283000000000001</v>
-      </c>
-      <c r="G45">
-        <v>4.1520000000000001</v>
-      </c>
-      <c r="H45">
-        <v>2.504</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
+      <c r="F45" s="35">
+        <v>54.42</v>
+      </c>
+      <c r="G45" s="35">
+        <v>7.7469999999999999</v>
+      </c>
+      <c r="H45" s="35">
+        <v>4.2</v>
+      </c>
+      <c r="I45" s="35">
+        <v>4.2</v>
+      </c>
+      <c r="J45" s="35">
         <v>2</v>
       </c>
       <c r="K45" s="29">
@@ -16401,8 +16565,29 @@
       <c r="B57" t="s">
         <v>2</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="35">
         <v>2020</v>
+      </c>
+      <c r="D57" s="35">
+        <v>53.847999999999999</v>
+      </c>
+      <c r="E57" s="35">
+        <v>4.5</v>
+      </c>
+      <c r="F57" s="35">
+        <v>54.42</v>
+      </c>
+      <c r="G57" s="35">
+        <v>7.7469999999999999</v>
+      </c>
+      <c r="H57" s="35">
+        <v>4.2</v>
+      </c>
+      <c r="I57" s="35">
+        <v>4.2</v>
+      </c>
+      <c r="J57" s="35">
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates Austrian capacities with e-control data. Adds H2 stacks to 2030 capacity in line with German hydrogen strategy for project asparagus
</commit_message>
<xml_diff>
--- a/data/processed/data_static.xlsx
+++ b/data/processed/data_static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8775C4-75BA-445A-939E-47429332C1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD72A45-DB1B-4BE8-AF62-87DE5EDA4E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="2235" windowWidth="23985" windowHeight="13995" tabRatio="860" activeTab="2" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
+    <workbookView xWindow="2580" yWindow="2160" windowWidth="22245" windowHeight="13995" tabRatio="860" activeTab="2" xr2:uid="{621F8D32-52B7-4CE4-9D99-ED32CD70233E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="16" r:id="rId1"/>
@@ -4355,7 +4355,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4388,13 +4388,13 @@
         <v>2012</v>
       </c>
       <c r="C2">
-        <v>0.36288500000000001</v>
+        <v>0.215</v>
       </c>
       <c r="D2">
-        <v>5.5190000000000001</v>
+        <v>5.53</v>
       </c>
       <c r="E2">
-        <v>1.373</v>
+        <v>1.337</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -4408,13 +4408,13 @@
         <v>2013</v>
       </c>
       <c r="C3">
-        <v>0.62597400000000003</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="D3">
-        <v>5.5730000000000004</v>
+        <v>5.58</v>
       </c>
       <c r="E3">
-        <v>1.6879999999999999</v>
+        <v>1.681</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4428,13 +4428,13 @@
         <v>2014</v>
       </c>
       <c r="C4">
-        <v>0.785246</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="D4">
-        <v>5.6150000000000002</v>
+        <v>5.6210000000000004</v>
       </c>
       <c r="E4">
-        <v>2.0960000000000001</v>
+        <v>2.11</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -4448,13 +4448,13 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0.93709799999999999</v>
+        <v>0.872</v>
       </c>
       <c r="D5">
-        <v>5.6559999999999997</v>
+        <v>5.6619999999999999</v>
       </c>
       <c r="E5">
-        <v>2.4209999999999998</v>
+        <v>2.4889999999999999</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -4468,13 +4468,13 @@
         <v>2016</v>
       </c>
       <c r="C6">
-        <v>1.0960160000000001</v>
+        <v>1.0329999999999999</v>
       </c>
       <c r="D6">
         <v>5.7</v>
       </c>
       <c r="E6">
-        <v>2.649</v>
+        <v>2.73</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -4488,13 +4488,13 @@
         <v>2017</v>
       </c>
       <c r="C7">
-        <v>1.2689710000000001</v>
+        <v>1.1930000000000001</v>
       </c>
       <c r="D7">
-        <v>5.7140000000000004</v>
+        <v>5.7160000000000002</v>
       </c>
       <c r="E7">
-        <v>2.8439999999999999</v>
+        <v>2.887</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -4508,13 +4508,13 @@
         <v>2018</v>
       </c>
       <c r="C8">
-        <v>1.4376409999999999</v>
+        <v>1.371</v>
       </c>
       <c r="D8">
-        <v>5.7220000000000004</v>
+        <v>5.7229999999999999</v>
       </c>
       <c r="E8">
-        <v>3.0449999999999999</v>
+        <v>3.133</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -4527,6 +4527,15 @@
       <c r="B9">
         <v>2019</v>
       </c>
+      <c r="C9">
+        <v>1.615</v>
+      </c>
+      <c r="D9">
+        <v>5.7969999999999997</v>
+      </c>
+      <c r="E9">
+        <v>3.2080000000000002</v>
+      </c>
       <c r="F9">
         <v>0</v>
       </c>
@@ -4537,6 +4546,15 @@
       </c>
       <c r="B10">
         <v>2020</v>
+      </c>
+      <c r="C10">
+        <v>1.976</v>
+      </c>
+      <c r="D10">
+        <v>5.7960000000000003</v>
+      </c>
+      <c r="E10">
+        <v>3.1640000000000001</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -10727,10 +10745,10 @@
   <dimension ref="A1:AZ74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="AN36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="AZ48" sqref="AZ48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12576,7 +12594,7 @@
         <v>1.6060000000000001</v>
       </c>
       <c r="AZ18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
@@ -12734,7 +12752,7 @@
         <v>1.393</v>
       </c>
       <c r="AZ19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
@@ -12892,7 +12910,7 @@
         <v>1481.5</v>
       </c>
       <c r="AZ20">
-        <v>0</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
@@ -15378,7 +15396,7 @@
         <v>0.28899999999999998</v>
       </c>
       <c r="AZ45" s="29">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:52" x14ac:dyDescent="0.25">
@@ -15536,7 +15554,7 @@
         <v>0.17299999999999999</v>
       </c>
       <c r="AZ46">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
@@ -15694,7 +15712,7 @@
         <v>98.55</v>
       </c>
       <c r="AZ47">
-        <v>0</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.25">

</xml_diff>